<commit_message>
Change template data stem paths
Made data stems relative to tests directory
</commit_message>
<xml_diff>
--- a/test_templates/faulty_batch_template1.xlsx
+++ b/test_templates/faulty_batch_template1.xlsx
@@ -2380,10 +2380,10 @@
     <t>hello</t>
   </si>
   <si>
-    <t>../TASBEFlowAnalytics-Tutorial/example_assay</t>
-  </si>
-  <si>
-    <t>../TASBEFlowAnalytics-Tutorial/example_controls</t>
+    <t>../../TASBEFlowAnalytics-Tutorial/example_assay</t>
+  </si>
+  <si>
+    <t>../../TASBEFlowAnalytics-Tutorial/example_controls</t>
   </si>
 </sst>
 </file>
@@ -3891,20 +3891,116 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3927,102 +4023,6 @@
     <xf numFmtId="49" fontId="16" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4101,12 +4101,21 @@
     <xf numFmtId="0" fontId="14" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4117,15 +4126,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="17" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5012,7 +5012,7 @@
   <dimension ref="A1:K48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5033,86 +5033,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="227" t="s">
+      <c r="A1" s="238" t="s">
         <v>385</v>
       </c>
-      <c r="B1" s="228"/>
-      <c r="C1" s="228"/>
-      <c r="D1" s="228"/>
-      <c r="E1" s="228"/>
-      <c r="F1" s="228"/>
-      <c r="G1" s="228"/>
-      <c r="H1" s="228"/>
-      <c r="I1" s="228"/>
-      <c r="J1" s="228"/>
-      <c r="K1" s="229"/>
+      <c r="B1" s="239"/>
+      <c r="C1" s="239"/>
+      <c r="D1" s="239"/>
+      <c r="E1" s="239"/>
+      <c r="F1" s="239"/>
+      <c r="G1" s="239"/>
+      <c r="H1" s="239"/>
+      <c r="I1" s="239"/>
+      <c r="J1" s="239"/>
+      <c r="K1" s="240"/>
     </row>
     <row r="2" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="88"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="243" t="s">
+      <c r="A3" s="217" t="s">
         <v>321</v>
       </c>
-      <c r="B3" s="244"/>
+      <c r="B3" s="218"/>
     </row>
     <row r="4" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="241" t="s">
+      <c r="A4" s="231" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="242"/>
+      <c r="B4" s="232"/>
     </row>
     <row r="5" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="257" t="s">
+      <c r="A5" s="233" t="s">
         <v>182</v>
       </c>
-      <c r="B5" s="258"/>
+      <c r="B5" s="234"/>
     </row>
     <row r="6" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="88"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="243" t="s">
+      <c r="A7" s="217" t="s">
         <v>276</v>
       </c>
-      <c r="B7" s="245"/>
-      <c r="C7" s="245"/>
-      <c r="D7" s="245"/>
-      <c r="E7" s="245"/>
-      <c r="F7" s="245"/>
-      <c r="G7" s="245"/>
-      <c r="H7" s="245"/>
-      <c r="I7" s="245"/>
-      <c r="J7" s="245"/>
-      <c r="K7" s="244"/>
+      <c r="B7" s="219"/>
+      <c r="C7" s="219"/>
+      <c r="D7" s="219"/>
+      <c r="E7" s="219"/>
+      <c r="F7" s="219"/>
+      <c r="G7" s="219"/>
+      <c r="H7" s="219"/>
+      <c r="I7" s="219"/>
+      <c r="J7" s="219"/>
+      <c r="K7" s="218"/>
     </row>
     <row r="8" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="230" t="s">
+      <c r="A8" s="241" t="s">
         <v>162</v>
       </c>
-      <c r="B8" s="231"/>
-      <c r="C8" s="231"/>
-      <c r="D8" s="231"/>
-      <c r="E8" s="231"/>
-      <c r="F8" s="231"/>
-      <c r="G8" s="231"/>
-      <c r="H8" s="231"/>
-      <c r="I8" s="231"/>
-      <c r="J8" s="231"/>
-      <c r="K8" s="232"/>
+      <c r="B8" s="242"/>
+      <c r="C8" s="242"/>
+      <c r="D8" s="242"/>
+      <c r="E8" s="242"/>
+      <c r="F8" s="242"/>
+      <c r="G8" s="242"/>
+      <c r="H8" s="242"/>
+      <c r="I8" s="242"/>
+      <c r="J8" s="242"/>
+      <c r="K8" s="243"/>
     </row>
     <row r="9" spans="1:11" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="233"/>
-      <c r="B9" s="234"/>
-      <c r="C9" s="234"/>
-      <c r="D9" s="234"/>
-      <c r="E9" s="234"/>
-      <c r="F9" s="234"/>
-      <c r="G9" s="234"/>
-      <c r="H9" s="234"/>
-      <c r="I9" s="234"/>
-      <c r="J9" s="234"/>
-      <c r="K9" s="235"/>
+      <c r="A9" s="244"/>
+      <c r="B9" s="245"/>
+      <c r="C9" s="245"/>
+      <c r="D9" s="245"/>
+      <c r="E9" s="245"/>
+      <c r="F9" s="245"/>
+      <c r="G9" s="245"/>
+      <c r="H9" s="245"/>
+      <c r="I9" s="245"/>
+      <c r="J9" s="245"/>
+      <c r="K9" s="246"/>
     </row>
     <row r="10" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="158"/>
@@ -5123,62 +5123,62 @@
       <c r="F10" s="144"/>
     </row>
     <row r="11" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="246" t="s">
+      <c r="A11" s="220" t="s">
         <v>277</v>
       </c>
-      <c r="B11" s="247"/>
-      <c r="C11" s="247"/>
-      <c r="D11" s="248"/>
+      <c r="B11" s="221"/>
+      <c r="C11" s="221"/>
+      <c r="D11" s="222"/>
       <c r="E11" s="89"/>
       <c r="F11" s="144"/>
     </row>
     <row r="12" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="249" t="s">
+      <c r="A12" s="223" t="s">
         <v>163</v>
       </c>
-      <c r="B12" s="250"/>
-      <c r="C12" s="251" t="s">
+      <c r="B12" s="224"/>
+      <c r="C12" s="225" t="s">
         <v>164</v>
       </c>
-      <c r="D12" s="252"/>
+      <c r="D12" s="226"/>
       <c r="E12" s="89"/>
       <c r="F12" s="144"/>
     </row>
     <row r="13" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="253"/>
-      <c r="B13" s="254"/>
-      <c r="C13" s="255"/>
-      <c r="D13" s="256"/>
+      <c r="A13" s="227"/>
+      <c r="B13" s="228"/>
+      <c r="C13" s="229"/>
+      <c r="D13" s="230"/>
       <c r="E13" s="89"/>
       <c r="F13" s="144"/>
     </row>
     <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:11" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="246" t="s">
+      <c r="A15" s="220" t="s">
         <v>278</v>
       </c>
-      <c r="B15" s="248"/>
-      <c r="E15" s="246" t="s">
+      <c r="B15" s="222"/>
+      <c r="E15" s="220" t="s">
         <v>320</v>
       </c>
-      <c r="F15" s="247"/>
-      <c r="G15" s="247"/>
-      <c r="H15" s="247"/>
-      <c r="I15" s="248"/>
+      <c r="F15" s="221"/>
+      <c r="G15" s="221"/>
+      <c r="H15" s="221"/>
+      <c r="I15" s="222"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="241" t="s">
+      <c r="A16" s="231" t="s">
         <v>236</v>
       </c>
-      <c r="B16" s="242"/>
+      <c r="B16" s="232"/>
       <c r="D16" s="90"/>
-      <c r="E16" s="236" t="s">
+      <c r="E16" s="247" t="s">
         <v>197</v>
       </c>
-      <c r="F16" s="237"/>
-      <c r="G16" s="237"/>
-      <c r="H16" s="237"/>
-      <c r="I16" s="238"/>
+      <c r="F16" s="248"/>
+      <c r="G16" s="248"/>
+      <c r="H16" s="248"/>
+      <c r="I16" s="249"/>
     </row>
     <row r="17" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="159" t="s">
@@ -5188,10 +5188,10 @@
         <v>281</v>
       </c>
       <c r="C17" s="91"/>
-      <c r="E17" s="239" t="s">
+      <c r="E17" s="250" t="s">
         <v>235</v>
       </c>
-      <c r="F17" s="240"/>
+      <c r="F17" s="251"/>
       <c r="G17" s="84" t="s">
         <v>159</v>
       </c>
@@ -5221,7 +5221,7 @@
       <c r="H18" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="I18" s="215" t="s">
+      <c r="I18" s="235" t="s">
         <v>474</v>
       </c>
       <c r="J18" s="82"/>
@@ -5244,7 +5244,7 @@
       <c r="H19" s="75" t="s">
         <v>196</v>
       </c>
-      <c r="I19" s="215"/>
+      <c r="I19" s="235"/>
       <c r="J19" s="82"/>
     </row>
     <row r="20" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5261,7 +5261,7 @@
       </c>
       <c r="G20" s="72"/>
       <c r="H20" s="72"/>
-      <c r="I20" s="216"/>
+      <c r="I20" s="236"/>
       <c r="J20" s="82"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -5283,24 +5283,24 @@
       <c r="A23" s="163"/>
       <c r="B23" s="94"/>
       <c r="C23" s="93"/>
-      <c r="E23" s="217" t="s">
+      <c r="E23" s="215" t="s">
         <v>198</v>
       </c>
-      <c r="F23" s="218"/>
-      <c r="G23" s="218"/>
-      <c r="H23" s="218"/>
-      <c r="I23" s="219"/>
+      <c r="F23" s="237"/>
+      <c r="G23" s="237"/>
+      <c r="H23" s="237"/>
+      <c r="I23" s="216"/>
     </row>
     <row r="24" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="217" t="s">
+      <c r="A24" s="215" t="s">
         <v>240</v>
       </c>
-      <c r="B24" s="219"/>
+      <c r="B24" s="216"/>
       <c r="C24" s="33"/>
-      <c r="E24" s="223" t="s">
+      <c r="E24" s="255" t="s">
         <v>235</v>
       </c>
-      <c r="F24" s="224"/>
+      <c r="F24" s="256"/>
       <c r="G24" s="83" t="s">
         <v>159</v>
       </c>
@@ -5329,7 +5329,7 @@
       <c r="H25" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="I25" s="220" t="s">
+      <c r="I25" s="252" t="s">
         <v>475</v>
       </c>
     </row>
@@ -5353,7 +5353,7 @@
       <c r="H26" s="75" t="s">
         <v>201</v>
       </c>
-      <c r="I26" s="221"/>
+      <c r="I26" s="253"/>
     </row>
     <row r="27" spans="1:10" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="161" t="s">
@@ -5369,7 +5369,7 @@
       </c>
       <c r="G27" s="72"/>
       <c r="H27" s="72"/>
-      <c r="I27" s="222"/>
+      <c r="I27" s="254"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="161" t="s">
@@ -5393,22 +5393,22 @@
       <c r="A30" s="162"/>
       <c r="B30" s="119"/>
       <c r="C30" s="91"/>
-      <c r="E30" s="217" t="s">
+      <c r="E30" s="215" t="s">
         <v>199</v>
       </c>
-      <c r="F30" s="218"/>
-      <c r="G30" s="218"/>
-      <c r="H30" s="218"/>
-      <c r="I30" s="219"/>
+      <c r="F30" s="237"/>
+      <c r="G30" s="237"/>
+      <c r="H30" s="237"/>
+      <c r="I30" s="216"/>
     </row>
     <row r="31" spans="1:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="163"/>
       <c r="B31" s="93"/>
       <c r="C31" s="93"/>
-      <c r="E31" s="225" t="s">
+      <c r="E31" s="257" t="s">
         <v>472</v>
       </c>
-      <c r="F31" s="226"/>
+      <c r="F31" s="258"/>
       <c r="G31" s="213" t="s">
         <v>159</v>
       </c>
@@ -5420,10 +5420,10 @@
       </c>
     </row>
     <row r="32" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="217" t="s">
+      <c r="A32" s="215" t="s">
         <v>241</v>
       </c>
-      <c r="B32" s="219"/>
+      <c r="B32" s="216"/>
       <c r="C32" s="33"/>
       <c r="E32" s="85">
         <v>1</v>
@@ -5433,7 +5433,7 @@
       </c>
       <c r="G32" s="34"/>
       <c r="H32" s="75"/>
-      <c r="I32" s="215"/>
+      <c r="I32" s="235"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="159" t="s">
@@ -5453,7 +5453,7 @@
         <v>5</v>
       </c>
       <c r="H33" s="34"/>
-      <c r="I33" s="215"/>
+      <c r="I33" s="235"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="160" t="s">
@@ -5468,7 +5468,7 @@
       <c r="F34" s="95"/>
       <c r="G34" s="34"/>
       <c r="H34" s="75"/>
-      <c r="I34" s="215"/>
+      <c r="I34" s="235"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="161" t="s">
@@ -5481,7 +5481,7 @@
       <c r="F35" s="95"/>
       <c r="G35" s="34"/>
       <c r="H35" s="34"/>
-      <c r="I35" s="215"/>
+      <c r="I35" s="235"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="161" t="s">
@@ -5494,7 +5494,7 @@
       <c r="F36" s="95"/>
       <c r="G36" s="34"/>
       <c r="H36" s="34"/>
-      <c r="I36" s="215"/>
+      <c r="I36" s="235"/>
     </row>
     <row r="37" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="161" t="s">
@@ -5507,7 +5507,7 @@
       <c r="F37" s="142"/>
       <c r="G37" s="72"/>
       <c r="H37" s="72"/>
-      <c r="I37" s="216"/>
+      <c r="I37" s="236"/>
     </row>
     <row r="38" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="162" t="s">
@@ -5520,17 +5520,17 @@
       <c r="B39" s="123"/>
     </row>
     <row r="40" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="E40" s="217" t="s">
+      <c r="E40" s="215" t="s">
         <v>200</v>
       </c>
-      <c r="F40" s="218"/>
-      <c r="G40" s="218"/>
-      <c r="H40" s="218"/>
-      <c r="I40" s="219"/>
+      <c r="F40" s="237"/>
+      <c r="G40" s="237"/>
+      <c r="H40" s="237"/>
+      <c r="I40" s="216"/>
     </row>
     <row r="41" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="E41" s="223"/>
-      <c r="F41" s="224"/>
+      <c r="E41" s="255"/>
+      <c r="F41" s="256"/>
       <c r="G41" s="83" t="s">
         <v>159</v>
       </c>
@@ -5548,7 +5548,7 @@
       <c r="F42" s="95"/>
       <c r="G42" s="34"/>
       <c r="H42" s="75"/>
-      <c r="I42" s="215"/>
+      <c r="I42" s="235"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E43" s="85">
@@ -5557,7 +5557,7 @@
       <c r="F43" s="95"/>
       <c r="G43" s="34"/>
       <c r="H43" s="34"/>
-      <c r="I43" s="215"/>
+      <c r="I43" s="235"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E44" s="85">
@@ -5566,7 +5566,7 @@
       <c r="F44" s="95"/>
       <c r="G44" s="34"/>
       <c r="H44" s="75"/>
-      <c r="I44" s="215"/>
+      <c r="I44" s="235"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E45" s="85">
@@ -5575,7 +5575,7 @@
       <c r="F45" s="95"/>
       <c r="G45" s="34"/>
       <c r="H45" s="34"/>
-      <c r="I45" s="215"/>
+      <c r="I45" s="235"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E46" s="85">
@@ -5584,7 +5584,7 @@
       <c r="F46" s="95"/>
       <c r="G46" s="34"/>
       <c r="H46" s="34"/>
-      <c r="I46" s="215"/>
+      <c r="I46" s="235"/>
     </row>
     <row r="47" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E47" s="86">
@@ -5593,11 +5593,25 @@
       <c r="F47" s="142"/>
       <c r="G47" s="72"/>
       <c r="H47" s="72"/>
-      <c r="I47" s="216"/>
+      <c r="I47" s="236"/>
     </row>
     <row r="48" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="I42:I47"/>
+    <mergeCell ref="E40:I40"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="I25:I27"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A8:K8"/>
+    <mergeCell ref="A9:K9"/>
+    <mergeCell ref="E16:I16"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="A16:B16"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="A3:B3"/>
@@ -5613,20 +5627,6 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="I32:I37"/>
     <mergeCell ref="E30:I30"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A8:K8"/>
-    <mergeCell ref="A9:K9"/>
-    <mergeCell ref="E16:I16"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="I42:I47"/>
-    <mergeCell ref="E40:I40"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="I25:I27"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E31:F31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7980,23 +7980,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="291" t="s">
+      <c r="A1" s="286" t="s">
         <v>244</v>
       </c>
-      <c r="B1" s="291"/>
-      <c r="C1" s="291"/>
-      <c r="D1" s="291"/>
-      <c r="E1" s="291"/>
-      <c r="F1" s="291"/>
-      <c r="G1" s="291"/>
-      <c r="H1" s="291"/>
-      <c r="I1" s="291"/>
-      <c r="J1" s="291"/>
-      <c r="K1" s="291"/>
-      <c r="L1" s="291"/>
-      <c r="M1" s="291"/>
-      <c r="N1" s="291"/>
-      <c r="O1" s="291"/>
+      <c r="B1" s="286"/>
+      <c r="C1" s="286"/>
+      <c r="D1" s="286"/>
+      <c r="E1" s="286"/>
+      <c r="F1" s="286"/>
+      <c r="G1" s="286"/>
+      <c r="H1" s="286"/>
+      <c r="I1" s="286"/>
+      <c r="J1" s="286"/>
+      <c r="K1" s="286"/>
+      <c r="L1" s="286"/>
+      <c r="M1" s="286"/>
+      <c r="N1" s="286"/>
+      <c r="O1" s="286"/>
       <c r="P1" s="32"/>
       <c r="Q1" s="32"/>
     </row>
@@ -8004,26 +8004,26 @@
       <c r="A2" s="204" t="s">
         <v>360</v>
       </c>
-      <c r="B2" s="292" t="s">
+      <c r="B2" s="287" t="s">
         <v>282</v>
       </c>
-      <c r="C2" s="292"/>
-      <c r="D2" s="292"/>
-      <c r="E2" s="292"/>
-      <c r="F2" s="292"/>
-      <c r="G2" s="292" t="s">
+      <c r="C2" s="287"/>
+      <c r="D2" s="287"/>
+      <c r="E2" s="287"/>
+      <c r="F2" s="287"/>
+      <c r="G2" s="287" t="s">
         <v>248</v>
       </c>
-      <c r="H2" s="292"/>
-      <c r="I2" s="292"/>
-      <c r="J2" s="292"/>
-      <c r="K2" s="292"/>
-      <c r="L2" s="292"/>
-      <c r="M2" s="287" t="s">
+      <c r="H2" s="287"/>
+      <c r="I2" s="287"/>
+      <c r="J2" s="287"/>
+      <c r="K2" s="287"/>
+      <c r="L2" s="287"/>
+      <c r="M2" s="290" t="s">
         <v>299</v>
       </c>
-      <c r="N2" s="287"/>
-      <c r="O2" s="287"/>
+      <c r="N2" s="290"/>
+      <c r="O2" s="290"/>
       <c r="P2" s="90"/>
       <c r="Q2" s="90"/>
     </row>
@@ -8031,21 +8031,21 @@
       <c r="A3" s="203" t="s">
         <v>361</v>
       </c>
-      <c r="B3" s="293" t="s">
+      <c r="B3" s="289" t="s">
         <v>298</v>
       </c>
-      <c r="C3" s="293"/>
-      <c r="D3" s="293"/>
-      <c r="E3" s="293"/>
-      <c r="F3" s="293"/>
-      <c r="G3" s="293" t="s">
+      <c r="C3" s="289"/>
+      <c r="D3" s="289"/>
+      <c r="E3" s="289"/>
+      <c r="F3" s="289"/>
+      <c r="G3" s="289" t="s">
         <v>306</v>
       </c>
-      <c r="H3" s="293"/>
-      <c r="I3" s="293"/>
-      <c r="J3" s="293"/>
-      <c r="K3" s="293"/>
-      <c r="L3" s="293"/>
+      <c r="H3" s="289"/>
+      <c r="I3" s="289"/>
+      <c r="J3" s="289"/>
+      <c r="K3" s="289"/>
+      <c r="L3" s="289"/>
       <c r="M3" s="203" t="s">
         <v>304</v>
       </c>
@@ -8061,25 +8061,25 @@
       <c r="A4" s="206">
         <v>8</v>
       </c>
-      <c r="B4" s="285" t="s">
+      <c r="B4" s="288" t="s">
         <v>246</v>
       </c>
-      <c r="C4" s="285"/>
-      <c r="D4" s="285" t="s">
+      <c r="C4" s="288"/>
+      <c r="D4" s="288" t="s">
         <v>247</v>
       </c>
-      <c r="E4" s="285"/>
-      <c r="F4" s="285"/>
-      <c r="G4" s="285" t="s">
+      <c r="E4" s="288"/>
+      <c r="F4" s="288"/>
+      <c r="G4" s="288" t="s">
         <v>249</v>
       </c>
-      <c r="H4" s="285"/>
-      <c r="I4" s="285"/>
-      <c r="J4" s="285" t="s">
+      <c r="H4" s="288"/>
+      <c r="I4" s="288"/>
+      <c r="J4" s="288" t="s">
         <v>307</v>
       </c>
-      <c r="K4" s="285"/>
-      <c r="L4" s="285"/>
+      <c r="K4" s="288"/>
+      <c r="L4" s="288"/>
       <c r="M4" s="168" t="s">
         <v>154</v>
       </c>
@@ -8092,21 +8092,21 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="193"/>
-      <c r="B5" s="286"/>
-      <c r="C5" s="286"/>
-      <c r="D5" s="286"/>
-      <c r="E5" s="286"/>
-      <c r="F5" s="286"/>
-      <c r="G5" s="286" t="s">
+      <c r="B5" s="285"/>
+      <c r="C5" s="285"/>
+      <c r="D5" s="285"/>
+      <c r="E5" s="285"/>
+      <c r="F5" s="285"/>
+      <c r="G5" s="285" t="s">
         <v>281</v>
       </c>
-      <c r="H5" s="286"/>
-      <c r="I5" s="286"/>
-      <c r="J5" s="286" t="s">
+      <c r="H5" s="285"/>
+      <c r="I5" s="285"/>
+      <c r="J5" s="285" t="s">
         <v>295</v>
       </c>
-      <c r="K5" s="286"/>
-      <c r="L5" s="286"/>
+      <c r="K5" s="285"/>
+      <c r="L5" s="285"/>
       <c r="M5" s="202"/>
       <c r="N5" s="202" t="s">
         <v>391</v>
@@ -8117,23 +8117,23 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="193"/>
-      <c r="B6" s="286" t="s">
+      <c r="B6" s="285" t="s">
         <v>281</v>
       </c>
-      <c r="C6" s="286"/>
-      <c r="D6" s="286" t="s">
+      <c r="C6" s="285"/>
+      <c r="D6" s="285" t="s">
         <v>291</v>
       </c>
-      <c r="E6" s="286"/>
-      <c r="F6" s="286"/>
-      <c r="G6" s="286" t="s">
+      <c r="E6" s="285"/>
+      <c r="F6" s="285"/>
+      <c r="G6" s="285" t="s">
         <v>288</v>
       </c>
-      <c r="H6" s="286"/>
-      <c r="I6" s="286"/>
-      <c r="J6" s="286"/>
-      <c r="K6" s="286"/>
-      <c r="L6" s="286"/>
+      <c r="H6" s="285"/>
+      <c r="I6" s="285"/>
+      <c r="J6" s="285"/>
+      <c r="K6" s="285"/>
+      <c r="L6" s="285"/>
       <c r="M6" s="202"/>
       <c r="N6" s="202" t="s">
         <v>392</v>
@@ -8144,57 +8144,57 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="193"/>
-      <c r="B7" s="286" t="s">
+      <c r="B7" s="285" t="s">
         <v>281</v>
       </c>
-      <c r="C7" s="286"/>
-      <c r="D7" s="286" t="s">
+      <c r="C7" s="285"/>
+      <c r="D7" s="285" t="s">
         <v>292</v>
       </c>
-      <c r="E7" s="286"/>
-      <c r="F7" s="286"/>
-      <c r="G7" s="286"/>
-      <c r="H7" s="286"/>
-      <c r="I7" s="286"/>
-      <c r="J7" s="286"/>
-      <c r="K7" s="286"/>
-      <c r="L7" s="286"/>
+      <c r="E7" s="285"/>
+      <c r="F7" s="285"/>
+      <c r="G7" s="285"/>
+      <c r="H7" s="285"/>
+      <c r="I7" s="285"/>
+      <c r="J7" s="285"/>
+      <c r="K7" s="285"/>
+      <c r="L7" s="285"/>
       <c r="M7" s="202"/>
       <c r="N7" s="202"/>
       <c r="O7" s="166"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="193"/>
-      <c r="B8" s="286"/>
-      <c r="C8" s="286"/>
-      <c r="D8" s="286" t="s">
+      <c r="B8" s="285"/>
+      <c r="C8" s="285"/>
+      <c r="D8" s="285" t="s">
         <v>272</v>
       </c>
-      <c r="E8" s="286"/>
-      <c r="F8" s="286"/>
-      <c r="G8" s="286"/>
-      <c r="H8" s="286"/>
-      <c r="I8" s="286"/>
-      <c r="J8" s="286"/>
-      <c r="K8" s="286"/>
-      <c r="L8" s="286"/>
+      <c r="E8" s="285"/>
+      <c r="F8" s="285"/>
+      <c r="G8" s="285"/>
+      <c r="H8" s="285"/>
+      <c r="I8" s="285"/>
+      <c r="J8" s="285"/>
+      <c r="K8" s="285"/>
+      <c r="L8" s="285"/>
       <c r="M8" s="202"/>
       <c r="N8" s="202"/>
       <c r="O8" s="166"/>
     </row>
     <row r="9" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:17" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="288" t="s">
+      <c r="A10" s="291" t="s">
         <v>359</v>
       </c>
-      <c r="B10" s="289"/>
-      <c r="C10" s="289"/>
-      <c r="D10" s="289"/>
-      <c r="E10" s="289"/>
-      <c r="F10" s="289"/>
-      <c r="G10" s="289"/>
-      <c r="H10" s="289"/>
-      <c r="I10" s="290"/>
+      <c r="B10" s="292"/>
+      <c r="C10" s="292"/>
+      <c r="D10" s="292"/>
+      <c r="E10" s="292"/>
+      <c r="F10" s="292"/>
+      <c r="G10" s="292"/>
+      <c r="H10" s="292"/>
+      <c r="I10" s="293"/>
     </row>
     <row r="11" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="133" t="s">
@@ -8794,12 +8794,15 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="A16:H19"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="B8:C8"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="G6:I6"/>
@@ -8816,15 +8819,12 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="G4:I4"/>
     <mergeCell ref="B2:F2"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="A16:H19"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G7:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8916,68 +8916,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="291" t="s">
+      <c r="A1" s="286" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="291"/>
-      <c r="C1" s="291"/>
-      <c r="D1" s="291"/>
-      <c r="E1" s="291"/>
-      <c r="F1" s="291"/>
-      <c r="G1" s="291"/>
-      <c r="H1" s="291"/>
-      <c r="I1" s="291"/>
-      <c r="J1" s="291"/>
-      <c r="K1" s="291"/>
-      <c r="L1" s="291"/>
-      <c r="M1" s="291"/>
-      <c r="N1" s="291"/>
-      <c r="O1" s="291"/>
-      <c r="P1" s="291"/>
+      <c r="B1" s="286"/>
+      <c r="C1" s="286"/>
+      <c r="D1" s="286"/>
+      <c r="E1" s="286"/>
+      <c r="F1" s="286"/>
+      <c r="G1" s="286"/>
+      <c r="H1" s="286"/>
+      <c r="I1" s="286"/>
+      <c r="J1" s="286"/>
+      <c r="K1" s="286"/>
+      <c r="L1" s="286"/>
+      <c r="M1" s="286"/>
+      <c r="N1" s="286"/>
+      <c r="O1" s="286"/>
+      <c r="P1" s="286"/>
       <c r="Q1" s="32"/>
     </row>
     <row r="2" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="292" t="s">
+      <c r="A2" s="287" t="s">
         <v>282</v>
       </c>
-      <c r="B2" s="292"/>
-      <c r="C2" s="292"/>
-      <c r="D2" s="292"/>
-      <c r="E2" s="292"/>
-      <c r="F2" s="292"/>
-      <c r="G2" s="292" t="s">
+      <c r="B2" s="287"/>
+      <c r="C2" s="287"/>
+      <c r="D2" s="287"/>
+      <c r="E2" s="287"/>
+      <c r="F2" s="287"/>
+      <c r="G2" s="287" t="s">
         <v>248</v>
       </c>
-      <c r="H2" s="292"/>
-      <c r="I2" s="292"/>
-      <c r="J2" s="292"/>
-      <c r="K2" s="292"/>
-      <c r="L2" s="292"/>
-      <c r="M2" s="287" t="s">
+      <c r="H2" s="287"/>
+      <c r="I2" s="287"/>
+      <c r="J2" s="287"/>
+      <c r="K2" s="287"/>
+      <c r="L2" s="287"/>
+      <c r="M2" s="290" t="s">
         <v>297</v>
       </c>
-      <c r="N2" s="287"/>
-      <c r="O2" s="287"/>
-      <c r="P2" s="287"/>
+      <c r="N2" s="290"/>
+      <c r="O2" s="290"/>
+      <c r="P2" s="290"/>
       <c r="Q2" s="90"/>
     </row>
     <row r="3" spans="1:17" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="293" t="s">
+      <c r="A3" s="289" t="s">
         <v>301</v>
       </c>
-      <c r="B3" s="293"/>
-      <c r="C3" s="293"/>
-      <c r="D3" s="293"/>
-      <c r="E3" s="293"/>
-      <c r="F3" s="293"/>
-      <c r="G3" s="293" t="s">
+      <c r="B3" s="289"/>
+      <c r="C3" s="289"/>
+      <c r="D3" s="289"/>
+      <c r="E3" s="289"/>
+      <c r="F3" s="289"/>
+      <c r="G3" s="289" t="s">
         <v>300</v>
       </c>
-      <c r="H3" s="293"/>
-      <c r="I3" s="293"/>
-      <c r="J3" s="293"/>
-      <c r="K3" s="293"/>
-      <c r="L3" s="293"/>
+      <c r="H3" s="289"/>
+      <c r="I3" s="289"/>
+      <c r="J3" s="289"/>
+      <c r="K3" s="289"/>
+      <c r="L3" s="289"/>
       <c r="M3" s="203" t="s">
         <v>303</v>
       </c>
@@ -8993,24 +8993,24 @@
       <c r="Q3" s="207"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="285" t="s">
+      <c r="A4" s="288" t="s">
         <v>246</v>
       </c>
-      <c r="B4" s="285"/>
-      <c r="C4" s="285"/>
-      <c r="D4" s="285" t="s">
+      <c r="B4" s="288"/>
+      <c r="C4" s="288"/>
+      <c r="D4" s="288" t="s">
         <v>247</v>
       </c>
-      <c r="E4" s="285"/>
-      <c r="F4" s="285"/>
-      <c r="G4" s="285" t="s">
+      <c r="E4" s="288"/>
+      <c r="F4" s="288"/>
+      <c r="G4" s="288" t="s">
         <v>250</v>
       </c>
-      <c r="H4" s="285"/>
-      <c r="I4" s="285"/>
-      <c r="J4" s="285"/>
-      <c r="K4" s="285"/>
-      <c r="L4" s="285"/>
+      <c r="H4" s="288"/>
+      <c r="I4" s="288"/>
+      <c r="J4" s="288"/>
+      <c r="K4" s="288"/>
+      <c r="L4" s="288"/>
       <c r="M4" s="168" t="s">
         <v>254</v>
       </c>
@@ -9025,12 +9025,12 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="286"/>
-      <c r="B5" s="286"/>
-      <c r="C5" s="286"/>
-      <c r="D5" s="286"/>
-      <c r="E5" s="286"/>
-      <c r="F5" s="286"/>
+      <c r="A5" s="285"/>
+      <c r="B5" s="285"/>
+      <c r="C5" s="285"/>
+      <c r="D5" s="285"/>
+      <c r="E5" s="285"/>
+      <c r="F5" s="285"/>
       <c r="G5" s="294" t="s">
         <v>4</v>
       </c>
@@ -9051,12 +9051,12 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="286"/>
-      <c r="B6" s="286"/>
-      <c r="C6" s="286"/>
-      <c r="D6" s="286"/>
-      <c r="E6" s="286"/>
-      <c r="F6" s="286"/>
+      <c r="A6" s="285"/>
+      <c r="B6" s="285"/>
+      <c r="C6" s="285"/>
+      <c r="D6" s="285"/>
+      <c r="E6" s="285"/>
+      <c r="F6" s="285"/>
       <c r="G6" s="294"/>
       <c r="H6" s="294"/>
       <c r="I6" s="294"/>
@@ -9069,12 +9069,12 @@
       <c r="P6" s="169"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="286"/>
-      <c r="B7" s="286"/>
-      <c r="C7" s="286"/>
-      <c r="D7" s="286"/>
-      <c r="E7" s="286"/>
-      <c r="F7" s="286"/>
+      <c r="A7" s="285"/>
+      <c r="B7" s="285"/>
+      <c r="C7" s="285"/>
+      <c r="D7" s="285"/>
+      <c r="E7" s="285"/>
+      <c r="F7" s="285"/>
       <c r="G7" s="294"/>
       <c r="H7" s="294"/>
       <c r="I7" s="294"/>
@@ -9087,12 +9087,12 @@
       <c r="P7" s="167"/>
     </row>
     <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="286"/>
-      <c r="B8" s="286"/>
-      <c r="C8" s="286"/>
-      <c r="D8" s="286"/>
-      <c r="E8" s="286"/>
-      <c r="F8" s="286"/>
+      <c r="A8" s="285"/>
+      <c r="B8" s="285"/>
+      <c r="C8" s="285"/>
+      <c r="D8" s="285"/>
+      <c r="E8" s="285"/>
+      <c r="F8" s="285"/>
       <c r="G8" s="294"/>
       <c r="H8" s="294"/>
       <c r="I8" s="294"/>
@@ -9106,17 +9106,17 @@
     </row>
     <row r="9" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:17" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="288" t="s">
+      <c r="A10" s="291" t="s">
         <v>358</v>
       </c>
-      <c r="B10" s="289"/>
-      <c r="C10" s="289"/>
-      <c r="D10" s="289"/>
-      <c r="E10" s="289"/>
-      <c r="F10" s="289"/>
-      <c r="G10" s="289"/>
-      <c r="H10" s="289"/>
-      <c r="I10" s="290"/>
+      <c r="B10" s="292"/>
+      <c r="C10" s="292"/>
+      <c r="D10" s="292"/>
+      <c r="E10" s="292"/>
+      <c r="F10" s="292"/>
+      <c r="G10" s="292"/>
+      <c r="H10" s="292"/>
+      <c r="I10" s="293"/>
     </row>
     <row r="11" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="133" t="s">
@@ -9449,6 +9449,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="G2:L2"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G5:L5"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="G3:L3"/>
     <mergeCell ref="A10:I10"/>
     <mergeCell ref="A21:G21"/>
     <mergeCell ref="D22:G22"/>
@@ -9465,16 +9475,6 @@
     <mergeCell ref="G7:L7"/>
     <mergeCell ref="G8:L8"/>
     <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G5:L5"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="G3:L3"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="G2:L2"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="A1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Correcting filepaths for Travis tests
</commit_message>
<xml_diff>
--- a/test_templates/faulty_batch_template1.xlsx
+++ b/test_templates/faulty_batch_template1.xlsx
@@ -2380,10 +2380,10 @@
     <t>hello</t>
   </si>
   <si>
-    <t>../../TASBEFlowAnalytics-Tutorial/example_assay</t>
-  </si>
-  <si>
-    <t>../../TASBEFlowAnalytics-Tutorial/example_controls</t>
+    <t>../TASBEFlowAnalytics-Tutorial/example_assay</t>
+  </si>
+  <si>
+    <t>../TASBEFlowAnalytics-Tutorial/example_controls</t>
   </si>
 </sst>
 </file>
@@ -3891,10 +3891,88 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3939,89 +4017,11 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4101,31 +4101,31 @@
     <xf numFmtId="0" fontId="14" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="17" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5012,7 +5012,7 @@
   <dimension ref="A1:K48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5033,86 +5033,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="238" t="s">
+      <c r="A1" s="227" t="s">
         <v>385</v>
       </c>
-      <c r="B1" s="239"/>
-      <c r="C1" s="239"/>
-      <c r="D1" s="239"/>
-      <c r="E1" s="239"/>
-      <c r="F1" s="239"/>
-      <c r="G1" s="239"/>
-      <c r="H1" s="239"/>
-      <c r="I1" s="239"/>
-      <c r="J1" s="239"/>
-      <c r="K1" s="240"/>
+      <c r="B1" s="228"/>
+      <c r="C1" s="228"/>
+      <c r="D1" s="228"/>
+      <c r="E1" s="228"/>
+      <c r="F1" s="228"/>
+      <c r="G1" s="228"/>
+      <c r="H1" s="228"/>
+      <c r="I1" s="228"/>
+      <c r="J1" s="228"/>
+      <c r="K1" s="229"/>
     </row>
     <row r="2" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="88"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="217" t="s">
+      <c r="A3" s="243" t="s">
         <v>321</v>
       </c>
-      <c r="B3" s="218"/>
+      <c r="B3" s="244"/>
     </row>
     <row r="4" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="231" t="s">
+      <c r="A4" s="241" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="232"/>
+      <c r="B4" s="242"/>
     </row>
     <row r="5" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="233" t="s">
+      <c r="A5" s="257" t="s">
         <v>182</v>
       </c>
-      <c r="B5" s="234"/>
+      <c r="B5" s="258"/>
     </row>
     <row r="6" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="88"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="217" t="s">
+      <c r="A7" s="243" t="s">
         <v>276</v>
       </c>
-      <c r="B7" s="219"/>
-      <c r="C7" s="219"/>
-      <c r="D7" s="219"/>
-      <c r="E7" s="219"/>
-      <c r="F7" s="219"/>
-      <c r="G7" s="219"/>
-      <c r="H7" s="219"/>
-      <c r="I7" s="219"/>
-      <c r="J7" s="219"/>
-      <c r="K7" s="218"/>
+      <c r="B7" s="245"/>
+      <c r="C7" s="245"/>
+      <c r="D7" s="245"/>
+      <c r="E7" s="245"/>
+      <c r="F7" s="245"/>
+      <c r="G7" s="245"/>
+      <c r="H7" s="245"/>
+      <c r="I7" s="245"/>
+      <c r="J7" s="245"/>
+      <c r="K7" s="244"/>
     </row>
     <row r="8" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="241" t="s">
+      <c r="A8" s="230" t="s">
         <v>162</v>
       </c>
-      <c r="B8" s="242"/>
-      <c r="C8" s="242"/>
-      <c r="D8" s="242"/>
-      <c r="E8" s="242"/>
-      <c r="F8" s="242"/>
-      <c r="G8" s="242"/>
-      <c r="H8" s="242"/>
-      <c r="I8" s="242"/>
-      <c r="J8" s="242"/>
-      <c r="K8" s="243"/>
+      <c r="B8" s="231"/>
+      <c r="C8" s="231"/>
+      <c r="D8" s="231"/>
+      <c r="E8" s="231"/>
+      <c r="F8" s="231"/>
+      <c r="G8" s="231"/>
+      <c r="H8" s="231"/>
+      <c r="I8" s="231"/>
+      <c r="J8" s="231"/>
+      <c r="K8" s="232"/>
     </row>
     <row r="9" spans="1:11" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="244"/>
-      <c r="B9" s="245"/>
-      <c r="C9" s="245"/>
-      <c r="D9" s="245"/>
-      <c r="E9" s="245"/>
-      <c r="F9" s="245"/>
-      <c r="G9" s="245"/>
-      <c r="H9" s="245"/>
-      <c r="I9" s="245"/>
-      <c r="J9" s="245"/>
-      <c r="K9" s="246"/>
+      <c r="A9" s="233"/>
+      <c r="B9" s="234"/>
+      <c r="C9" s="234"/>
+      <c r="D9" s="234"/>
+      <c r="E9" s="234"/>
+      <c r="F9" s="234"/>
+      <c r="G9" s="234"/>
+      <c r="H9" s="234"/>
+      <c r="I9" s="234"/>
+      <c r="J9" s="234"/>
+      <c r="K9" s="235"/>
     </row>
     <row r="10" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="158"/>
@@ -5123,62 +5123,62 @@
       <c r="F10" s="144"/>
     </row>
     <row r="11" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="220" t="s">
+      <c r="A11" s="246" t="s">
         <v>277</v>
       </c>
-      <c r="B11" s="221"/>
-      <c r="C11" s="221"/>
-      <c r="D11" s="222"/>
+      <c r="B11" s="247"/>
+      <c r="C11" s="247"/>
+      <c r="D11" s="248"/>
       <c r="E11" s="89"/>
       <c r="F11" s="144"/>
     </row>
     <row r="12" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="223" t="s">
+      <c r="A12" s="249" t="s">
         <v>163</v>
       </c>
-      <c r="B12" s="224"/>
-      <c r="C12" s="225" t="s">
+      <c r="B12" s="250"/>
+      <c r="C12" s="251" t="s">
         <v>164</v>
       </c>
-      <c r="D12" s="226"/>
+      <c r="D12" s="252"/>
       <c r="E12" s="89"/>
       <c r="F12" s="144"/>
     </row>
     <row r="13" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="227"/>
-      <c r="B13" s="228"/>
-      <c r="C13" s="229"/>
-      <c r="D13" s="230"/>
+      <c r="A13" s="253"/>
+      <c r="B13" s="254"/>
+      <c r="C13" s="255"/>
+      <c r="D13" s="256"/>
       <c r="E13" s="89"/>
       <c r="F13" s="144"/>
     </row>
     <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:11" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="220" t="s">
+      <c r="A15" s="246" t="s">
         <v>278</v>
       </c>
-      <c r="B15" s="222"/>
-      <c r="E15" s="220" t="s">
+      <c r="B15" s="248"/>
+      <c r="E15" s="246" t="s">
         <v>320</v>
       </c>
-      <c r="F15" s="221"/>
-      <c r="G15" s="221"/>
-      <c r="H15" s="221"/>
-      <c r="I15" s="222"/>
+      <c r="F15" s="247"/>
+      <c r="G15" s="247"/>
+      <c r="H15" s="247"/>
+      <c r="I15" s="248"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="231" t="s">
+      <c r="A16" s="241" t="s">
         <v>236</v>
       </c>
-      <c r="B16" s="232"/>
+      <c r="B16" s="242"/>
       <c r="D16" s="90"/>
-      <c r="E16" s="247" t="s">
+      <c r="E16" s="236" t="s">
         <v>197</v>
       </c>
-      <c r="F16" s="248"/>
-      <c r="G16" s="248"/>
-      <c r="H16" s="248"/>
-      <c r="I16" s="249"/>
+      <c r="F16" s="237"/>
+      <c r="G16" s="237"/>
+      <c r="H16" s="237"/>
+      <c r="I16" s="238"/>
     </row>
     <row r="17" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="159" t="s">
@@ -5188,10 +5188,10 @@
         <v>281</v>
       </c>
       <c r="C17" s="91"/>
-      <c r="E17" s="250" t="s">
+      <c r="E17" s="239" t="s">
         <v>235</v>
       </c>
-      <c r="F17" s="251"/>
+      <c r="F17" s="240"/>
       <c r="G17" s="84" t="s">
         <v>159</v>
       </c>
@@ -5221,7 +5221,7 @@
       <c r="H18" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="I18" s="235" t="s">
+      <c r="I18" s="215" t="s">
         <v>474</v>
       </c>
       <c r="J18" s="82"/>
@@ -5244,7 +5244,7 @@
       <c r="H19" s="75" t="s">
         <v>196</v>
       </c>
-      <c r="I19" s="235"/>
+      <c r="I19" s="215"/>
       <c r="J19" s="82"/>
     </row>
     <row r="20" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5261,7 +5261,7 @@
       </c>
       <c r="G20" s="72"/>
       <c r="H20" s="72"/>
-      <c r="I20" s="236"/>
+      <c r="I20" s="216"/>
       <c r="J20" s="82"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -5283,24 +5283,24 @@
       <c r="A23" s="163"/>
       <c r="B23" s="94"/>
       <c r="C23" s="93"/>
-      <c r="E23" s="215" t="s">
+      <c r="E23" s="217" t="s">
         <v>198</v>
       </c>
-      <c r="F23" s="237"/>
-      <c r="G23" s="237"/>
-      <c r="H23" s="237"/>
-      <c r="I23" s="216"/>
+      <c r="F23" s="218"/>
+      <c r="G23" s="218"/>
+      <c r="H23" s="218"/>
+      <c r="I23" s="219"/>
     </row>
     <row r="24" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="215" t="s">
+      <c r="A24" s="217" t="s">
         <v>240</v>
       </c>
-      <c r="B24" s="216"/>
+      <c r="B24" s="219"/>
       <c r="C24" s="33"/>
-      <c r="E24" s="255" t="s">
+      <c r="E24" s="223" t="s">
         <v>235</v>
       </c>
-      <c r="F24" s="256"/>
+      <c r="F24" s="224"/>
       <c r="G24" s="83" t="s">
         <v>159</v>
       </c>
@@ -5329,7 +5329,7 @@
       <c r="H25" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="I25" s="252" t="s">
+      <c r="I25" s="220" t="s">
         <v>475</v>
       </c>
     </row>
@@ -5353,7 +5353,7 @@
       <c r="H26" s="75" t="s">
         <v>201</v>
       </c>
-      <c r="I26" s="253"/>
+      <c r="I26" s="221"/>
     </row>
     <row r="27" spans="1:10" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="161" t="s">
@@ -5369,7 +5369,7 @@
       </c>
       <c r="G27" s="72"/>
       <c r="H27" s="72"/>
-      <c r="I27" s="254"/>
+      <c r="I27" s="222"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="161" t="s">
@@ -5393,22 +5393,22 @@
       <c r="A30" s="162"/>
       <c r="B30" s="119"/>
       <c r="C30" s="91"/>
-      <c r="E30" s="215" t="s">
+      <c r="E30" s="217" t="s">
         <v>199</v>
       </c>
-      <c r="F30" s="237"/>
-      <c r="G30" s="237"/>
-      <c r="H30" s="237"/>
-      <c r="I30" s="216"/>
+      <c r="F30" s="218"/>
+      <c r="G30" s="218"/>
+      <c r="H30" s="218"/>
+      <c r="I30" s="219"/>
     </row>
     <row r="31" spans="1:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="163"/>
       <c r="B31" s="93"/>
       <c r="C31" s="93"/>
-      <c r="E31" s="257" t="s">
+      <c r="E31" s="225" t="s">
         <v>472</v>
       </c>
-      <c r="F31" s="258"/>
+      <c r="F31" s="226"/>
       <c r="G31" s="213" t="s">
         <v>159</v>
       </c>
@@ -5420,10 +5420,10 @@
       </c>
     </row>
     <row r="32" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="215" t="s">
+      <c r="A32" s="217" t="s">
         <v>241</v>
       </c>
-      <c r="B32" s="216"/>
+      <c r="B32" s="219"/>
       <c r="C32" s="33"/>
       <c r="E32" s="85">
         <v>1</v>
@@ -5433,7 +5433,7 @@
       </c>
       <c r="G32" s="34"/>
       <c r="H32" s="75"/>
-      <c r="I32" s="235"/>
+      <c r="I32" s="215"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="159" t="s">
@@ -5453,7 +5453,7 @@
         <v>5</v>
       </c>
       <c r="H33" s="34"/>
-      <c r="I33" s="235"/>
+      <c r="I33" s="215"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="160" t="s">
@@ -5468,7 +5468,7 @@
       <c r="F34" s="95"/>
       <c r="G34" s="34"/>
       <c r="H34" s="75"/>
-      <c r="I34" s="235"/>
+      <c r="I34" s="215"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="161" t="s">
@@ -5481,7 +5481,7 @@
       <c r="F35" s="95"/>
       <c r="G35" s="34"/>
       <c r="H35" s="34"/>
-      <c r="I35" s="235"/>
+      <c r="I35" s="215"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="161" t="s">
@@ -5494,7 +5494,7 @@
       <c r="F36" s="95"/>
       <c r="G36" s="34"/>
       <c r="H36" s="34"/>
-      <c r="I36" s="235"/>
+      <c r="I36" s="215"/>
     </row>
     <row r="37" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="161" t="s">
@@ -5507,7 +5507,7 @@
       <c r="F37" s="142"/>
       <c r="G37" s="72"/>
       <c r="H37" s="72"/>
-      <c r="I37" s="236"/>
+      <c r="I37" s="216"/>
     </row>
     <row r="38" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="162" t="s">
@@ -5520,17 +5520,17 @@
       <c r="B39" s="123"/>
     </row>
     <row r="40" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="E40" s="215" t="s">
+      <c r="E40" s="217" t="s">
         <v>200</v>
       </c>
-      <c r="F40" s="237"/>
-      <c r="G40" s="237"/>
-      <c r="H40" s="237"/>
-      <c r="I40" s="216"/>
+      <c r="F40" s="218"/>
+      <c r="G40" s="218"/>
+      <c r="H40" s="218"/>
+      <c r="I40" s="219"/>
     </row>
     <row r="41" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="E41" s="255"/>
-      <c r="F41" s="256"/>
+      <c r="E41" s="223"/>
+      <c r="F41" s="224"/>
       <c r="G41" s="83" t="s">
         <v>159</v>
       </c>
@@ -5548,7 +5548,7 @@
       <c r="F42" s="95"/>
       <c r="G42" s="34"/>
       <c r="H42" s="75"/>
-      <c r="I42" s="235"/>
+      <c r="I42" s="215"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E43" s="85">
@@ -5557,7 +5557,7 @@
       <c r="F43" s="95"/>
       <c r="G43" s="34"/>
       <c r="H43" s="34"/>
-      <c r="I43" s="235"/>
+      <c r="I43" s="215"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E44" s="85">
@@ -5566,7 +5566,7 @@
       <c r="F44" s="95"/>
       <c r="G44" s="34"/>
       <c r="H44" s="75"/>
-      <c r="I44" s="235"/>
+      <c r="I44" s="215"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E45" s="85">
@@ -5575,7 +5575,7 @@
       <c r="F45" s="95"/>
       <c r="G45" s="34"/>
       <c r="H45" s="34"/>
-      <c r="I45" s="235"/>
+      <c r="I45" s="215"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E46" s="85">
@@ -5584,7 +5584,7 @@
       <c r="F46" s="95"/>
       <c r="G46" s="34"/>
       <c r="H46" s="34"/>
-      <c r="I46" s="235"/>
+      <c r="I46" s="215"/>
     </row>
     <row r="47" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E47" s="86">
@@ -5593,25 +5593,11 @@
       <c r="F47" s="142"/>
       <c r="G47" s="72"/>
       <c r="H47" s="72"/>
-      <c r="I47" s="236"/>
+      <c r="I47" s="216"/>
     </row>
     <row r="48" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="I42:I47"/>
-    <mergeCell ref="E40:I40"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="I25:I27"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A8:K8"/>
-    <mergeCell ref="A9:K9"/>
-    <mergeCell ref="E16:I16"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="A16:B16"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="A3:B3"/>
@@ -5627,6 +5613,20 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="I32:I37"/>
     <mergeCell ref="E30:I30"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A8:K8"/>
+    <mergeCell ref="A9:K9"/>
+    <mergeCell ref="E16:I16"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="I42:I47"/>
+    <mergeCell ref="E40:I40"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="I25:I27"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E31:F31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7980,23 +7980,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="286" t="s">
+      <c r="A1" s="291" t="s">
         <v>244</v>
       </c>
-      <c r="B1" s="286"/>
-      <c r="C1" s="286"/>
-      <c r="D1" s="286"/>
-      <c r="E1" s="286"/>
-      <c r="F1" s="286"/>
-      <c r="G1" s="286"/>
-      <c r="H1" s="286"/>
-      <c r="I1" s="286"/>
-      <c r="J1" s="286"/>
-      <c r="K1" s="286"/>
-      <c r="L1" s="286"/>
-      <c r="M1" s="286"/>
-      <c r="N1" s="286"/>
-      <c r="O1" s="286"/>
+      <c r="B1" s="291"/>
+      <c r="C1" s="291"/>
+      <c r="D1" s="291"/>
+      <c r="E1" s="291"/>
+      <c r="F1" s="291"/>
+      <c r="G1" s="291"/>
+      <c r="H1" s="291"/>
+      <c r="I1" s="291"/>
+      <c r="J1" s="291"/>
+      <c r="K1" s="291"/>
+      <c r="L1" s="291"/>
+      <c r="M1" s="291"/>
+      <c r="N1" s="291"/>
+      <c r="O1" s="291"/>
       <c r="P1" s="32"/>
       <c r="Q1" s="32"/>
     </row>
@@ -8004,26 +8004,26 @@
       <c r="A2" s="204" t="s">
         <v>360</v>
       </c>
-      <c r="B2" s="287" t="s">
+      <c r="B2" s="292" t="s">
         <v>282</v>
       </c>
-      <c r="C2" s="287"/>
-      <c r="D2" s="287"/>
-      <c r="E2" s="287"/>
-      <c r="F2" s="287"/>
-      <c r="G2" s="287" t="s">
+      <c r="C2" s="292"/>
+      <c r="D2" s="292"/>
+      <c r="E2" s="292"/>
+      <c r="F2" s="292"/>
+      <c r="G2" s="292" t="s">
         <v>248</v>
       </c>
-      <c r="H2" s="287"/>
-      <c r="I2" s="287"/>
-      <c r="J2" s="287"/>
-      <c r="K2" s="287"/>
-      <c r="L2" s="287"/>
-      <c r="M2" s="290" t="s">
+      <c r="H2" s="292"/>
+      <c r="I2" s="292"/>
+      <c r="J2" s="292"/>
+      <c r="K2" s="292"/>
+      <c r="L2" s="292"/>
+      <c r="M2" s="287" t="s">
         <v>299</v>
       </c>
-      <c r="N2" s="290"/>
-      <c r="O2" s="290"/>
+      <c r="N2" s="287"/>
+      <c r="O2" s="287"/>
       <c r="P2" s="90"/>
       <c r="Q2" s="90"/>
     </row>
@@ -8031,21 +8031,21 @@
       <c r="A3" s="203" t="s">
         <v>361</v>
       </c>
-      <c r="B3" s="289" t="s">
+      <c r="B3" s="293" t="s">
         <v>298</v>
       </c>
-      <c r="C3" s="289"/>
-      <c r="D3" s="289"/>
-      <c r="E3" s="289"/>
-      <c r="F3" s="289"/>
-      <c r="G3" s="289" t="s">
+      <c r="C3" s="293"/>
+      <c r="D3" s="293"/>
+      <c r="E3" s="293"/>
+      <c r="F3" s="293"/>
+      <c r="G3" s="293" t="s">
         <v>306</v>
       </c>
-      <c r="H3" s="289"/>
-      <c r="I3" s="289"/>
-      <c r="J3" s="289"/>
-      <c r="K3" s="289"/>
-      <c r="L3" s="289"/>
+      <c r="H3" s="293"/>
+      <c r="I3" s="293"/>
+      <c r="J3" s="293"/>
+      <c r="K3" s="293"/>
+      <c r="L3" s="293"/>
       <c r="M3" s="203" t="s">
         <v>304</v>
       </c>
@@ -8061,25 +8061,25 @@
       <c r="A4" s="206">
         <v>8</v>
       </c>
-      <c r="B4" s="288" t="s">
+      <c r="B4" s="285" t="s">
         <v>246</v>
       </c>
-      <c r="C4" s="288"/>
-      <c r="D4" s="288" t="s">
+      <c r="C4" s="285"/>
+      <c r="D4" s="285" t="s">
         <v>247</v>
       </c>
-      <c r="E4" s="288"/>
-      <c r="F4" s="288"/>
-      <c r="G4" s="288" t="s">
+      <c r="E4" s="285"/>
+      <c r="F4" s="285"/>
+      <c r="G4" s="285" t="s">
         <v>249</v>
       </c>
-      <c r="H4" s="288"/>
-      <c r="I4" s="288"/>
-      <c r="J4" s="288" t="s">
+      <c r="H4" s="285"/>
+      <c r="I4" s="285"/>
+      <c r="J4" s="285" t="s">
         <v>307</v>
       </c>
-      <c r="K4" s="288"/>
-      <c r="L4" s="288"/>
+      <c r="K4" s="285"/>
+      <c r="L4" s="285"/>
       <c r="M4" s="168" t="s">
         <v>154</v>
       </c>
@@ -8092,21 +8092,21 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="193"/>
-      <c r="B5" s="285"/>
-      <c r="C5" s="285"/>
-      <c r="D5" s="285"/>
-      <c r="E5" s="285"/>
-      <c r="F5" s="285"/>
-      <c r="G5" s="285" t="s">
+      <c r="B5" s="286"/>
+      <c r="C5" s="286"/>
+      <c r="D5" s="286"/>
+      <c r="E5" s="286"/>
+      <c r="F5" s="286"/>
+      <c r="G5" s="286" t="s">
         <v>281</v>
       </c>
-      <c r="H5" s="285"/>
-      <c r="I5" s="285"/>
-      <c r="J5" s="285" t="s">
+      <c r="H5" s="286"/>
+      <c r="I5" s="286"/>
+      <c r="J5" s="286" t="s">
         <v>295</v>
       </c>
-      <c r="K5" s="285"/>
-      <c r="L5" s="285"/>
+      <c r="K5" s="286"/>
+      <c r="L5" s="286"/>
       <c r="M5" s="202"/>
       <c r="N5" s="202" t="s">
         <v>391</v>
@@ -8117,23 +8117,23 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="193"/>
-      <c r="B6" s="285" t="s">
+      <c r="B6" s="286" t="s">
         <v>281</v>
       </c>
-      <c r="C6" s="285"/>
-      <c r="D6" s="285" t="s">
+      <c r="C6" s="286"/>
+      <c r="D6" s="286" t="s">
         <v>291</v>
       </c>
-      <c r="E6" s="285"/>
-      <c r="F6" s="285"/>
-      <c r="G6" s="285" t="s">
+      <c r="E6" s="286"/>
+      <c r="F6" s="286"/>
+      <c r="G6" s="286" t="s">
         <v>288</v>
       </c>
-      <c r="H6" s="285"/>
-      <c r="I6" s="285"/>
-      <c r="J6" s="285"/>
-      <c r="K6" s="285"/>
-      <c r="L6" s="285"/>
+      <c r="H6" s="286"/>
+      <c r="I6" s="286"/>
+      <c r="J6" s="286"/>
+      <c r="K6" s="286"/>
+      <c r="L6" s="286"/>
       <c r="M6" s="202"/>
       <c r="N6" s="202" t="s">
         <v>392</v>
@@ -8144,57 +8144,57 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="193"/>
-      <c r="B7" s="285" t="s">
+      <c r="B7" s="286" t="s">
         <v>281</v>
       </c>
-      <c r="C7" s="285"/>
-      <c r="D7" s="285" t="s">
+      <c r="C7" s="286"/>
+      <c r="D7" s="286" t="s">
         <v>292</v>
       </c>
-      <c r="E7" s="285"/>
-      <c r="F7" s="285"/>
-      <c r="G7" s="285"/>
-      <c r="H7" s="285"/>
-      <c r="I7" s="285"/>
-      <c r="J7" s="285"/>
-      <c r="K7" s="285"/>
-      <c r="L7" s="285"/>
+      <c r="E7" s="286"/>
+      <c r="F7" s="286"/>
+      <c r="G7" s="286"/>
+      <c r="H7" s="286"/>
+      <c r="I7" s="286"/>
+      <c r="J7" s="286"/>
+      <c r="K7" s="286"/>
+      <c r="L7" s="286"/>
       <c r="M7" s="202"/>
       <c r="N7" s="202"/>
       <c r="O7" s="166"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="193"/>
-      <c r="B8" s="285"/>
-      <c r="C8" s="285"/>
-      <c r="D8" s="285" t="s">
+      <c r="B8" s="286"/>
+      <c r="C8" s="286"/>
+      <c r="D8" s="286" t="s">
         <v>272</v>
       </c>
-      <c r="E8" s="285"/>
-      <c r="F8" s="285"/>
-      <c r="G8" s="285"/>
-      <c r="H8" s="285"/>
-      <c r="I8" s="285"/>
-      <c r="J8" s="285"/>
-      <c r="K8" s="285"/>
-      <c r="L8" s="285"/>
+      <c r="E8" s="286"/>
+      <c r="F8" s="286"/>
+      <c r="G8" s="286"/>
+      <c r="H8" s="286"/>
+      <c r="I8" s="286"/>
+      <c r="J8" s="286"/>
+      <c r="K8" s="286"/>
+      <c r="L8" s="286"/>
       <c r="M8" s="202"/>
       <c r="N8" s="202"/>
       <c r="O8" s="166"/>
     </row>
     <row r="9" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:17" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="291" t="s">
+      <c r="A10" s="288" t="s">
         <v>359</v>
       </c>
-      <c r="B10" s="292"/>
-      <c r="C10" s="292"/>
-      <c r="D10" s="292"/>
-      <c r="E10" s="292"/>
-      <c r="F10" s="292"/>
-      <c r="G10" s="292"/>
-      <c r="H10" s="292"/>
-      <c r="I10" s="293"/>
+      <c r="B10" s="289"/>
+      <c r="C10" s="289"/>
+      <c r="D10" s="289"/>
+      <c r="E10" s="289"/>
+      <c r="F10" s="289"/>
+      <c r="G10" s="289"/>
+      <c r="H10" s="289"/>
+      <c r="I10" s="290"/>
     </row>
     <row r="11" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="133" t="s">
@@ -8794,15 +8794,12 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="A16:H19"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G7:I7"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="G6:I6"/>
@@ -8819,12 +8816,15 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="G4:I4"/>
     <mergeCell ref="B2:F2"/>
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="A16:H19"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="B8:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8916,68 +8916,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="286" t="s">
+      <c r="A1" s="291" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="286"/>
-      <c r="C1" s="286"/>
-      <c r="D1" s="286"/>
-      <c r="E1" s="286"/>
-      <c r="F1" s="286"/>
-      <c r="G1" s="286"/>
-      <c r="H1" s="286"/>
-      <c r="I1" s="286"/>
-      <c r="J1" s="286"/>
-      <c r="K1" s="286"/>
-      <c r="L1" s="286"/>
-      <c r="M1" s="286"/>
-      <c r="N1" s="286"/>
-      <c r="O1" s="286"/>
-      <c r="P1" s="286"/>
+      <c r="B1" s="291"/>
+      <c r="C1" s="291"/>
+      <c r="D1" s="291"/>
+      <c r="E1" s="291"/>
+      <c r="F1" s="291"/>
+      <c r="G1" s="291"/>
+      <c r="H1" s="291"/>
+      <c r="I1" s="291"/>
+      <c r="J1" s="291"/>
+      <c r="K1" s="291"/>
+      <c r="L1" s="291"/>
+      <c r="M1" s="291"/>
+      <c r="N1" s="291"/>
+      <c r="O1" s="291"/>
+      <c r="P1" s="291"/>
       <c r="Q1" s="32"/>
     </row>
     <row r="2" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="287" t="s">
+      <c r="A2" s="292" t="s">
         <v>282</v>
       </c>
-      <c r="B2" s="287"/>
-      <c r="C2" s="287"/>
-      <c r="D2" s="287"/>
-      <c r="E2" s="287"/>
-      <c r="F2" s="287"/>
-      <c r="G2" s="287" t="s">
+      <c r="B2" s="292"/>
+      <c r="C2" s="292"/>
+      <c r="D2" s="292"/>
+      <c r="E2" s="292"/>
+      <c r="F2" s="292"/>
+      <c r="G2" s="292" t="s">
         <v>248</v>
       </c>
-      <c r="H2" s="287"/>
-      <c r="I2" s="287"/>
-      <c r="J2" s="287"/>
-      <c r="K2" s="287"/>
-      <c r="L2" s="287"/>
-      <c r="M2" s="290" t="s">
+      <c r="H2" s="292"/>
+      <c r="I2" s="292"/>
+      <c r="J2" s="292"/>
+      <c r="K2" s="292"/>
+      <c r="L2" s="292"/>
+      <c r="M2" s="287" t="s">
         <v>297</v>
       </c>
-      <c r="N2" s="290"/>
-      <c r="O2" s="290"/>
-      <c r="P2" s="290"/>
+      <c r="N2" s="287"/>
+      <c r="O2" s="287"/>
+      <c r="P2" s="287"/>
       <c r="Q2" s="90"/>
     </row>
     <row r="3" spans="1:17" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="289" t="s">
+      <c r="A3" s="293" t="s">
         <v>301</v>
       </c>
-      <c r="B3" s="289"/>
-      <c r="C3" s="289"/>
-      <c r="D3" s="289"/>
-      <c r="E3" s="289"/>
-      <c r="F3" s="289"/>
-      <c r="G3" s="289" t="s">
+      <c r="B3" s="293"/>
+      <c r="C3" s="293"/>
+      <c r="D3" s="293"/>
+      <c r="E3" s="293"/>
+      <c r="F3" s="293"/>
+      <c r="G3" s="293" t="s">
         <v>300</v>
       </c>
-      <c r="H3" s="289"/>
-      <c r="I3" s="289"/>
-      <c r="J3" s="289"/>
-      <c r="K3" s="289"/>
-      <c r="L3" s="289"/>
+      <c r="H3" s="293"/>
+      <c r="I3" s="293"/>
+      <c r="J3" s="293"/>
+      <c r="K3" s="293"/>
+      <c r="L3" s="293"/>
       <c r="M3" s="203" t="s">
         <v>303</v>
       </c>
@@ -8993,24 +8993,24 @@
       <c r="Q3" s="207"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="288" t="s">
+      <c r="A4" s="285" t="s">
         <v>246</v>
       </c>
-      <c r="B4" s="288"/>
-      <c r="C4" s="288"/>
-      <c r="D4" s="288" t="s">
+      <c r="B4" s="285"/>
+      <c r="C4" s="285"/>
+      <c r="D4" s="285" t="s">
         <v>247</v>
       </c>
-      <c r="E4" s="288"/>
-      <c r="F4" s="288"/>
-      <c r="G4" s="288" t="s">
+      <c r="E4" s="285"/>
+      <c r="F4" s="285"/>
+      <c r="G4" s="285" t="s">
         <v>250</v>
       </c>
-      <c r="H4" s="288"/>
-      <c r="I4" s="288"/>
-      <c r="J4" s="288"/>
-      <c r="K4" s="288"/>
-      <c r="L4" s="288"/>
+      <c r="H4" s="285"/>
+      <c r="I4" s="285"/>
+      <c r="J4" s="285"/>
+      <c r="K4" s="285"/>
+      <c r="L4" s="285"/>
       <c r="M4" s="168" t="s">
         <v>254</v>
       </c>
@@ -9025,12 +9025,12 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="285"/>
-      <c r="B5" s="285"/>
-      <c r="C5" s="285"/>
-      <c r="D5" s="285"/>
-      <c r="E5" s="285"/>
-      <c r="F5" s="285"/>
+      <c r="A5" s="286"/>
+      <c r="B5" s="286"/>
+      <c r="C5" s="286"/>
+      <c r="D5" s="286"/>
+      <c r="E5" s="286"/>
+      <c r="F5" s="286"/>
       <c r="G5" s="294" t="s">
         <v>4</v>
       </c>
@@ -9051,12 +9051,12 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="285"/>
-      <c r="B6" s="285"/>
-      <c r="C6" s="285"/>
-      <c r="D6" s="285"/>
-      <c r="E6" s="285"/>
-      <c r="F6" s="285"/>
+      <c r="A6" s="286"/>
+      <c r="B6" s="286"/>
+      <c r="C6" s="286"/>
+      <c r="D6" s="286"/>
+      <c r="E6" s="286"/>
+      <c r="F6" s="286"/>
       <c r="G6" s="294"/>
       <c r="H6" s="294"/>
       <c r="I6" s="294"/>
@@ -9069,12 +9069,12 @@
       <c r="P6" s="169"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="285"/>
-      <c r="B7" s="285"/>
-      <c r="C7" s="285"/>
-      <c r="D7" s="285"/>
-      <c r="E7" s="285"/>
-      <c r="F7" s="285"/>
+      <c r="A7" s="286"/>
+      <c r="B7" s="286"/>
+      <c r="C7" s="286"/>
+      <c r="D7" s="286"/>
+      <c r="E7" s="286"/>
+      <c r="F7" s="286"/>
       <c r="G7" s="294"/>
       <c r="H7" s="294"/>
       <c r="I7" s="294"/>
@@ -9087,12 +9087,12 @@
       <c r="P7" s="167"/>
     </row>
     <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="285"/>
-      <c r="B8" s="285"/>
-      <c r="C8" s="285"/>
-      <c r="D8" s="285"/>
-      <c r="E8" s="285"/>
-      <c r="F8" s="285"/>
+      <c r="A8" s="286"/>
+      <c r="B8" s="286"/>
+      <c r="C8" s="286"/>
+      <c r="D8" s="286"/>
+      <c r="E8" s="286"/>
+      <c r="F8" s="286"/>
       <c r="G8" s="294"/>
       <c r="H8" s="294"/>
       <c r="I8" s="294"/>
@@ -9106,17 +9106,17 @@
     </row>
     <row r="9" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:17" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="291" t="s">
+      <c r="A10" s="288" t="s">
         <v>358</v>
       </c>
-      <c r="B10" s="292"/>
-      <c r="C10" s="292"/>
-      <c r="D10" s="292"/>
-      <c r="E10" s="292"/>
-      <c r="F10" s="292"/>
-      <c r="G10" s="292"/>
-      <c r="H10" s="292"/>
-      <c r="I10" s="293"/>
+      <c r="B10" s="289"/>
+      <c r="C10" s="289"/>
+      <c r="D10" s="289"/>
+      <c r="E10" s="289"/>
+      <c r="F10" s="289"/>
+      <c r="G10" s="289"/>
+      <c r="H10" s="289"/>
+      <c r="I10" s="290"/>
     </row>
     <row r="11" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="133" t="s">
@@ -9449,16 +9449,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="G2:L2"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G5:L5"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="G3:L3"/>
     <mergeCell ref="A10:I10"/>
     <mergeCell ref="A21:G21"/>
     <mergeCell ref="D22:G22"/>
@@ -9475,6 +9465,16 @@
     <mergeCell ref="G7:L7"/>
     <mergeCell ref="G8:L8"/>
     <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G5:L5"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="G3:L3"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="G2:L2"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="A1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added tests for #287
</commit_message>
<xml_diff>
--- a/test_templates/faulty_batch_template1.xlsx
+++ b/test_templates/faulty_batch_template1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-50385" yWindow="1080" windowWidth="47745" windowHeight="25665" firstSheet="4" activeTab="5"/>
+    <workbookView xWindow="-50385" yWindow="1080" windowWidth="47745" windowHeight="25665" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Experiment" sheetId="6" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="939" uniqueCount="480">
   <si>
     <t>blank plasmid</t>
   </si>
@@ -3911,10 +3911,95 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3959,89 +4044,11 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4121,31 +4128,31 @@
     <xf numFmtId="0" fontId="14" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="17" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4201,13 +4208,6 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5060,86 +5060,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="237" t="s">
+      <c r="A1" s="228" t="s">
         <v>385</v>
       </c>
-      <c r="B1" s="238"/>
-      <c r="C1" s="238"/>
-      <c r="D1" s="238"/>
-      <c r="E1" s="238"/>
-      <c r="F1" s="238"/>
-      <c r="G1" s="238"/>
-      <c r="H1" s="238"/>
-      <c r="I1" s="238"/>
-      <c r="J1" s="238"/>
-      <c r="K1" s="239"/>
+      <c r="B1" s="229"/>
+      <c r="C1" s="229"/>
+      <c r="D1" s="229"/>
+      <c r="E1" s="229"/>
+      <c r="F1" s="229"/>
+      <c r="G1" s="229"/>
+      <c r="H1" s="229"/>
+      <c r="I1" s="229"/>
+      <c r="J1" s="229"/>
+      <c r="K1" s="230"/>
     </row>
     <row r="2" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="87"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="216" t="s">
+      <c r="A3" s="244" t="s">
         <v>321</v>
       </c>
-      <c r="B3" s="217"/>
+      <c r="B3" s="245"/>
     </row>
     <row r="4" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="230" t="s">
+      <c r="A4" s="242" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="231"/>
+      <c r="B4" s="243"/>
     </row>
     <row r="5" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="232" t="s">
+      <c r="A5" s="258" t="s">
         <v>182</v>
       </c>
-      <c r="B5" s="233"/>
+      <c r="B5" s="259"/>
     </row>
     <row r="6" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="87"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="216" t="s">
+      <c r="A7" s="244" t="s">
         <v>276</v>
       </c>
-      <c r="B7" s="218"/>
-      <c r="C7" s="218"/>
-      <c r="D7" s="218"/>
-      <c r="E7" s="218"/>
-      <c r="F7" s="218"/>
-      <c r="G7" s="218"/>
-      <c r="H7" s="218"/>
-      <c r="I7" s="218"/>
-      <c r="J7" s="218"/>
-      <c r="K7" s="217"/>
+      <c r="B7" s="246"/>
+      <c r="C7" s="246"/>
+      <c r="D7" s="246"/>
+      <c r="E7" s="246"/>
+      <c r="F7" s="246"/>
+      <c r="G7" s="246"/>
+      <c r="H7" s="246"/>
+      <c r="I7" s="246"/>
+      <c r="J7" s="246"/>
+      <c r="K7" s="245"/>
     </row>
     <row r="8" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="240" t="s">
+      <c r="A8" s="231" t="s">
         <v>162</v>
       </c>
-      <c r="B8" s="241"/>
-      <c r="C8" s="241"/>
-      <c r="D8" s="241"/>
-      <c r="E8" s="241"/>
-      <c r="F8" s="241"/>
-      <c r="G8" s="241"/>
-      <c r="H8" s="241"/>
-      <c r="I8" s="241"/>
-      <c r="J8" s="241"/>
-      <c r="K8" s="242"/>
+      <c r="B8" s="232"/>
+      <c r="C8" s="232"/>
+      <c r="D8" s="232"/>
+      <c r="E8" s="232"/>
+      <c r="F8" s="232"/>
+      <c r="G8" s="232"/>
+      <c r="H8" s="232"/>
+      <c r="I8" s="232"/>
+      <c r="J8" s="232"/>
+      <c r="K8" s="233"/>
     </row>
     <row r="9" spans="1:11" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="243"/>
-      <c r="B9" s="244"/>
-      <c r="C9" s="244"/>
-      <c r="D9" s="244"/>
-      <c r="E9" s="244"/>
-      <c r="F9" s="244"/>
-      <c r="G9" s="244"/>
-      <c r="H9" s="244"/>
-      <c r="I9" s="244"/>
-      <c r="J9" s="244"/>
-      <c r="K9" s="245"/>
+      <c r="A9" s="234"/>
+      <c r="B9" s="235"/>
+      <c r="C9" s="235"/>
+      <c r="D9" s="235"/>
+      <c r="E9" s="235"/>
+      <c r="F9" s="235"/>
+      <c r="G9" s="235"/>
+      <c r="H9" s="235"/>
+      <c r="I9" s="235"/>
+      <c r="J9" s="235"/>
+      <c r="K9" s="236"/>
     </row>
     <row r="10" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="157"/>
@@ -5150,62 +5150,62 @@
       <c r="F10" s="143"/>
     </row>
     <row r="11" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="219" t="s">
+      <c r="A11" s="247" t="s">
         <v>277</v>
       </c>
-      <c r="B11" s="220"/>
-      <c r="C11" s="220"/>
-      <c r="D11" s="221"/>
+      <c r="B11" s="248"/>
+      <c r="C11" s="248"/>
+      <c r="D11" s="249"/>
       <c r="E11" s="88"/>
       <c r="F11" s="143"/>
     </row>
     <row r="12" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="222" t="s">
+      <c r="A12" s="250" t="s">
         <v>163</v>
       </c>
-      <c r="B12" s="223"/>
-      <c r="C12" s="224" t="s">
+      <c r="B12" s="251"/>
+      <c r="C12" s="252" t="s">
         <v>164</v>
       </c>
-      <c r="D12" s="225"/>
+      <c r="D12" s="253"/>
       <c r="E12" s="88"/>
       <c r="F12" s="143"/>
     </row>
     <row r="13" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="226"/>
-      <c r="B13" s="227"/>
-      <c r="C13" s="228"/>
-      <c r="D13" s="229"/>
+      <c r="A13" s="254"/>
+      <c r="B13" s="255"/>
+      <c r="C13" s="256"/>
+      <c r="D13" s="257"/>
       <c r="E13" s="88"/>
       <c r="F13" s="143"/>
     </row>
     <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:11" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="219" t="s">
+      <c r="A15" s="247" t="s">
         <v>278</v>
       </c>
-      <c r="B15" s="221"/>
-      <c r="E15" s="219" t="s">
+      <c r="B15" s="249"/>
+      <c r="E15" s="247" t="s">
         <v>320</v>
       </c>
-      <c r="F15" s="220"/>
-      <c r="G15" s="220"/>
-      <c r="H15" s="220"/>
-      <c r="I15" s="221"/>
+      <c r="F15" s="248"/>
+      <c r="G15" s="248"/>
+      <c r="H15" s="248"/>
+      <c r="I15" s="249"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="230" t="s">
+      <c r="A16" s="242" t="s">
         <v>236</v>
       </c>
-      <c r="B16" s="231"/>
+      <c r="B16" s="243"/>
       <c r="D16" s="89"/>
-      <c r="E16" s="246" t="s">
+      <c r="E16" s="237" t="s">
         <v>197</v>
       </c>
-      <c r="F16" s="247"/>
-      <c r="G16" s="247"/>
-      <c r="H16" s="247"/>
-      <c r="I16" s="248"/>
+      <c r="F16" s="238"/>
+      <c r="G16" s="238"/>
+      <c r="H16" s="238"/>
+      <c r="I16" s="239"/>
     </row>
     <row r="17" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="158" t="s">
@@ -5215,10 +5215,10 @@
         <v>281</v>
       </c>
       <c r="C17" s="90"/>
-      <c r="E17" s="249" t="s">
+      <c r="E17" s="240" t="s">
         <v>235</v>
       </c>
-      <c r="F17" s="250"/>
+      <c r="F17" s="241"/>
       <c r="G17" s="83" t="s">
         <v>159</v>
       </c>
@@ -5248,7 +5248,7 @@
       <c r="H18" s="33" t="s">
         <v>161</v>
       </c>
-      <c r="I18" s="234" t="s">
+      <c r="I18" s="216" t="s">
         <v>474</v>
       </c>
       <c r="J18" s="81"/>
@@ -5271,7 +5271,7 @@
       <c r="H19" s="74" t="s">
         <v>196</v>
       </c>
-      <c r="I19" s="234"/>
+      <c r="I19" s="216"/>
       <c r="J19" s="81"/>
     </row>
     <row r="20" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5288,7 +5288,7 @@
       </c>
       <c r="G20" s="71"/>
       <c r="H20" s="71"/>
-      <c r="I20" s="235"/>
+      <c r="I20" s="217"/>
       <c r="J20" s="81"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -5310,24 +5310,24 @@
       <c r="A23" s="162"/>
       <c r="B23" s="93"/>
       <c r="C23" s="92"/>
-      <c r="E23" s="214" t="s">
+      <c r="E23" s="218" t="s">
         <v>198</v>
       </c>
-      <c r="F23" s="236"/>
-      <c r="G23" s="236"/>
-      <c r="H23" s="236"/>
-      <c r="I23" s="215"/>
+      <c r="F23" s="219"/>
+      <c r="G23" s="219"/>
+      <c r="H23" s="219"/>
+      <c r="I23" s="220"/>
     </row>
     <row r="24" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="214" t="s">
+      <c r="A24" s="218" t="s">
         <v>240</v>
       </c>
-      <c r="B24" s="215"/>
+      <c r="B24" s="220"/>
       <c r="C24" s="32"/>
-      <c r="E24" s="254" t="s">
+      <c r="E24" s="224" t="s">
         <v>235</v>
       </c>
-      <c r="F24" s="255"/>
+      <c r="F24" s="225"/>
       <c r="G24" s="82" t="s">
         <v>159</v>
       </c>
@@ -5356,7 +5356,7 @@
       <c r="H25" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="I25" s="251" t="s">
+      <c r="I25" s="221" t="s">
         <v>475</v>
       </c>
     </row>
@@ -5380,7 +5380,7 @@
       <c r="H26" s="74" t="s">
         <v>201</v>
       </c>
-      <c r="I26" s="252"/>
+      <c r="I26" s="222"/>
     </row>
     <row r="27" spans="1:10" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="160" t="s">
@@ -5396,7 +5396,7 @@
       </c>
       <c r="G27" s="71"/>
       <c r="H27" s="71"/>
-      <c r="I27" s="253"/>
+      <c r="I27" s="223"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="160" t="s">
@@ -5420,22 +5420,22 @@
       <c r="A30" s="161"/>
       <c r="B30" s="118"/>
       <c r="C30" s="90"/>
-      <c r="E30" s="214" t="s">
+      <c r="E30" s="218" t="s">
         <v>199</v>
       </c>
-      <c r="F30" s="236"/>
-      <c r="G30" s="236"/>
-      <c r="H30" s="236"/>
-      <c r="I30" s="215"/>
+      <c r="F30" s="219"/>
+      <c r="G30" s="219"/>
+      <c r="H30" s="219"/>
+      <c r="I30" s="220"/>
     </row>
     <row r="31" spans="1:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="162"/>
       <c r="B31" s="92"/>
       <c r="C31" s="92"/>
-      <c r="E31" s="256" t="s">
+      <c r="E31" s="226" t="s">
         <v>472</v>
       </c>
-      <c r="F31" s="257"/>
+      <c r="F31" s="227"/>
       <c r="G31" s="212" t="s">
         <v>159</v>
       </c>
@@ -5447,10 +5447,10 @@
       </c>
     </row>
     <row r="32" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="214" t="s">
+      <c r="A32" s="218" t="s">
         <v>241</v>
       </c>
-      <c r="B32" s="215"/>
+      <c r="B32" s="220"/>
       <c r="C32" s="32"/>
       <c r="E32" s="84">
         <v>1</v>
@@ -5460,7 +5460,7 @@
       </c>
       <c r="G32" s="33"/>
       <c r="H32" s="74"/>
-      <c r="I32" s="234"/>
+      <c r="I32" s="216"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="158" t="s">
@@ -5480,7 +5480,7 @@
         <v>5</v>
       </c>
       <c r="H33" s="33"/>
-      <c r="I33" s="234"/>
+      <c r="I33" s="216"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="159" t="s">
@@ -5495,7 +5495,7 @@
       <c r="F34" s="94"/>
       <c r="G34" s="33"/>
       <c r="H34" s="74"/>
-      <c r="I34" s="234"/>
+      <c r="I34" s="216"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="160" t="s">
@@ -5508,7 +5508,7 @@
       <c r="F35" s="94"/>
       <c r="G35" s="33"/>
       <c r="H35" s="33"/>
-      <c r="I35" s="234"/>
+      <c r="I35" s="216"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="160" t="s">
@@ -5521,7 +5521,7 @@
       <c r="F36" s="94"/>
       <c r="G36" s="33"/>
       <c r="H36" s="33"/>
-      <c r="I36" s="234"/>
+      <c r="I36" s="216"/>
     </row>
     <row r="37" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="160" t="s">
@@ -5534,7 +5534,7 @@
       <c r="F37" s="141"/>
       <c r="G37" s="71"/>
       <c r="H37" s="71"/>
-      <c r="I37" s="235"/>
+      <c r="I37" s="217"/>
     </row>
     <row r="38" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="161" t="s">
@@ -5547,17 +5547,17 @@
       <c r="B39" s="122"/>
     </row>
     <row r="40" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="E40" s="214" t="s">
+      <c r="E40" s="218" t="s">
         <v>200</v>
       </c>
-      <c r="F40" s="236"/>
-      <c r="G40" s="236"/>
-      <c r="H40" s="236"/>
-      <c r="I40" s="215"/>
+      <c r="F40" s="219"/>
+      <c r="G40" s="219"/>
+      <c r="H40" s="219"/>
+      <c r="I40" s="220"/>
     </row>
     <row r="41" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="E41" s="254"/>
-      <c r="F41" s="255"/>
+      <c r="E41" s="224"/>
+      <c r="F41" s="225"/>
       <c r="G41" s="82" t="s">
         <v>159</v>
       </c>
@@ -5575,7 +5575,7 @@
       <c r="F42" s="94"/>
       <c r="G42" s="33"/>
       <c r="H42" s="74"/>
-      <c r="I42" s="234"/>
+      <c r="I42" s="216"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E43" s="84">
@@ -5584,7 +5584,7 @@
       <c r="F43" s="94"/>
       <c r="G43" s="33"/>
       <c r="H43" s="33"/>
-      <c r="I43" s="234"/>
+      <c r="I43" s="216"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E44" s="84">
@@ -5593,7 +5593,7 @@
       <c r="F44" s="94"/>
       <c r="G44" s="33"/>
       <c r="H44" s="74"/>
-      <c r="I44" s="234"/>
+      <c r="I44" s="216"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E45" s="84">
@@ -5602,7 +5602,7 @@
       <c r="F45" s="94"/>
       <c r="G45" s="33"/>
       <c r="H45" s="33"/>
-      <c r="I45" s="234"/>
+      <c r="I45" s="216"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E46" s="84">
@@ -5611,7 +5611,7 @@
       <c r="F46" s="94"/>
       <c r="G46" s="33"/>
       <c r="H46" s="33"/>
-      <c r="I46" s="234"/>
+      <c r="I46" s="216"/>
     </row>
     <row r="47" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E47" s="85">
@@ -5620,25 +5620,11 @@
       <c r="F47" s="141"/>
       <c r="G47" s="71"/>
       <c r="H47" s="71"/>
-      <c r="I47" s="235"/>
+      <c r="I47" s="217"/>
     </row>
     <row r="48" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="I42:I47"/>
-    <mergeCell ref="E40:I40"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="I25:I27"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A8:K8"/>
-    <mergeCell ref="A9:K9"/>
-    <mergeCell ref="E16:I16"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="A16:B16"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="A3:B3"/>
@@ -5654,6 +5640,20 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="I32:I37"/>
     <mergeCell ref="E30:I30"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A8:K8"/>
+    <mergeCell ref="A9:K9"/>
+    <mergeCell ref="E16:I16"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="I42:I47"/>
+    <mergeCell ref="E40:I40"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="I25:I27"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E31:F31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5693,32 +5693,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="260" t="s">
+      <c r="A1" s="262" t="s">
         <v>386</v>
       </c>
-      <c r="B1" s="261"/>
-      <c r="C1" s="261"/>
-      <c r="D1" s="261"/>
-      <c r="E1" s="261"/>
-      <c r="F1" s="261"/>
-      <c r="G1" s="261"/>
-      <c r="H1" s="261"/>
-      <c r="I1" s="261"/>
-      <c r="J1" s="262"/>
+      <c r="B1" s="263"/>
+      <c r="C1" s="263"/>
+      <c r="D1" s="263"/>
+      <c r="E1" s="263"/>
+      <c r="F1" s="263"/>
+      <c r="G1" s="263"/>
+      <c r="H1" s="263"/>
+      <c r="I1" s="263"/>
+      <c r="J1" s="264"/>
     </row>
     <row r="2" spans="1:15" s="1" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="263" t="s">
+      <c r="A2" s="265" t="s">
         <v>242</v>
       </c>
-      <c r="B2" s="264"/>
-      <c r="C2" s="264"/>
-      <c r="D2" s="264"/>
-      <c r="E2" s="264"/>
-      <c r="F2" s="264"/>
-      <c r="G2" s="264"/>
-      <c r="H2" s="264"/>
-      <c r="I2" s="264"/>
-      <c r="J2" s="265"/>
+      <c r="B2" s="266"/>
+      <c r="C2" s="266"/>
+      <c r="D2" s="266"/>
+      <c r="E2" s="266"/>
+      <c r="F2" s="266"/>
+      <c r="G2" s="266"/>
+      <c r="H2" s="266"/>
+      <c r="I2" s="266"/>
+      <c r="J2" s="267"/>
       <c r="K2" s="79"/>
       <c r="L2" s="79"/>
       <c r="M2" s="75"/>
@@ -5732,13 +5732,13 @@
       <c r="B3" s="182" t="s">
         <v>322</v>
       </c>
-      <c r="C3" s="266" t="s">
+      <c r="C3" s="268" t="s">
         <v>293</v>
       </c>
-      <c r="D3" s="267"/>
-      <c r="E3" s="267"/>
-      <c r="F3" s="267"/>
-      <c r="G3" s="268"/>
+      <c r="D3" s="269"/>
+      <c r="E3" s="269"/>
+      <c r="F3" s="269"/>
+      <c r="G3" s="270"/>
       <c r="H3" s="182" t="s">
         <v>323</v>
       </c>
@@ -6363,25 +6363,25 @@
     </row>
     <row r="26" spans="1:17" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:17" s="1" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="278" t="s">
+      <c r="A27" s="280" t="s">
         <v>243</v>
       </c>
-      <c r="B27" s="279"/>
-      <c r="C27" s="279"/>
-      <c r="D27" s="279"/>
-      <c r="E27" s="279"/>
-      <c r="F27" s="279"/>
-      <c r="G27" s="279"/>
-      <c r="H27" s="279"/>
-      <c r="I27" s="279"/>
-      <c r="J27" s="279"/>
-      <c r="K27" s="279"/>
-      <c r="L27" s="279"/>
-      <c r="M27" s="279"/>
-      <c r="N27" s="279"/>
-      <c r="O27" s="279"/>
-      <c r="P27" s="279"/>
-      <c r="Q27" s="280"/>
+      <c r="B27" s="281"/>
+      <c r="C27" s="281"/>
+      <c r="D27" s="281"/>
+      <c r="E27" s="281"/>
+      <c r="F27" s="281"/>
+      <c r="G27" s="281"/>
+      <c r="H27" s="281"/>
+      <c r="I27" s="281"/>
+      <c r="J27" s="281"/>
+      <c r="K27" s="281"/>
+      <c r="L27" s="281"/>
+      <c r="M27" s="281"/>
+      <c r="N27" s="281"/>
+      <c r="O27" s="281"/>
+      <c r="P27" s="281"/>
+      <c r="Q27" s="282"/>
     </row>
     <row r="28" spans="1:17" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="138" t="s">
@@ -6530,70 +6530,70 @@
     </row>
     <row r="31" spans="1:17" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:17" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A32" s="275" t="s">
+      <c r="A32" s="277" t="s">
         <v>283</v>
       </c>
-      <c r="B32" s="276"/>
-      <c r="C32" s="276"/>
-      <c r="D32" s="276"/>
-      <c r="E32" s="276"/>
-      <c r="F32" s="276"/>
-      <c r="G32" s="276"/>
-      <c r="H32" s="277"/>
+      <c r="B32" s="278"/>
+      <c r="C32" s="278"/>
+      <c r="D32" s="278"/>
+      <c r="E32" s="278"/>
+      <c r="F32" s="278"/>
+      <c r="G32" s="278"/>
+      <c r="H32" s="279"/>
     </row>
     <row r="33" spans="1:8" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="269" t="s">
+      <c r="A33" s="271" t="s">
         <v>368</v>
       </c>
-      <c r="B33" s="270"/>
-      <c r="C33" s="270"/>
-      <c r="D33" s="270"/>
-      <c r="E33" s="270"/>
-      <c r="F33" s="270"/>
-      <c r="G33" s="270"/>
-      <c r="H33" s="271"/>
+      <c r="B33" s="272"/>
+      <c r="C33" s="272"/>
+      <c r="D33" s="272"/>
+      <c r="E33" s="272"/>
+      <c r="F33" s="272"/>
+      <c r="G33" s="272"/>
+      <c r="H33" s="273"/>
     </row>
     <row r="34" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="269"/>
-      <c r="B34" s="270"/>
-      <c r="C34" s="270"/>
-      <c r="D34" s="270"/>
-      <c r="E34" s="270"/>
-      <c r="F34" s="270"/>
-      <c r="G34" s="270"/>
-      <c r="H34" s="271"/>
+      <c r="A34" s="271"/>
+      <c r="B34" s="272"/>
+      <c r="C34" s="272"/>
+      <c r="D34" s="272"/>
+      <c r="E34" s="272"/>
+      <c r="F34" s="272"/>
+      <c r="G34" s="272"/>
+      <c r="H34" s="273"/>
     </row>
     <row r="35" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="269"/>
-      <c r="B35" s="270"/>
-      <c r="C35" s="270"/>
-      <c r="D35" s="270"/>
-      <c r="E35" s="270"/>
-      <c r="F35" s="270"/>
-      <c r="G35" s="270"/>
-      <c r="H35" s="271"/>
+      <c r="A35" s="271"/>
+      <c r="B35" s="272"/>
+      <c r="C35" s="272"/>
+      <c r="D35" s="272"/>
+      <c r="E35" s="272"/>
+      <c r="F35" s="272"/>
+      <c r="G35" s="272"/>
+      <c r="H35" s="273"/>
     </row>
     <row r="36" spans="1:8" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="272"/>
-      <c r="B36" s="273"/>
-      <c r="C36" s="273"/>
-      <c r="D36" s="273"/>
-      <c r="E36" s="273"/>
-      <c r="F36" s="273"/>
-      <c r="G36" s="273"/>
-      <c r="H36" s="274"/>
+      <c r="A36" s="274"/>
+      <c r="B36" s="275"/>
+      <c r="C36" s="275"/>
+      <c r="D36" s="275"/>
+      <c r="E36" s="275"/>
+      <c r="F36" s="275"/>
+      <c r="G36" s="275"/>
+      <c r="H36" s="276"/>
     </row>
     <row r="37" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="38" spans="1:8" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A38" s="259" t="s">
+      <c r="A38" s="261" t="s">
         <v>312</v>
       </c>
-      <c r="B38" s="259"/>
-      <c r="C38" s="259"/>
-      <c r="D38" s="259"/>
-      <c r="E38" s="259"/>
-      <c r="F38" s="259"/>
-      <c r="G38" s="259"/>
+      <c r="B38" s="261"/>
+      <c r="C38" s="261"/>
+      <c r="D38" s="261"/>
+      <c r="E38" s="261"/>
+      <c r="F38" s="261"/>
+      <c r="G38" s="261"/>
     </row>
     <row r="39" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="78" t="s">
@@ -6605,12 +6605,12 @@
       <c r="C39" s="78" t="s">
         <v>314</v>
       </c>
-      <c r="D39" s="258" t="s">
+      <c r="D39" s="260" t="s">
         <v>315</v>
       </c>
-      <c r="E39" s="258"/>
-      <c r="F39" s="258"/>
-      <c r="G39" s="258"/>
+      <c r="E39" s="260"/>
+      <c r="F39" s="260"/>
+      <c r="G39" s="260"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
@@ -7135,8 +7135,8 @@
   </sheetPr>
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7155,32 +7155,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="114" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="281" t="s">
+      <c r="A1" s="283" t="s">
         <v>387</v>
       </c>
-      <c r="B1" s="282"/>
-      <c r="C1" s="282"/>
-      <c r="D1" s="282"/>
-      <c r="E1" s="282"/>
-      <c r="F1" s="282"/>
-      <c r="G1" s="282"/>
-      <c r="H1" s="282"/>
-      <c r="I1" s="282"/>
-      <c r="J1" s="283"/>
+      <c r="B1" s="284"/>
+      <c r="C1" s="284"/>
+      <c r="D1" s="284"/>
+      <c r="E1" s="284"/>
+      <c r="F1" s="284"/>
+      <c r="G1" s="284"/>
+      <c r="H1" s="284"/>
+      <c r="I1" s="284"/>
+      <c r="J1" s="285"/>
     </row>
     <row r="2" spans="1:10" s="114" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="278" t="s">
+      <c r="A2" s="280" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="279"/>
-      <c r="C2" s="279"/>
-      <c r="D2" s="279"/>
-      <c r="E2" s="279"/>
-      <c r="F2" s="279"/>
-      <c r="G2" s="279"/>
-      <c r="H2" s="279"/>
-      <c r="I2" s="279"/>
-      <c r="J2" s="280"/>
+      <c r="B2" s="281"/>
+      <c r="C2" s="281"/>
+      <c r="D2" s="281"/>
+      <c r="E2" s="281"/>
+      <c r="F2" s="281"/>
+      <c r="G2" s="281"/>
+      <c r="H2" s="281"/>
+      <c r="I2" s="281"/>
+      <c r="J2" s="282"/>
     </row>
     <row r="3" spans="1:10" s="114" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="132" t="s">
@@ -7259,18 +7259,18 @@
       <c r="J5" s="170"/>
     </row>
     <row r="6" spans="1:10" s="114" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="278" t="s">
+      <c r="A6" s="280" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="279"/>
-      <c r="C6" s="279"/>
-      <c r="D6" s="279"/>
-      <c r="E6" s="279"/>
-      <c r="F6" s="279"/>
-      <c r="G6" s="279"/>
-      <c r="H6" s="279"/>
-      <c r="I6" s="279"/>
-      <c r="J6" s="280"/>
+      <c r="B6" s="281"/>
+      <c r="C6" s="281"/>
+      <c r="D6" s="281"/>
+      <c r="E6" s="281"/>
+      <c r="F6" s="281"/>
+      <c r="G6" s="281"/>
+      <c r="H6" s="281"/>
+      <c r="I6" s="281"/>
+      <c r="J6" s="282"/>
     </row>
     <row r="7" spans="1:10" s="114" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="125" t="s">
@@ -7321,18 +7321,18 @@
       <c r="J9" s="72"/>
     </row>
     <row r="10" spans="1:10" s="114" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="278" t="s">
+      <c r="A10" s="280" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="279"/>
-      <c r="C10" s="279"/>
-      <c r="D10" s="279"/>
-      <c r="E10" s="279"/>
-      <c r="F10" s="279"/>
-      <c r="G10" s="279"/>
-      <c r="H10" s="279"/>
-      <c r="I10" s="279"/>
-      <c r="J10" s="280"/>
+      <c r="B10" s="281"/>
+      <c r="C10" s="281"/>
+      <c r="D10" s="281"/>
+      <c r="E10" s="281"/>
+      <c r="F10" s="281"/>
+      <c r="G10" s="281"/>
+      <c r="H10" s="281"/>
+      <c r="I10" s="281"/>
+      <c r="J10" s="282"/>
     </row>
     <row r="11" spans="1:10" s="114" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="128"/>
@@ -7476,13 +7476,27 @@
       <c r="A16" s="107">
         <v>4</v>
       </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
+      <c r="B16" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="E16" s="4">
+        <v>488</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>175</v>
+      </c>
       <c r="I16" s="4"/>
       <c r="J16" s="5"/>
     </row>
@@ -7543,18 +7557,18 @@
       <c r="J20" s="9"/>
     </row>
     <row r="21" spans="1:10" s="114" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="278" t="s">
+      <c r="A21" s="280" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="279"/>
-      <c r="C21" s="279"/>
-      <c r="D21" s="279"/>
-      <c r="E21" s="279"/>
-      <c r="F21" s="279"/>
-      <c r="G21" s="279"/>
-      <c r="H21" s="279"/>
-      <c r="I21" s="279"/>
-      <c r="J21" s="280"/>
+      <c r="B21" s="281"/>
+      <c r="C21" s="281"/>
+      <c r="D21" s="281"/>
+      <c r="E21" s="281"/>
+      <c r="F21" s="281"/>
+      <c r="G21" s="281"/>
+      <c r="H21" s="281"/>
+      <c r="I21" s="281"/>
+      <c r="J21" s="282"/>
     </row>
     <row r="22" spans="1:10" s="114" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="132" t="s">
@@ -7617,18 +7631,18 @@
       <c r="J24" s="9"/>
     </row>
     <row r="25" spans="1:10" s="114" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="278" t="s">
+      <c r="A25" s="280" t="s">
         <v>153</v>
       </c>
-      <c r="B25" s="279"/>
-      <c r="C25" s="279"/>
-      <c r="D25" s="279"/>
-      <c r="E25" s="279"/>
-      <c r="F25" s="279"/>
-      <c r="G25" s="279"/>
-      <c r="H25" s="279"/>
-      <c r="I25" s="279"/>
-      <c r="J25" s="280"/>
+      <c r="B25" s="281"/>
+      <c r="C25" s="281"/>
+      <c r="D25" s="281"/>
+      <c r="E25" s="281"/>
+      <c r="F25" s="281"/>
+      <c r="G25" s="281"/>
+      <c r="H25" s="281"/>
+      <c r="I25" s="281"/>
+      <c r="J25" s="282"/>
     </row>
     <row r="26" spans="1:10" s="114" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="132" t="s">
@@ -7690,70 +7704,70 @@
     </row>
     <row r="29" spans="1:10" s="114" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:10" s="114" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="275" t="s">
+      <c r="A30" s="277" t="s">
         <v>283</v>
       </c>
-      <c r="B30" s="276"/>
-      <c r="C30" s="276"/>
-      <c r="D30" s="276"/>
-      <c r="E30" s="276"/>
-      <c r="F30" s="276"/>
-      <c r="G30" s="276"/>
-      <c r="H30" s="277"/>
+      <c r="B30" s="278"/>
+      <c r="C30" s="278"/>
+      <c r="D30" s="278"/>
+      <c r="E30" s="278"/>
+      <c r="F30" s="278"/>
+      <c r="G30" s="278"/>
+      <c r="H30" s="279"/>
     </row>
     <row r="31" spans="1:10" s="114" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="269" t="s">
+      <c r="A31" s="271" t="s">
         <v>367</v>
       </c>
-      <c r="B31" s="270"/>
-      <c r="C31" s="270"/>
-      <c r="D31" s="270"/>
-      <c r="E31" s="270"/>
-      <c r="F31" s="270"/>
-      <c r="G31" s="270"/>
-      <c r="H31" s="271"/>
+      <c r="B31" s="272"/>
+      <c r="C31" s="272"/>
+      <c r="D31" s="272"/>
+      <c r="E31" s="272"/>
+      <c r="F31" s="272"/>
+      <c r="G31" s="272"/>
+      <c r="H31" s="273"/>
     </row>
     <row r="32" spans="1:10" s="114" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="269"/>
-      <c r="B32" s="270"/>
-      <c r="C32" s="270"/>
-      <c r="D32" s="270"/>
-      <c r="E32" s="270"/>
-      <c r="F32" s="270"/>
-      <c r="G32" s="270"/>
-      <c r="H32" s="271"/>
+      <c r="A32" s="271"/>
+      <c r="B32" s="272"/>
+      <c r="C32" s="272"/>
+      <c r="D32" s="272"/>
+      <c r="E32" s="272"/>
+      <c r="F32" s="272"/>
+      <c r="G32" s="272"/>
+      <c r="H32" s="273"/>
     </row>
     <row r="33" spans="1:8" s="114" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="269"/>
-      <c r="B33" s="270"/>
-      <c r="C33" s="270"/>
-      <c r="D33" s="270"/>
-      <c r="E33" s="270"/>
-      <c r="F33" s="270"/>
-      <c r="G33" s="270"/>
-      <c r="H33" s="271"/>
+      <c r="A33" s="271"/>
+      <c r="B33" s="272"/>
+      <c r="C33" s="272"/>
+      <c r="D33" s="272"/>
+      <c r="E33" s="272"/>
+      <c r="F33" s="272"/>
+      <c r="G33" s="272"/>
+      <c r="H33" s="273"/>
     </row>
     <row r="34" spans="1:8" s="114" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="272"/>
-      <c r="B34" s="273"/>
-      <c r="C34" s="273"/>
-      <c r="D34" s="273"/>
-      <c r="E34" s="273"/>
-      <c r="F34" s="273"/>
-      <c r="G34" s="273"/>
-      <c r="H34" s="274"/>
+      <c r="A34" s="274"/>
+      <c r="B34" s="275"/>
+      <c r="C34" s="275"/>
+      <c r="D34" s="275"/>
+      <c r="E34" s="275"/>
+      <c r="F34" s="275"/>
+      <c r="G34" s="275"/>
+      <c r="H34" s="276"/>
     </row>
     <row r="35" spans="1:8" s="114" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:8" s="114" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A36" s="259" t="s">
+      <c r="A36" s="261" t="s">
         <v>312</v>
       </c>
-      <c r="B36" s="259"/>
-      <c r="C36" s="259"/>
-      <c r="D36" s="259"/>
-      <c r="E36" s="259"/>
-      <c r="F36" s="259"/>
-      <c r="G36" s="259"/>
+      <c r="B36" s="261"/>
+      <c r="C36" s="261"/>
+      <c r="D36" s="261"/>
+      <c r="E36" s="261"/>
+      <c r="F36" s="261"/>
+      <c r="G36" s="261"/>
     </row>
     <row r="37" spans="1:8" s="114" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="78" t="s">
@@ -7765,12 +7779,12 @@
       <c r="C37" s="78" t="s">
         <v>314</v>
       </c>
-      <c r="D37" s="258" t="s">
+      <c r="D37" s="260" t="s">
         <v>315</v>
       </c>
-      <c r="E37" s="258"/>
-      <c r="F37" s="258"/>
-      <c r="G37" s="258"/>
+      <c r="E37" s="260"/>
+      <c r="F37" s="260"/>
+      <c r="G37" s="260"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -8007,23 +8021,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="285" t="s">
+      <c r="A1" s="292" t="s">
         <v>244</v>
       </c>
-      <c r="B1" s="285"/>
-      <c r="C1" s="285"/>
-      <c r="D1" s="285"/>
-      <c r="E1" s="285"/>
-      <c r="F1" s="285"/>
-      <c r="G1" s="285"/>
-      <c r="H1" s="285"/>
-      <c r="I1" s="285"/>
-      <c r="J1" s="285"/>
-      <c r="K1" s="285"/>
-      <c r="L1" s="285"/>
-      <c r="M1" s="285"/>
-      <c r="N1" s="285"/>
-      <c r="O1" s="285"/>
+      <c r="B1" s="292"/>
+      <c r="C1" s="292"/>
+      <c r="D1" s="292"/>
+      <c r="E1" s="292"/>
+      <c r="F1" s="292"/>
+      <c r="G1" s="292"/>
+      <c r="H1" s="292"/>
+      <c r="I1" s="292"/>
+      <c r="J1" s="292"/>
+      <c r="K1" s="292"/>
+      <c r="L1" s="292"/>
+      <c r="M1" s="292"/>
+      <c r="N1" s="292"/>
+      <c r="O1" s="292"/>
       <c r="P1" s="31"/>
       <c r="Q1" s="31"/>
     </row>
@@ -8031,26 +8045,26 @@
       <c r="A2" s="203" t="s">
         <v>360</v>
       </c>
-      <c r="B2" s="286" t="s">
+      <c r="B2" s="293" t="s">
         <v>282</v>
       </c>
-      <c r="C2" s="286"/>
-      <c r="D2" s="286"/>
-      <c r="E2" s="286"/>
-      <c r="F2" s="286"/>
-      <c r="G2" s="286" t="s">
+      <c r="C2" s="293"/>
+      <c r="D2" s="293"/>
+      <c r="E2" s="293"/>
+      <c r="F2" s="293"/>
+      <c r="G2" s="293" t="s">
         <v>248</v>
       </c>
-      <c r="H2" s="286"/>
-      <c r="I2" s="286"/>
-      <c r="J2" s="286"/>
-      <c r="K2" s="286"/>
-      <c r="L2" s="286"/>
-      <c r="M2" s="289" t="s">
+      <c r="H2" s="293"/>
+      <c r="I2" s="293"/>
+      <c r="J2" s="293"/>
+      <c r="K2" s="293"/>
+      <c r="L2" s="293"/>
+      <c r="M2" s="288" t="s">
         <v>299</v>
       </c>
-      <c r="N2" s="289"/>
-      <c r="O2" s="289"/>
+      <c r="N2" s="288"/>
+      <c r="O2" s="288"/>
       <c r="P2" s="89"/>
       <c r="Q2" s="89"/>
     </row>
@@ -8058,21 +8072,21 @@
       <c r="A3" s="202" t="s">
         <v>361</v>
       </c>
-      <c r="B3" s="288" t="s">
+      <c r="B3" s="294" t="s">
         <v>298</v>
       </c>
-      <c r="C3" s="288"/>
-      <c r="D3" s="288"/>
-      <c r="E3" s="288"/>
-      <c r="F3" s="288"/>
-      <c r="G3" s="288" t="s">
+      <c r="C3" s="294"/>
+      <c r="D3" s="294"/>
+      <c r="E3" s="294"/>
+      <c r="F3" s="294"/>
+      <c r="G3" s="294" t="s">
         <v>306</v>
       </c>
-      <c r="H3" s="288"/>
-      <c r="I3" s="288"/>
-      <c r="J3" s="288"/>
-      <c r="K3" s="288"/>
-      <c r="L3" s="288"/>
+      <c r="H3" s="294"/>
+      <c r="I3" s="294"/>
+      <c r="J3" s="294"/>
+      <c r="K3" s="294"/>
+      <c r="L3" s="294"/>
       <c r="M3" s="202" t="s">
         <v>304</v>
       </c>
@@ -8088,25 +8102,25 @@
       <c r="A4" s="205">
         <v>8</v>
       </c>
-      <c r="B4" s="287" t="s">
+      <c r="B4" s="286" t="s">
         <v>246</v>
       </c>
-      <c r="C4" s="287"/>
-      <c r="D4" s="287" t="s">
+      <c r="C4" s="286"/>
+      <c r="D4" s="286" t="s">
         <v>247</v>
       </c>
-      <c r="E4" s="287"/>
-      <c r="F4" s="287"/>
-      <c r="G4" s="287" t="s">
+      <c r="E4" s="286"/>
+      <c r="F4" s="286"/>
+      <c r="G4" s="286" t="s">
         <v>249</v>
       </c>
-      <c r="H4" s="287"/>
-      <c r="I4" s="287"/>
-      <c r="J4" s="287" t="s">
+      <c r="H4" s="286"/>
+      <c r="I4" s="286"/>
+      <c r="J4" s="286" t="s">
         <v>307</v>
       </c>
-      <c r="K4" s="287"/>
-      <c r="L4" s="287"/>
+      <c r="K4" s="286"/>
+      <c r="L4" s="286"/>
       <c r="M4" s="167" t="s">
         <v>154</v>
       </c>
@@ -8119,21 +8133,21 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="192"/>
-      <c r="B5" s="284"/>
-      <c r="C5" s="284"/>
-      <c r="D5" s="284"/>
-      <c r="E5" s="284"/>
-      <c r="F5" s="284"/>
-      <c r="G5" s="284" t="s">
+      <c r="B5" s="287"/>
+      <c r="C5" s="287"/>
+      <c r="D5" s="287"/>
+      <c r="E5" s="287"/>
+      <c r="F5" s="287"/>
+      <c r="G5" s="287" t="s">
         <v>281</v>
       </c>
-      <c r="H5" s="284"/>
-      <c r="I5" s="284"/>
-      <c r="J5" s="284" t="s">
+      <c r="H5" s="287"/>
+      <c r="I5" s="287"/>
+      <c r="J5" s="287" t="s">
         <v>295</v>
       </c>
-      <c r="K5" s="284"/>
-      <c r="L5" s="284"/>
+      <c r="K5" s="287"/>
+      <c r="L5" s="287"/>
       <c r="M5" s="201"/>
       <c r="N5" s="201" t="s">
         <v>391</v>
@@ -8144,23 +8158,23 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="192"/>
-      <c r="B6" s="284" t="s">
+      <c r="B6" s="287" t="s">
         <v>281</v>
       </c>
-      <c r="C6" s="284"/>
-      <c r="D6" s="284" t="s">
+      <c r="C6" s="287"/>
+      <c r="D6" s="287" t="s">
         <v>291</v>
       </c>
-      <c r="E6" s="284"/>
-      <c r="F6" s="284"/>
-      <c r="G6" s="284" t="s">
+      <c r="E6" s="287"/>
+      <c r="F6" s="287"/>
+      <c r="G6" s="287" t="s">
         <v>288</v>
       </c>
-      <c r="H6" s="284"/>
-      <c r="I6" s="284"/>
-      <c r="J6" s="284"/>
-      <c r="K6" s="284"/>
-      <c r="L6" s="284"/>
+      <c r="H6" s="287"/>
+      <c r="I6" s="287"/>
+      <c r="J6" s="287"/>
+      <c r="K6" s="287"/>
+      <c r="L6" s="287"/>
       <c r="M6" s="201"/>
       <c r="N6" s="201" t="s">
         <v>392</v>
@@ -8171,57 +8185,57 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="192"/>
-      <c r="B7" s="284" t="s">
+      <c r="B7" s="287" t="s">
         <v>281</v>
       </c>
-      <c r="C7" s="284"/>
-      <c r="D7" s="284" t="s">
+      <c r="C7" s="287"/>
+      <c r="D7" s="287" t="s">
         <v>292</v>
       </c>
-      <c r="E7" s="284"/>
-      <c r="F7" s="284"/>
-      <c r="G7" s="284"/>
-      <c r="H7" s="284"/>
-      <c r="I7" s="284"/>
-      <c r="J7" s="284"/>
-      <c r="K7" s="284"/>
-      <c r="L7" s="284"/>
+      <c r="E7" s="287"/>
+      <c r="F7" s="287"/>
+      <c r="G7" s="287"/>
+      <c r="H7" s="287"/>
+      <c r="I7" s="287"/>
+      <c r="J7" s="287"/>
+      <c r="K7" s="287"/>
+      <c r="L7" s="287"/>
       <c r="M7" s="201"/>
       <c r="N7" s="201"/>
       <c r="O7" s="165"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="192"/>
-      <c r="B8" s="284"/>
-      <c r="C8" s="284"/>
-      <c r="D8" s="284" t="s">
+      <c r="B8" s="287"/>
+      <c r="C8" s="287"/>
+      <c r="D8" s="287" t="s">
         <v>272</v>
       </c>
-      <c r="E8" s="284"/>
-      <c r="F8" s="284"/>
-      <c r="G8" s="284"/>
-      <c r="H8" s="284"/>
-      <c r="I8" s="284"/>
-      <c r="J8" s="284"/>
-      <c r="K8" s="284"/>
-      <c r="L8" s="284"/>
+      <c r="E8" s="287"/>
+      <c r="F8" s="287"/>
+      <c r="G8" s="287"/>
+      <c r="H8" s="287"/>
+      <c r="I8" s="287"/>
+      <c r="J8" s="287"/>
+      <c r="K8" s="287"/>
+      <c r="L8" s="287"/>
       <c r="M8" s="201"/>
       <c r="N8" s="201"/>
       <c r="O8" s="165"/>
     </row>
     <row r="9" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:17" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="290" t="s">
+      <c r="A10" s="289" t="s">
         <v>359</v>
       </c>
-      <c r="B10" s="291"/>
-      <c r="C10" s="291"/>
-      <c r="D10" s="291"/>
-      <c r="E10" s="291"/>
-      <c r="F10" s="291"/>
-      <c r="G10" s="291"/>
-      <c r="H10" s="291"/>
-      <c r="I10" s="292"/>
+      <c r="B10" s="290"/>
+      <c r="C10" s="290"/>
+      <c r="D10" s="290"/>
+      <c r="E10" s="290"/>
+      <c r="F10" s="290"/>
+      <c r="G10" s="290"/>
+      <c r="H10" s="290"/>
+      <c r="I10" s="291"/>
     </row>
     <row r="11" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="132" t="s">
@@ -8304,69 +8318,69 @@
     </row>
     <row r="14" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="275" t="s">
+      <c r="A15" s="277" t="s">
         <v>283</v>
       </c>
-      <c r="B15" s="276"/>
-      <c r="C15" s="276"/>
-      <c r="D15" s="276"/>
-      <c r="E15" s="276"/>
-      <c r="F15" s="276"/>
-      <c r="G15" s="276"/>
-      <c r="H15" s="277"/>
+      <c r="B15" s="278"/>
+      <c r="C15" s="278"/>
+      <c r="D15" s="278"/>
+      <c r="E15" s="278"/>
+      <c r="F15" s="278"/>
+      <c r="G15" s="278"/>
+      <c r="H15" s="279"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="269" t="s">
+      <c r="A16" s="271" t="s">
         <v>369</v>
       </c>
-      <c r="B16" s="270"/>
-      <c r="C16" s="270"/>
-      <c r="D16" s="270"/>
-      <c r="E16" s="270"/>
-      <c r="F16" s="270"/>
-      <c r="G16" s="270"/>
-      <c r="H16" s="271"/>
+      <c r="B16" s="272"/>
+      <c r="C16" s="272"/>
+      <c r="D16" s="272"/>
+      <c r="E16" s="272"/>
+      <c r="F16" s="272"/>
+      <c r="G16" s="272"/>
+      <c r="H16" s="273"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="269"/>
-      <c r="B17" s="270"/>
-      <c r="C17" s="270"/>
-      <c r="D17" s="270"/>
-      <c r="E17" s="270"/>
-      <c r="F17" s="270"/>
-      <c r="G17" s="270"/>
-      <c r="H17" s="271"/>
+      <c r="A17" s="271"/>
+      <c r="B17" s="272"/>
+      <c r="C17" s="272"/>
+      <c r="D17" s="272"/>
+      <c r="E17" s="272"/>
+      <c r="F17" s="272"/>
+      <c r="G17" s="272"/>
+      <c r="H17" s="273"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="269"/>
-      <c r="B18" s="270"/>
-      <c r="C18" s="270"/>
-      <c r="D18" s="270"/>
-      <c r="E18" s="270"/>
-      <c r="F18" s="270"/>
-      <c r="G18" s="270"/>
-      <c r="H18" s="271"/>
+      <c r="A18" s="271"/>
+      <c r="B18" s="272"/>
+      <c r="C18" s="272"/>
+      <c r="D18" s="272"/>
+      <c r="E18" s="272"/>
+      <c r="F18" s="272"/>
+      <c r="G18" s="272"/>
+      <c r="H18" s="273"/>
     </row>
     <row r="19" spans="1:8" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="272"/>
-      <c r="B19" s="273"/>
-      <c r="C19" s="273"/>
-      <c r="D19" s="273"/>
-      <c r="E19" s="273"/>
-      <c r="F19" s="273"/>
-      <c r="G19" s="273"/>
-      <c r="H19" s="274"/>
+      <c r="A19" s="274"/>
+      <c r="B19" s="275"/>
+      <c r="C19" s="275"/>
+      <c r="D19" s="275"/>
+      <c r="E19" s="275"/>
+      <c r="F19" s="275"/>
+      <c r="G19" s="275"/>
+      <c r="H19" s="276"/>
     </row>
     <row r="21" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A21" s="259" t="s">
+      <c r="A21" s="261" t="s">
         <v>312</v>
       </c>
-      <c r="B21" s="259"/>
-      <c r="C21" s="259"/>
-      <c r="D21" s="259"/>
-      <c r="E21" s="259"/>
-      <c r="F21" s="259"/>
-      <c r="G21" s="259"/>
+      <c r="B21" s="261"/>
+      <c r="C21" s="261"/>
+      <c r="D21" s="261"/>
+      <c r="E21" s="261"/>
+      <c r="F21" s="261"/>
+      <c r="G21" s="261"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="78" t="s">
@@ -8378,12 +8392,12 @@
       <c r="C22" s="78" t="s">
         <v>314</v>
       </c>
-      <c r="D22" s="258" t="s">
+      <c r="D22" s="260" t="s">
         <v>315</v>
       </c>
-      <c r="E22" s="258"/>
-      <c r="F22" s="258"/>
-      <c r="G22" s="258"/>
+      <c r="E22" s="260"/>
+      <c r="F22" s="260"/>
+      <c r="G22" s="260"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -8821,15 +8835,12 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="A16:H19"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G7:I7"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="G6:I6"/>
@@ -8846,12 +8857,15 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="G4:I4"/>
     <mergeCell ref="B2:F2"/>
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="A16:H19"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="B8:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8943,68 +8957,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="285" t="s">
+      <c r="A1" s="292" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="285"/>
-      <c r="C1" s="285"/>
-      <c r="D1" s="285"/>
-      <c r="E1" s="285"/>
-      <c r="F1" s="285"/>
-      <c r="G1" s="285"/>
-      <c r="H1" s="285"/>
-      <c r="I1" s="285"/>
-      <c r="J1" s="285"/>
-      <c r="K1" s="285"/>
-      <c r="L1" s="285"/>
-      <c r="M1" s="285"/>
-      <c r="N1" s="285"/>
-      <c r="O1" s="285"/>
-      <c r="P1" s="285"/>
+      <c r="B1" s="292"/>
+      <c r="C1" s="292"/>
+      <c r="D1" s="292"/>
+      <c r="E1" s="292"/>
+      <c r="F1" s="292"/>
+      <c r="G1" s="292"/>
+      <c r="H1" s="292"/>
+      <c r="I1" s="292"/>
+      <c r="J1" s="292"/>
+      <c r="K1" s="292"/>
+      <c r="L1" s="292"/>
+      <c r="M1" s="292"/>
+      <c r="N1" s="292"/>
+      <c r="O1" s="292"/>
+      <c r="P1" s="292"/>
       <c r="Q1" s="31"/>
     </row>
     <row r="2" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="286" t="s">
+      <c r="A2" s="293" t="s">
         <v>282</v>
       </c>
-      <c r="B2" s="286"/>
-      <c r="C2" s="286"/>
-      <c r="D2" s="286"/>
-      <c r="E2" s="286"/>
-      <c r="F2" s="286"/>
-      <c r="G2" s="286" t="s">
+      <c r="B2" s="293"/>
+      <c r="C2" s="293"/>
+      <c r="D2" s="293"/>
+      <c r="E2" s="293"/>
+      <c r="F2" s="293"/>
+      <c r="G2" s="293" t="s">
         <v>248</v>
       </c>
-      <c r="H2" s="286"/>
-      <c r="I2" s="286"/>
-      <c r="J2" s="286"/>
-      <c r="K2" s="286"/>
-      <c r="L2" s="286"/>
-      <c r="M2" s="289" t="s">
+      <c r="H2" s="293"/>
+      <c r="I2" s="293"/>
+      <c r="J2" s="293"/>
+      <c r="K2" s="293"/>
+      <c r="L2" s="293"/>
+      <c r="M2" s="288" t="s">
         <v>297</v>
       </c>
-      <c r="N2" s="289"/>
-      <c r="O2" s="289"/>
-      <c r="P2" s="289"/>
+      <c r="N2" s="288"/>
+      <c r="O2" s="288"/>
+      <c r="P2" s="288"/>
       <c r="Q2" s="89"/>
     </row>
     <row r="3" spans="1:17" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="288" t="s">
+      <c r="A3" s="294" t="s">
         <v>301</v>
       </c>
-      <c r="B3" s="288"/>
-      <c r="C3" s="288"/>
-      <c r="D3" s="288"/>
-      <c r="E3" s="288"/>
-      <c r="F3" s="288"/>
-      <c r="G3" s="288" t="s">
+      <c r="B3" s="294"/>
+      <c r="C3" s="294"/>
+      <c r="D3" s="294"/>
+      <c r="E3" s="294"/>
+      <c r="F3" s="294"/>
+      <c r="G3" s="294" t="s">
         <v>300</v>
       </c>
-      <c r="H3" s="288"/>
-      <c r="I3" s="288"/>
-      <c r="J3" s="288"/>
-      <c r="K3" s="288"/>
-      <c r="L3" s="288"/>
+      <c r="H3" s="294"/>
+      <c r="I3" s="294"/>
+      <c r="J3" s="294"/>
+      <c r="K3" s="294"/>
+      <c r="L3" s="294"/>
       <c r="M3" s="202" t="s">
         <v>303</v>
       </c>
@@ -9020,24 +9034,24 @@
       <c r="Q3" s="206"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="287" t="s">
+      <c r="A4" s="286" t="s">
         <v>246</v>
       </c>
-      <c r="B4" s="287"/>
-      <c r="C4" s="287"/>
-      <c r="D4" s="287" t="s">
+      <c r="B4" s="286"/>
+      <c r="C4" s="286"/>
+      <c r="D4" s="286" t="s">
         <v>247</v>
       </c>
-      <c r="E4" s="287"/>
-      <c r="F4" s="287"/>
-      <c r="G4" s="287" t="s">
+      <c r="E4" s="286"/>
+      <c r="F4" s="286"/>
+      <c r="G4" s="286" t="s">
         <v>250</v>
       </c>
-      <c r="H4" s="287"/>
-      <c r="I4" s="287"/>
-      <c r="J4" s="287"/>
-      <c r="K4" s="287"/>
-      <c r="L4" s="287"/>
+      <c r="H4" s="286"/>
+      <c r="I4" s="286"/>
+      <c r="J4" s="286"/>
+      <c r="K4" s="286"/>
+      <c r="L4" s="286"/>
       <c r="M4" s="167" t="s">
         <v>254</v>
       </c>
@@ -9052,20 +9066,20 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="284"/>
-      <c r="B5" s="284"/>
-      <c r="C5" s="284"/>
-      <c r="D5" s="284"/>
-      <c r="E5" s="284"/>
-      <c r="F5" s="284"/>
-      <c r="G5" s="293" t="s">
+      <c r="A5" s="287"/>
+      <c r="B5" s="287"/>
+      <c r="C5" s="287"/>
+      <c r="D5" s="287"/>
+      <c r="E5" s="287"/>
+      <c r="F5" s="287"/>
+      <c r="G5" s="295" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="293"/>
-      <c r="I5" s="293"/>
-      <c r="J5" s="293"/>
-      <c r="K5" s="293"/>
-      <c r="L5" s="293"/>
+      <c r="H5" s="295"/>
+      <c r="I5" s="295"/>
+      <c r="J5" s="295"/>
+      <c r="K5" s="295"/>
+      <c r="L5" s="295"/>
       <c r="M5" s="201" t="s">
         <v>294</v>
       </c>
@@ -9078,54 +9092,54 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="284"/>
-      <c r="B6" s="284"/>
-      <c r="C6" s="284"/>
-      <c r="D6" s="284"/>
-      <c r="E6" s="284"/>
-      <c r="F6" s="284"/>
-      <c r="G6" s="293"/>
-      <c r="H6" s="293"/>
-      <c r="I6" s="293"/>
-      <c r="J6" s="293"/>
-      <c r="K6" s="293"/>
-      <c r="L6" s="293"/>
+      <c r="A6" s="287"/>
+      <c r="B6" s="287"/>
+      <c r="C6" s="287"/>
+      <c r="D6" s="287"/>
+      <c r="E6" s="287"/>
+      <c r="F6" s="287"/>
+      <c r="G6" s="295"/>
+      <c r="H6" s="295"/>
+      <c r="I6" s="295"/>
+      <c r="J6" s="295"/>
+      <c r="K6" s="295"/>
+      <c r="L6" s="295"/>
       <c r="M6" s="201"/>
       <c r="N6" s="201"/>
       <c r="O6" s="201"/>
       <c r="P6" s="168"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="284"/>
-      <c r="B7" s="284"/>
-      <c r="C7" s="284"/>
-      <c r="D7" s="284"/>
-      <c r="E7" s="284"/>
-      <c r="F7" s="284"/>
-      <c r="G7" s="293"/>
-      <c r="H7" s="293"/>
-      <c r="I7" s="293"/>
-      <c r="J7" s="293"/>
-      <c r="K7" s="293"/>
-      <c r="L7" s="293"/>
+      <c r="A7" s="287"/>
+      <c r="B7" s="287"/>
+      <c r="C7" s="287"/>
+      <c r="D7" s="287"/>
+      <c r="E7" s="287"/>
+      <c r="F7" s="287"/>
+      <c r="G7" s="295"/>
+      <c r="H7" s="295"/>
+      <c r="I7" s="295"/>
+      <c r="J7" s="295"/>
+      <c r="K7" s="295"/>
+      <c r="L7" s="295"/>
       <c r="M7" s="201"/>
       <c r="N7" s="201"/>
       <c r="O7" s="201"/>
       <c r="P7" s="166"/>
     </row>
     <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="284"/>
-      <c r="B8" s="284"/>
-      <c r="C8" s="284"/>
-      <c r="D8" s="284"/>
-      <c r="E8" s="284"/>
-      <c r="F8" s="284"/>
-      <c r="G8" s="293"/>
-      <c r="H8" s="293"/>
-      <c r="I8" s="293"/>
-      <c r="J8" s="293"/>
-      <c r="K8" s="293"/>
-      <c r="L8" s="293"/>
+      <c r="A8" s="287"/>
+      <c r="B8" s="287"/>
+      <c r="C8" s="287"/>
+      <c r="D8" s="287"/>
+      <c r="E8" s="287"/>
+      <c r="F8" s="287"/>
+      <c r="G8" s="295"/>
+      <c r="H8" s="295"/>
+      <c r="I8" s="295"/>
+      <c r="J8" s="295"/>
+      <c r="K8" s="295"/>
+      <c r="L8" s="295"/>
       <c r="M8" s="201"/>
       <c r="N8" s="201"/>
       <c r="O8" s="201"/>
@@ -9133,17 +9147,17 @@
     </row>
     <row r="9" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:17" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="290" t="s">
+      <c r="A10" s="289" t="s">
         <v>358</v>
       </c>
-      <c r="B10" s="291"/>
-      <c r="C10" s="291"/>
-      <c r="D10" s="291"/>
-      <c r="E10" s="291"/>
-      <c r="F10" s="291"/>
-      <c r="G10" s="291"/>
-      <c r="H10" s="291"/>
-      <c r="I10" s="292"/>
+      <c r="B10" s="290"/>
+      <c r="C10" s="290"/>
+      <c r="D10" s="290"/>
+      <c r="E10" s="290"/>
+      <c r="F10" s="290"/>
+      <c r="G10" s="290"/>
+      <c r="H10" s="290"/>
+      <c r="I10" s="291"/>
     </row>
     <row r="11" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="132" t="s">
@@ -9225,69 +9239,69 @@
     </row>
     <row r="14" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="275" t="s">
+      <c r="A15" s="277" t="s">
         <v>283</v>
       </c>
-      <c r="B15" s="276"/>
-      <c r="C15" s="276"/>
-      <c r="D15" s="276"/>
-      <c r="E15" s="276"/>
-      <c r="F15" s="276"/>
-      <c r="G15" s="276"/>
-      <c r="H15" s="277"/>
+      <c r="B15" s="278"/>
+      <c r="C15" s="278"/>
+      <c r="D15" s="278"/>
+      <c r="E15" s="278"/>
+      <c r="F15" s="278"/>
+      <c r="G15" s="278"/>
+      <c r="H15" s="279"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="269" t="s">
+      <c r="A16" s="271" t="s">
         <v>370</v>
       </c>
-      <c r="B16" s="270"/>
-      <c r="C16" s="270"/>
-      <c r="D16" s="270"/>
-      <c r="E16" s="270"/>
-      <c r="F16" s="270"/>
-      <c r="G16" s="270"/>
-      <c r="H16" s="271"/>
+      <c r="B16" s="272"/>
+      <c r="C16" s="272"/>
+      <c r="D16" s="272"/>
+      <c r="E16" s="272"/>
+      <c r="F16" s="272"/>
+      <c r="G16" s="272"/>
+      <c r="H16" s="273"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="269"/>
-      <c r="B17" s="270"/>
-      <c r="C17" s="270"/>
-      <c r="D17" s="270"/>
-      <c r="E17" s="270"/>
-      <c r="F17" s="270"/>
-      <c r="G17" s="270"/>
-      <c r="H17" s="271"/>
+      <c r="A17" s="271"/>
+      <c r="B17" s="272"/>
+      <c r="C17" s="272"/>
+      <c r="D17" s="272"/>
+      <c r="E17" s="272"/>
+      <c r="F17" s="272"/>
+      <c r="G17" s="272"/>
+      <c r="H17" s="273"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="269"/>
-      <c r="B18" s="270"/>
-      <c r="C18" s="270"/>
-      <c r="D18" s="270"/>
-      <c r="E18" s="270"/>
-      <c r="F18" s="270"/>
-      <c r="G18" s="270"/>
-      <c r="H18" s="271"/>
+      <c r="A18" s="271"/>
+      <c r="B18" s="272"/>
+      <c r="C18" s="272"/>
+      <c r="D18" s="272"/>
+      <c r="E18" s="272"/>
+      <c r="F18" s="272"/>
+      <c r="G18" s="272"/>
+      <c r="H18" s="273"/>
     </row>
     <row r="19" spans="1:8" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="272"/>
-      <c r="B19" s="273"/>
-      <c r="C19" s="273"/>
-      <c r="D19" s="273"/>
-      <c r="E19" s="273"/>
-      <c r="F19" s="273"/>
-      <c r="G19" s="273"/>
-      <c r="H19" s="274"/>
+      <c r="A19" s="274"/>
+      <c r="B19" s="275"/>
+      <c r="C19" s="275"/>
+      <c r="D19" s="275"/>
+      <c r="E19" s="275"/>
+      <c r="F19" s="275"/>
+      <c r="G19" s="275"/>
+      <c r="H19" s="276"/>
     </row>
     <row r="21" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A21" s="259" t="s">
+      <c r="A21" s="261" t="s">
         <v>312</v>
       </c>
-      <c r="B21" s="259"/>
-      <c r="C21" s="259"/>
-      <c r="D21" s="259"/>
-      <c r="E21" s="259"/>
-      <c r="F21" s="259"/>
-      <c r="G21" s="259"/>
+      <c r="B21" s="261"/>
+      <c r="C21" s="261"/>
+      <c r="D21" s="261"/>
+      <c r="E21" s="261"/>
+      <c r="F21" s="261"/>
+      <c r="G21" s="261"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="78" t="s">
@@ -9299,12 +9313,12 @@
       <c r="C22" s="78" t="s">
         <v>314</v>
       </c>
-      <c r="D22" s="258" t="s">
+      <c r="D22" s="260" t="s">
         <v>315</v>
       </c>
-      <c r="E22" s="258"/>
-      <c r="F22" s="258"/>
-      <c r="G22" s="258"/>
+      <c r="E22" s="260"/>
+      <c r="F22" s="260"/>
+      <c r="G22" s="260"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -9476,16 +9490,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="G2:L2"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G5:L5"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="G3:L3"/>
     <mergeCell ref="A10:I10"/>
     <mergeCell ref="A21:G21"/>
     <mergeCell ref="D22:G22"/>
@@ -9502,6 +9506,16 @@
     <mergeCell ref="G7:L7"/>
     <mergeCell ref="G8:L8"/>
     <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G5:L5"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="G3:L3"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="G2:L2"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="A1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9567,7 +9581,7 @@
   </sheetPr>
   <dimension ref="A1:M66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -9583,12 +9597,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="294" t="s">
+      <c r="A1" s="296" t="s">
         <v>251</v>
       </c>
-      <c r="B1" s="295"/>
-      <c r="C1" s="295"/>
-      <c r="D1" s="296"/>
+      <c r="B1" s="297"/>
+      <c r="C1" s="297"/>
+      <c r="D1" s="298"/>
       <c r="E1" s="66"/>
       <c r="F1" s="66"/>
       <c r="G1" s="66"/>
@@ -9671,25 +9685,25 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="310" t="s">
+      <c r="A7" s="214" t="s">
         <v>476</v>
       </c>
       <c r="B7" s="16" t="s">
         <v>477</v>
       </c>
-      <c r="C7" s="311"/>
+      <c r="C7" s="215"/>
       <c r="D7" s="24">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="310" t="s">
+      <c r="A8" s="214" t="s">
         <v>478</v>
       </c>
       <c r="B8" s="16" t="s">
         <v>479</v>
       </c>
-      <c r="C8" s="311"/>
+      <c r="C8" s="215"/>
       <c r="D8" s="24">
         <v>1</v>
       </c>
@@ -10349,23 +10363,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="300" t="s">
+      <c r="A1" s="302" t="s">
         <v>222</v>
       </c>
-      <c r="B1" s="301"/>
-      <c r="C1" s="301"/>
-      <c r="D1" s="301"/>
-      <c r="E1" s="301"/>
-      <c r="F1" s="301"/>
-      <c r="G1" s="301"/>
-      <c r="H1" s="301"/>
-      <c r="I1" s="301"/>
-      <c r="J1" s="301"/>
-      <c r="K1" s="301"/>
-      <c r="L1" s="301"/>
-      <c r="M1" s="301"/>
-      <c r="N1" s="301"/>
-      <c r="O1" s="301"/>
+      <c r="B1" s="303"/>
+      <c r="C1" s="303"/>
+      <c r="D1" s="303"/>
+      <c r="E1" s="303"/>
+      <c r="F1" s="303"/>
+      <c r="G1" s="303"/>
+      <c r="H1" s="303"/>
+      <c r="I1" s="303"/>
+      <c r="J1" s="303"/>
+      <c r="K1" s="303"/>
+      <c r="L1" s="303"/>
+      <c r="M1" s="303"/>
+      <c r="N1" s="303"/>
+      <c r="O1" s="303"/>
     </row>
     <row r="2" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="34"/>
@@ -10383,17 +10397,17 @@
       <c r="M2" s="35"/>
     </row>
     <row r="3" spans="1:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="297" t="s">
+      <c r="B3" s="299" t="s">
         <v>223</v>
       </c>
-      <c r="C3" s="298"/>
-      <c r="D3" s="298"/>
-      <c r="E3" s="298"/>
-      <c r="F3" s="298"/>
-      <c r="G3" s="298"/>
-      <c r="H3" s="298"/>
-      <c r="I3" s="298"/>
-      <c r="J3" s="299"/>
+      <c r="C3" s="300"/>
+      <c r="D3" s="300"/>
+      <c r="E3" s="300"/>
+      <c r="F3" s="300"/>
+      <c r="G3" s="300"/>
+      <c r="H3" s="300"/>
+      <c r="I3" s="300"/>
+      <c r="J3" s="301"/>
     </row>
     <row r="4" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B4" s="37"/>
@@ -10584,21 +10598,21 @@
     </row>
     <row r="18" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="2:14" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B19" s="297" t="s">
+      <c r="B19" s="299" t="s">
         <v>223</v>
       </c>
-      <c r="C19" s="298"/>
-      <c r="D19" s="298"/>
-      <c r="E19" s="298"/>
-      <c r="F19" s="298"/>
-      <c r="G19" s="298"/>
-      <c r="H19" s="298"/>
-      <c r="I19" s="298"/>
-      <c r="J19" s="298"/>
-      <c r="K19" s="298"/>
-      <c r="L19" s="298"/>
-      <c r="M19" s="298"/>
-      <c r="N19" s="299"/>
+      <c r="C19" s="300"/>
+      <c r="D19" s="300"/>
+      <c r="E19" s="300"/>
+      <c r="F19" s="300"/>
+      <c r="G19" s="300"/>
+      <c r="H19" s="300"/>
+      <c r="I19" s="300"/>
+      <c r="J19" s="300"/>
+      <c r="K19" s="300"/>
+      <c r="L19" s="300"/>
+      <c r="M19" s="300"/>
+      <c r="N19" s="301"/>
     </row>
     <row r="20" spans="2:14" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B20" s="37"/>
@@ -10800,27 +10814,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="305" t="s">
+      <c r="A1" s="307" t="s">
         <v>233</v>
       </c>
-      <c r="B1" s="306"/>
-      <c r="C1" s="306"/>
-      <c r="D1" s="306"/>
-      <c r="E1" s="306"/>
-      <c r="F1" s="306"/>
-      <c r="G1" s="306"/>
-      <c r="H1" s="306"/>
-      <c r="I1" s="306"/>
-      <c r="J1" s="306"/>
-      <c r="K1" s="306"/>
-      <c r="L1" s="306"/>
-      <c r="M1" s="306"/>
-      <c r="N1" s="306"/>
-      <c r="O1" s="306"/>
-      <c r="P1" s="306"/>
-      <c r="Q1" s="306"/>
-      <c r="R1" s="306"/>
-      <c r="S1" s="306"/>
+      <c r="B1" s="308"/>
+      <c r="C1" s="308"/>
+      <c r="D1" s="308"/>
+      <c r="E1" s="308"/>
+      <c r="F1" s="308"/>
+      <c r="G1" s="308"/>
+      <c r="H1" s="308"/>
+      <c r="I1" s="308"/>
+      <c r="J1" s="308"/>
+      <c r="K1" s="308"/>
+      <c r="L1" s="308"/>
+      <c r="M1" s="308"/>
+      <c r="N1" s="308"/>
+      <c r="O1" s="308"/>
+      <c r="P1" s="308"/>
+      <c r="Q1" s="308"/>
+      <c r="R1" s="308"/>
+      <c r="S1" s="308"/>
     </row>
     <row r="2" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="35"/>
@@ -10834,26 +10848,26 @@
       <c r="I2" s="35"/>
     </row>
     <row r="3" spans="1:20" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="297" t="s">
+      <c r="B3" s="299" t="s">
         <v>223</v>
       </c>
-      <c r="C3" s="298"/>
-      <c r="D3" s="298"/>
-      <c r="E3" s="298"/>
-      <c r="F3" s="298"/>
-      <c r="G3" s="298"/>
-      <c r="H3" s="298"/>
-      <c r="I3" s="298"/>
-      <c r="J3" s="299"/>
-      <c r="L3" s="302" t="s">
+      <c r="C3" s="300"/>
+      <c r="D3" s="300"/>
+      <c r="E3" s="300"/>
+      <c r="F3" s="300"/>
+      <c r="G3" s="300"/>
+      <c r="H3" s="300"/>
+      <c r="I3" s="300"/>
+      <c r="J3" s="301"/>
+      <c r="L3" s="304" t="s">
         <v>223</v>
       </c>
-      <c r="M3" s="303"/>
-      <c r="N3" s="303"/>
-      <c r="O3" s="303"/>
-      <c r="P3" s="303"/>
-      <c r="Q3" s="303"/>
-      <c r="R3" s="304"/>
+      <c r="M3" s="305"/>
+      <c r="N3" s="305"/>
+      <c r="O3" s="305"/>
+      <c r="P3" s="305"/>
+      <c r="Q3" s="305"/>
+      <c r="R3" s="306"/>
       <c r="S3" s="36"/>
       <c r="T3" s="36"/>
     </row>
@@ -11084,23 +11098,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="307" t="s">
+      <c r="A1" s="309" t="s">
         <v>232</v>
       </c>
-      <c r="B1" s="308"/>
-      <c r="C1" s="308"/>
-      <c r="D1" s="308"/>
-      <c r="E1" s="308"/>
-      <c r="F1" s="308"/>
-      <c r="G1" s="308"/>
-      <c r="H1" s="308"/>
-      <c r="I1" s="308"/>
-      <c r="J1" s="308"/>
-      <c r="K1" s="308"/>
-      <c r="L1" s="308"/>
-      <c r="M1" s="308"/>
-      <c r="N1" s="308"/>
-      <c r="O1" s="309"/>
+      <c r="B1" s="310"/>
+      <c r="C1" s="310"/>
+      <c r="D1" s="310"/>
+      <c r="E1" s="310"/>
+      <c r="F1" s="310"/>
+      <c r="G1" s="310"/>
+      <c r="H1" s="310"/>
+      <c r="I1" s="310"/>
+      <c r="J1" s="310"/>
+      <c r="K1" s="310"/>
+      <c r="L1" s="310"/>
+      <c r="M1" s="310"/>
+      <c r="N1" s="310"/>
+      <c r="O1" s="311"/>
     </row>
     <row r="2" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="34"/>
@@ -11113,22 +11127,22 @@
       <c r="H2" s="52"/>
     </row>
     <row r="3" spans="1:16" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="297" t="s">
+      <c r="B3" s="299" t="s">
         <v>223</v>
       </c>
-      <c r="C3" s="298"/>
-      <c r="D3" s="298"/>
-      <c r="E3" s="298"/>
-      <c r="F3" s="298"/>
-      <c r="G3" s="298"/>
-      <c r="H3" s="299"/>
-      <c r="J3" s="302" t="s">
+      <c r="C3" s="300"/>
+      <c r="D3" s="300"/>
+      <c r="E3" s="300"/>
+      <c r="F3" s="300"/>
+      <c r="G3" s="300"/>
+      <c r="H3" s="301"/>
+      <c r="J3" s="304" t="s">
         <v>223</v>
       </c>
-      <c r="K3" s="303"/>
-      <c r="L3" s="303"/>
-      <c r="M3" s="303"/>
-      <c r="N3" s="304"/>
+      <c r="K3" s="305"/>
+      <c r="L3" s="305"/>
+      <c r="M3" s="305"/>
+      <c r="N3" s="306"/>
       <c r="O3" s="36"/>
       <c r="P3" s="36"/>
     </row>

</xml_diff>

<commit_message>
Improved TASBESession log in analyzeFromExcel
</commit_message>
<xml_diff>
--- a/test_templates/faulty_batch_template1.xlsx
+++ b/test_templates/faulty_batch_template1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-50385" yWindow="1080" windowWidth="47745" windowHeight="25665" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="-50385" yWindow="1080" windowWidth="47745" windowHeight="25665" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Experiment" sheetId="6" r:id="rId1"/>
@@ -3918,20 +3918,116 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3954,102 +4050,6 @@
     <xf numFmtId="49" fontId="16" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4128,12 +4128,21 @@
     <xf numFmtId="0" fontId="14" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4144,15 +4153,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="17" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5060,86 +5060,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="228" t="s">
+      <c r="A1" s="239" t="s">
         <v>385</v>
       </c>
-      <c r="B1" s="229"/>
-      <c r="C1" s="229"/>
-      <c r="D1" s="229"/>
-      <c r="E1" s="229"/>
-      <c r="F1" s="229"/>
-      <c r="G1" s="229"/>
-      <c r="H1" s="229"/>
-      <c r="I1" s="229"/>
-      <c r="J1" s="229"/>
-      <c r="K1" s="230"/>
+      <c r="B1" s="240"/>
+      <c r="C1" s="240"/>
+      <c r="D1" s="240"/>
+      <c r="E1" s="240"/>
+      <c r="F1" s="240"/>
+      <c r="G1" s="240"/>
+      <c r="H1" s="240"/>
+      <c r="I1" s="240"/>
+      <c r="J1" s="240"/>
+      <c r="K1" s="241"/>
     </row>
     <row r="2" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="87"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="244" t="s">
+      <c r="A3" s="218" t="s">
         <v>321</v>
       </c>
-      <c r="B3" s="245"/>
+      <c r="B3" s="219"/>
     </row>
     <row r="4" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="242" t="s">
+      <c r="A4" s="232" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="243"/>
+      <c r="B4" s="233"/>
     </row>
     <row r="5" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="258" t="s">
+      <c r="A5" s="234" t="s">
         <v>182</v>
       </c>
-      <c r="B5" s="259"/>
+      <c r="B5" s="235"/>
     </row>
     <row r="6" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="87"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="244" t="s">
+      <c r="A7" s="218" t="s">
         <v>276</v>
       </c>
-      <c r="B7" s="246"/>
-      <c r="C7" s="246"/>
-      <c r="D7" s="246"/>
-      <c r="E7" s="246"/>
-      <c r="F7" s="246"/>
-      <c r="G7" s="246"/>
-      <c r="H7" s="246"/>
-      <c r="I7" s="246"/>
-      <c r="J7" s="246"/>
-      <c r="K7" s="245"/>
+      <c r="B7" s="220"/>
+      <c r="C7" s="220"/>
+      <c r="D7" s="220"/>
+      <c r="E7" s="220"/>
+      <c r="F7" s="220"/>
+      <c r="G7" s="220"/>
+      <c r="H7" s="220"/>
+      <c r="I7" s="220"/>
+      <c r="J7" s="220"/>
+      <c r="K7" s="219"/>
     </row>
     <row r="8" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="231" t="s">
+      <c r="A8" s="242" t="s">
         <v>162</v>
       </c>
-      <c r="B8" s="232"/>
-      <c r="C8" s="232"/>
-      <c r="D8" s="232"/>
-      <c r="E8" s="232"/>
-      <c r="F8" s="232"/>
-      <c r="G8" s="232"/>
-      <c r="H8" s="232"/>
-      <c r="I8" s="232"/>
-      <c r="J8" s="232"/>
-      <c r="K8" s="233"/>
+      <c r="B8" s="243"/>
+      <c r="C8" s="243"/>
+      <c r="D8" s="243"/>
+      <c r="E8" s="243"/>
+      <c r="F8" s="243"/>
+      <c r="G8" s="243"/>
+      <c r="H8" s="243"/>
+      <c r="I8" s="243"/>
+      <c r="J8" s="243"/>
+      <c r="K8" s="244"/>
     </row>
     <row r="9" spans="1:11" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="234"/>
-      <c r="B9" s="235"/>
-      <c r="C9" s="235"/>
-      <c r="D9" s="235"/>
-      <c r="E9" s="235"/>
-      <c r="F9" s="235"/>
-      <c r="G9" s="235"/>
-      <c r="H9" s="235"/>
-      <c r="I9" s="235"/>
-      <c r="J9" s="235"/>
-      <c r="K9" s="236"/>
+      <c r="A9" s="245"/>
+      <c r="B9" s="246"/>
+      <c r="C9" s="246"/>
+      <c r="D9" s="246"/>
+      <c r="E9" s="246"/>
+      <c r="F9" s="246"/>
+      <c r="G9" s="246"/>
+      <c r="H9" s="246"/>
+      <c r="I9" s="246"/>
+      <c r="J9" s="246"/>
+      <c r="K9" s="247"/>
     </row>
     <row r="10" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="157"/>
@@ -5150,62 +5150,62 @@
       <c r="F10" s="143"/>
     </row>
     <row r="11" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="247" t="s">
+      <c r="A11" s="221" t="s">
         <v>277</v>
       </c>
-      <c r="B11" s="248"/>
-      <c r="C11" s="248"/>
-      <c r="D11" s="249"/>
+      <c r="B11" s="222"/>
+      <c r="C11" s="222"/>
+      <c r="D11" s="223"/>
       <c r="E11" s="88"/>
       <c r="F11" s="143"/>
     </row>
     <row r="12" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="250" t="s">
+      <c r="A12" s="224" t="s">
         <v>163</v>
       </c>
-      <c r="B12" s="251"/>
-      <c r="C12" s="252" t="s">
+      <c r="B12" s="225"/>
+      <c r="C12" s="226" t="s">
         <v>164</v>
       </c>
-      <c r="D12" s="253"/>
+      <c r="D12" s="227"/>
       <c r="E12" s="88"/>
       <c r="F12" s="143"/>
     </row>
     <row r="13" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="254"/>
-      <c r="B13" s="255"/>
-      <c r="C13" s="256"/>
-      <c r="D13" s="257"/>
+      <c r="A13" s="228"/>
+      <c r="B13" s="229"/>
+      <c r="C13" s="230"/>
+      <c r="D13" s="231"/>
       <c r="E13" s="88"/>
       <c r="F13" s="143"/>
     </row>
     <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:11" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="247" t="s">
+      <c r="A15" s="221" t="s">
         <v>278</v>
       </c>
-      <c r="B15" s="249"/>
-      <c r="E15" s="247" t="s">
+      <c r="B15" s="223"/>
+      <c r="E15" s="221" t="s">
         <v>320</v>
       </c>
-      <c r="F15" s="248"/>
-      <c r="G15" s="248"/>
-      <c r="H15" s="248"/>
-      <c r="I15" s="249"/>
+      <c r="F15" s="222"/>
+      <c r="G15" s="222"/>
+      <c r="H15" s="222"/>
+      <c r="I15" s="223"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="242" t="s">
+      <c r="A16" s="232" t="s">
         <v>236</v>
       </c>
-      <c r="B16" s="243"/>
+      <c r="B16" s="233"/>
       <c r="D16" s="89"/>
-      <c r="E16" s="237" t="s">
+      <c r="E16" s="248" t="s">
         <v>197</v>
       </c>
-      <c r="F16" s="238"/>
-      <c r="G16" s="238"/>
-      <c r="H16" s="238"/>
-      <c r="I16" s="239"/>
+      <c r="F16" s="249"/>
+      <c r="G16" s="249"/>
+      <c r="H16" s="249"/>
+      <c r="I16" s="250"/>
     </row>
     <row r="17" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="158" t="s">
@@ -5215,10 +5215,10 @@
         <v>281</v>
       </c>
       <c r="C17" s="90"/>
-      <c r="E17" s="240" t="s">
+      <c r="E17" s="251" t="s">
         <v>235</v>
       </c>
-      <c r="F17" s="241"/>
+      <c r="F17" s="252"/>
       <c r="G17" s="83" t="s">
         <v>159</v>
       </c>
@@ -5248,7 +5248,7 @@
       <c r="H18" s="33" t="s">
         <v>161</v>
       </c>
-      <c r="I18" s="216" t="s">
+      <c r="I18" s="236" t="s">
         <v>474</v>
       </c>
       <c r="J18" s="81"/>
@@ -5271,7 +5271,7 @@
       <c r="H19" s="74" t="s">
         <v>196</v>
       </c>
-      <c r="I19" s="216"/>
+      <c r="I19" s="236"/>
       <c r="J19" s="81"/>
     </row>
     <row r="20" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5288,7 +5288,7 @@
       </c>
       <c r="G20" s="71"/>
       <c r="H20" s="71"/>
-      <c r="I20" s="217"/>
+      <c r="I20" s="237"/>
       <c r="J20" s="81"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -5310,24 +5310,24 @@
       <c r="A23" s="162"/>
       <c r="B23" s="93"/>
       <c r="C23" s="92"/>
-      <c r="E23" s="218" t="s">
+      <c r="E23" s="216" t="s">
         <v>198</v>
       </c>
-      <c r="F23" s="219"/>
-      <c r="G23" s="219"/>
-      <c r="H23" s="219"/>
-      <c r="I23" s="220"/>
+      <c r="F23" s="238"/>
+      <c r="G23" s="238"/>
+      <c r="H23" s="238"/>
+      <c r="I23" s="217"/>
     </row>
     <row r="24" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="218" t="s">
+      <c r="A24" s="216" t="s">
         <v>240</v>
       </c>
-      <c r="B24" s="220"/>
+      <c r="B24" s="217"/>
       <c r="C24" s="32"/>
-      <c r="E24" s="224" t="s">
+      <c r="E24" s="256" t="s">
         <v>235</v>
       </c>
-      <c r="F24" s="225"/>
+      <c r="F24" s="257"/>
       <c r="G24" s="82" t="s">
         <v>159</v>
       </c>
@@ -5356,7 +5356,7 @@
       <c r="H25" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="I25" s="221" t="s">
+      <c r="I25" s="253" t="s">
         <v>475</v>
       </c>
     </row>
@@ -5380,7 +5380,7 @@
       <c r="H26" s="74" t="s">
         <v>201</v>
       </c>
-      <c r="I26" s="222"/>
+      <c r="I26" s="254"/>
     </row>
     <row r="27" spans="1:10" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="160" t="s">
@@ -5396,7 +5396,7 @@
       </c>
       <c r="G27" s="71"/>
       <c r="H27" s="71"/>
-      <c r="I27" s="223"/>
+      <c r="I27" s="255"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="160" t="s">
@@ -5420,22 +5420,22 @@
       <c r="A30" s="161"/>
       <c r="B30" s="118"/>
       <c r="C30" s="90"/>
-      <c r="E30" s="218" t="s">
+      <c r="E30" s="216" t="s">
         <v>199</v>
       </c>
-      <c r="F30" s="219"/>
-      <c r="G30" s="219"/>
-      <c r="H30" s="219"/>
-      <c r="I30" s="220"/>
+      <c r="F30" s="238"/>
+      <c r="G30" s="238"/>
+      <c r="H30" s="238"/>
+      <c r="I30" s="217"/>
     </row>
     <row r="31" spans="1:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="162"/>
       <c r="B31" s="92"/>
       <c r="C31" s="92"/>
-      <c r="E31" s="226" t="s">
+      <c r="E31" s="258" t="s">
         <v>472</v>
       </c>
-      <c r="F31" s="227"/>
+      <c r="F31" s="259"/>
       <c r="G31" s="212" t="s">
         <v>159</v>
       </c>
@@ -5447,10 +5447,10 @@
       </c>
     </row>
     <row r="32" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="218" t="s">
+      <c r="A32" s="216" t="s">
         <v>241</v>
       </c>
-      <c r="B32" s="220"/>
+      <c r="B32" s="217"/>
       <c r="C32" s="32"/>
       <c r="E32" s="84">
         <v>1</v>
@@ -5460,7 +5460,7 @@
       </c>
       <c r="G32" s="33"/>
       <c r="H32" s="74"/>
-      <c r="I32" s="216"/>
+      <c r="I32" s="236"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="158" t="s">
@@ -5480,7 +5480,7 @@
         <v>5</v>
       </c>
       <c r="H33" s="33"/>
-      <c r="I33" s="216"/>
+      <c r="I33" s="236"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="159" t="s">
@@ -5495,7 +5495,7 @@
       <c r="F34" s="94"/>
       <c r="G34" s="33"/>
       <c r="H34" s="74"/>
-      <c r="I34" s="216"/>
+      <c r="I34" s="236"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="160" t="s">
@@ -5508,7 +5508,7 @@
       <c r="F35" s="94"/>
       <c r="G35" s="33"/>
       <c r="H35" s="33"/>
-      <c r="I35" s="216"/>
+      <c r="I35" s="236"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="160" t="s">
@@ -5521,7 +5521,7 @@
       <c r="F36" s="94"/>
       <c r="G36" s="33"/>
       <c r="H36" s="33"/>
-      <c r="I36" s="216"/>
+      <c r="I36" s="236"/>
     </row>
     <row r="37" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="160" t="s">
@@ -5534,7 +5534,7 @@
       <c r="F37" s="141"/>
       <c r="G37" s="71"/>
       <c r="H37" s="71"/>
-      <c r="I37" s="217"/>
+      <c r="I37" s="237"/>
     </row>
     <row r="38" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="161" t="s">
@@ -5547,17 +5547,17 @@
       <c r="B39" s="122"/>
     </row>
     <row r="40" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="E40" s="218" t="s">
+      <c r="E40" s="216" t="s">
         <v>200</v>
       </c>
-      <c r="F40" s="219"/>
-      <c r="G40" s="219"/>
-      <c r="H40" s="219"/>
-      <c r="I40" s="220"/>
+      <c r="F40" s="238"/>
+      <c r="G40" s="238"/>
+      <c r="H40" s="238"/>
+      <c r="I40" s="217"/>
     </row>
     <row r="41" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="E41" s="224"/>
-      <c r="F41" s="225"/>
+      <c r="E41" s="256"/>
+      <c r="F41" s="257"/>
       <c r="G41" s="82" t="s">
         <v>159</v>
       </c>
@@ -5575,7 +5575,7 @@
       <c r="F42" s="94"/>
       <c r="G42" s="33"/>
       <c r="H42" s="74"/>
-      <c r="I42" s="216"/>
+      <c r="I42" s="236"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E43" s="84">
@@ -5584,7 +5584,7 @@
       <c r="F43" s="94"/>
       <c r="G43" s="33"/>
       <c r="H43" s="33"/>
-      <c r="I43" s="216"/>
+      <c r="I43" s="236"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E44" s="84">
@@ -5593,7 +5593,7 @@
       <c r="F44" s="94"/>
       <c r="G44" s="33"/>
       <c r="H44" s="74"/>
-      <c r="I44" s="216"/>
+      <c r="I44" s="236"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E45" s="84">
@@ -5602,7 +5602,7 @@
       <c r="F45" s="94"/>
       <c r="G45" s="33"/>
       <c r="H45" s="33"/>
-      <c r="I45" s="216"/>
+      <c r="I45" s="236"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E46" s="84">
@@ -5611,7 +5611,7 @@
       <c r="F46" s="94"/>
       <c r="G46" s="33"/>
       <c r="H46" s="33"/>
-      <c r="I46" s="216"/>
+      <c r="I46" s="236"/>
     </row>
     <row r="47" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E47" s="85">
@@ -5620,11 +5620,25 @@
       <c r="F47" s="141"/>
       <c r="G47" s="71"/>
       <c r="H47" s="71"/>
-      <c r="I47" s="217"/>
+      <c r="I47" s="237"/>
     </row>
     <row r="48" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="I42:I47"/>
+    <mergeCell ref="E40:I40"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="I25:I27"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A8:K8"/>
+    <mergeCell ref="A9:K9"/>
+    <mergeCell ref="E16:I16"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="A16:B16"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="A3:B3"/>
@@ -5640,20 +5654,6 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="I32:I37"/>
     <mergeCell ref="E30:I30"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A8:K8"/>
-    <mergeCell ref="A9:K9"/>
-    <mergeCell ref="E16:I16"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="I42:I47"/>
-    <mergeCell ref="E40:I40"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="I25:I27"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E31:F31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5667,8 +5667,8 @@
   </sheetPr>
   <dimension ref="A1:Q71"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7135,8 +7135,8 @@
   </sheetPr>
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView topLeftCell="A6" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8021,23 +8021,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="292" t="s">
+      <c r="A1" s="287" t="s">
         <v>244</v>
       </c>
-      <c r="B1" s="292"/>
-      <c r="C1" s="292"/>
-      <c r="D1" s="292"/>
-      <c r="E1" s="292"/>
-      <c r="F1" s="292"/>
-      <c r="G1" s="292"/>
-      <c r="H1" s="292"/>
-      <c r="I1" s="292"/>
-      <c r="J1" s="292"/>
-      <c r="K1" s="292"/>
-      <c r="L1" s="292"/>
-      <c r="M1" s="292"/>
-      <c r="N1" s="292"/>
-      <c r="O1" s="292"/>
+      <c r="B1" s="287"/>
+      <c r="C1" s="287"/>
+      <c r="D1" s="287"/>
+      <c r="E1" s="287"/>
+      <c r="F1" s="287"/>
+      <c r="G1" s="287"/>
+      <c r="H1" s="287"/>
+      <c r="I1" s="287"/>
+      <c r="J1" s="287"/>
+      <c r="K1" s="287"/>
+      <c r="L1" s="287"/>
+      <c r="M1" s="287"/>
+      <c r="N1" s="287"/>
+      <c r="O1" s="287"/>
       <c r="P1" s="31"/>
       <c r="Q1" s="31"/>
     </row>
@@ -8045,26 +8045,26 @@
       <c r="A2" s="203" t="s">
         <v>360</v>
       </c>
-      <c r="B2" s="293" t="s">
+      <c r="B2" s="288" t="s">
         <v>282</v>
       </c>
-      <c r="C2" s="293"/>
-      <c r="D2" s="293"/>
-      <c r="E2" s="293"/>
-      <c r="F2" s="293"/>
-      <c r="G2" s="293" t="s">
+      <c r="C2" s="288"/>
+      <c r="D2" s="288"/>
+      <c r="E2" s="288"/>
+      <c r="F2" s="288"/>
+      <c r="G2" s="288" t="s">
         <v>248</v>
       </c>
-      <c r="H2" s="293"/>
-      <c r="I2" s="293"/>
-      <c r="J2" s="293"/>
-      <c r="K2" s="293"/>
-      <c r="L2" s="293"/>
-      <c r="M2" s="288" t="s">
+      <c r="H2" s="288"/>
+      <c r="I2" s="288"/>
+      <c r="J2" s="288"/>
+      <c r="K2" s="288"/>
+      <c r="L2" s="288"/>
+      <c r="M2" s="291" t="s">
         <v>299</v>
       </c>
-      <c r="N2" s="288"/>
-      <c r="O2" s="288"/>
+      <c r="N2" s="291"/>
+      <c r="O2" s="291"/>
       <c r="P2" s="89"/>
       <c r="Q2" s="89"/>
     </row>
@@ -8072,21 +8072,21 @@
       <c r="A3" s="202" t="s">
         <v>361</v>
       </c>
-      <c r="B3" s="294" t="s">
+      <c r="B3" s="290" t="s">
         <v>298</v>
       </c>
-      <c r="C3" s="294"/>
-      <c r="D3" s="294"/>
-      <c r="E3" s="294"/>
-      <c r="F3" s="294"/>
-      <c r="G3" s="294" t="s">
+      <c r="C3" s="290"/>
+      <c r="D3" s="290"/>
+      <c r="E3" s="290"/>
+      <c r="F3" s="290"/>
+      <c r="G3" s="290" t="s">
         <v>306</v>
       </c>
-      <c r="H3" s="294"/>
-      <c r="I3" s="294"/>
-      <c r="J3" s="294"/>
-      <c r="K3" s="294"/>
-      <c r="L3" s="294"/>
+      <c r="H3" s="290"/>
+      <c r="I3" s="290"/>
+      <c r="J3" s="290"/>
+      <c r="K3" s="290"/>
+      <c r="L3" s="290"/>
       <c r="M3" s="202" t="s">
         <v>304</v>
       </c>
@@ -8102,25 +8102,25 @@
       <c r="A4" s="205">
         <v>8</v>
       </c>
-      <c r="B4" s="286" t="s">
+      <c r="B4" s="289" t="s">
         <v>246</v>
       </c>
-      <c r="C4" s="286"/>
-      <c r="D4" s="286" t="s">
+      <c r="C4" s="289"/>
+      <c r="D4" s="289" t="s">
         <v>247</v>
       </c>
-      <c r="E4" s="286"/>
-      <c r="F4" s="286"/>
-      <c r="G4" s="286" t="s">
+      <c r="E4" s="289"/>
+      <c r="F4" s="289"/>
+      <c r="G4" s="289" t="s">
         <v>249</v>
       </c>
-      <c r="H4" s="286"/>
-      <c r="I4" s="286"/>
-      <c r="J4" s="286" t="s">
+      <c r="H4" s="289"/>
+      <c r="I4" s="289"/>
+      <c r="J4" s="289" t="s">
         <v>307</v>
       </c>
-      <c r="K4" s="286"/>
-      <c r="L4" s="286"/>
+      <c r="K4" s="289"/>
+      <c r="L4" s="289"/>
       <c r="M4" s="167" t="s">
         <v>154</v>
       </c>
@@ -8133,21 +8133,21 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="192"/>
-      <c r="B5" s="287"/>
-      <c r="C5" s="287"/>
-      <c r="D5" s="287"/>
-      <c r="E5" s="287"/>
-      <c r="F5" s="287"/>
-      <c r="G5" s="287" t="s">
+      <c r="B5" s="286"/>
+      <c r="C5" s="286"/>
+      <c r="D5" s="286"/>
+      <c r="E5" s="286"/>
+      <c r="F5" s="286"/>
+      <c r="G5" s="286" t="s">
         <v>281</v>
       </c>
-      <c r="H5" s="287"/>
-      <c r="I5" s="287"/>
-      <c r="J5" s="287" t="s">
+      <c r="H5" s="286"/>
+      <c r="I5" s="286"/>
+      <c r="J5" s="286" t="s">
         <v>295</v>
       </c>
-      <c r="K5" s="287"/>
-      <c r="L5" s="287"/>
+      <c r="K5" s="286"/>
+      <c r="L5" s="286"/>
       <c r="M5" s="201"/>
       <c r="N5" s="201" t="s">
         <v>391</v>
@@ -8158,23 +8158,23 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="192"/>
-      <c r="B6" s="287" t="s">
+      <c r="B6" s="286" t="s">
         <v>281</v>
       </c>
-      <c r="C6" s="287"/>
-      <c r="D6" s="287" t="s">
+      <c r="C6" s="286"/>
+      <c r="D6" s="286" t="s">
         <v>291</v>
       </c>
-      <c r="E6" s="287"/>
-      <c r="F6" s="287"/>
-      <c r="G6" s="287" t="s">
+      <c r="E6" s="286"/>
+      <c r="F6" s="286"/>
+      <c r="G6" s="286" t="s">
         <v>288</v>
       </c>
-      <c r="H6" s="287"/>
-      <c r="I6" s="287"/>
-      <c r="J6" s="287"/>
-      <c r="K6" s="287"/>
-      <c r="L6" s="287"/>
+      <c r="H6" s="286"/>
+      <c r="I6" s="286"/>
+      <c r="J6" s="286"/>
+      <c r="K6" s="286"/>
+      <c r="L6" s="286"/>
       <c r="M6" s="201"/>
       <c r="N6" s="201" t="s">
         <v>392</v>
@@ -8185,57 +8185,57 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="192"/>
-      <c r="B7" s="287" t="s">
+      <c r="B7" s="286" t="s">
         <v>281</v>
       </c>
-      <c r="C7" s="287"/>
-      <c r="D7" s="287" t="s">
+      <c r="C7" s="286"/>
+      <c r="D7" s="286" t="s">
         <v>292</v>
       </c>
-      <c r="E7" s="287"/>
-      <c r="F7" s="287"/>
-      <c r="G7" s="287"/>
-      <c r="H7" s="287"/>
-      <c r="I7" s="287"/>
-      <c r="J7" s="287"/>
-      <c r="K7" s="287"/>
-      <c r="L7" s="287"/>
+      <c r="E7" s="286"/>
+      <c r="F7" s="286"/>
+      <c r="G7" s="286"/>
+      <c r="H7" s="286"/>
+      <c r="I7" s="286"/>
+      <c r="J7" s="286"/>
+      <c r="K7" s="286"/>
+      <c r="L7" s="286"/>
       <c r="M7" s="201"/>
       <c r="N7" s="201"/>
       <c r="O7" s="165"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="192"/>
-      <c r="B8" s="287"/>
-      <c r="C8" s="287"/>
-      <c r="D8" s="287" t="s">
+      <c r="B8" s="286"/>
+      <c r="C8" s="286"/>
+      <c r="D8" s="286" t="s">
         <v>272</v>
       </c>
-      <c r="E8" s="287"/>
-      <c r="F8" s="287"/>
-      <c r="G8" s="287"/>
-      <c r="H8" s="287"/>
-      <c r="I8" s="287"/>
-      <c r="J8" s="287"/>
-      <c r="K8" s="287"/>
-      <c r="L8" s="287"/>
+      <c r="E8" s="286"/>
+      <c r="F8" s="286"/>
+      <c r="G8" s="286"/>
+      <c r="H8" s="286"/>
+      <c r="I8" s="286"/>
+      <c r="J8" s="286"/>
+      <c r="K8" s="286"/>
+      <c r="L8" s="286"/>
       <c r="M8" s="201"/>
       <c r="N8" s="201"/>
       <c r="O8" s="165"/>
     </row>
     <row r="9" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:17" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="289" t="s">
+      <c r="A10" s="292" t="s">
         <v>359</v>
       </c>
-      <c r="B10" s="290"/>
-      <c r="C10" s="290"/>
-      <c r="D10" s="290"/>
-      <c r="E10" s="290"/>
-      <c r="F10" s="290"/>
-      <c r="G10" s="290"/>
-      <c r="H10" s="290"/>
-      <c r="I10" s="291"/>
+      <c r="B10" s="293"/>
+      <c r="C10" s="293"/>
+      <c r="D10" s="293"/>
+      <c r="E10" s="293"/>
+      <c r="F10" s="293"/>
+      <c r="G10" s="293"/>
+      <c r="H10" s="293"/>
+      <c r="I10" s="294"/>
     </row>
     <row r="11" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="132" t="s">
@@ -8835,12 +8835,15 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="A16:H19"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="B8:C8"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="G6:I6"/>
@@ -8857,15 +8860,12 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="G4:I4"/>
     <mergeCell ref="B2:F2"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="A16:H19"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G7:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8957,68 +8957,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="292" t="s">
+      <c r="A1" s="287" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="292"/>
-      <c r="C1" s="292"/>
-      <c r="D1" s="292"/>
-      <c r="E1" s="292"/>
-      <c r="F1" s="292"/>
-      <c r="G1" s="292"/>
-      <c r="H1" s="292"/>
-      <c r="I1" s="292"/>
-      <c r="J1" s="292"/>
-      <c r="K1" s="292"/>
-      <c r="L1" s="292"/>
-      <c r="M1" s="292"/>
-      <c r="N1" s="292"/>
-      <c r="O1" s="292"/>
-      <c r="P1" s="292"/>
+      <c r="B1" s="287"/>
+      <c r="C1" s="287"/>
+      <c r="D1" s="287"/>
+      <c r="E1" s="287"/>
+      <c r="F1" s="287"/>
+      <c r="G1" s="287"/>
+      <c r="H1" s="287"/>
+      <c r="I1" s="287"/>
+      <c r="J1" s="287"/>
+      <c r="K1" s="287"/>
+      <c r="L1" s="287"/>
+      <c r="M1" s="287"/>
+      <c r="N1" s="287"/>
+      <c r="O1" s="287"/>
+      <c r="P1" s="287"/>
       <c r="Q1" s="31"/>
     </row>
     <row r="2" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="293" t="s">
+      <c r="A2" s="288" t="s">
         <v>282</v>
       </c>
-      <c r="B2" s="293"/>
-      <c r="C2" s="293"/>
-      <c r="D2" s="293"/>
-      <c r="E2" s="293"/>
-      <c r="F2" s="293"/>
-      <c r="G2" s="293" t="s">
+      <c r="B2" s="288"/>
+      <c r="C2" s="288"/>
+      <c r="D2" s="288"/>
+      <c r="E2" s="288"/>
+      <c r="F2" s="288"/>
+      <c r="G2" s="288" t="s">
         <v>248</v>
       </c>
-      <c r="H2" s="293"/>
-      <c r="I2" s="293"/>
-      <c r="J2" s="293"/>
-      <c r="K2" s="293"/>
-      <c r="L2" s="293"/>
-      <c r="M2" s="288" t="s">
+      <c r="H2" s="288"/>
+      <c r="I2" s="288"/>
+      <c r="J2" s="288"/>
+      <c r="K2" s="288"/>
+      <c r="L2" s="288"/>
+      <c r="M2" s="291" t="s">
         <v>297</v>
       </c>
-      <c r="N2" s="288"/>
-      <c r="O2" s="288"/>
-      <c r="P2" s="288"/>
+      <c r="N2" s="291"/>
+      <c r="O2" s="291"/>
+      <c r="P2" s="291"/>
       <c r="Q2" s="89"/>
     </row>
     <row r="3" spans="1:17" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="294" t="s">
+      <c r="A3" s="290" t="s">
         <v>301</v>
       </c>
-      <c r="B3" s="294"/>
-      <c r="C3" s="294"/>
-      <c r="D3" s="294"/>
-      <c r="E3" s="294"/>
-      <c r="F3" s="294"/>
-      <c r="G3" s="294" t="s">
+      <c r="B3" s="290"/>
+      <c r="C3" s="290"/>
+      <c r="D3" s="290"/>
+      <c r="E3" s="290"/>
+      <c r="F3" s="290"/>
+      <c r="G3" s="290" t="s">
         <v>300</v>
       </c>
-      <c r="H3" s="294"/>
-      <c r="I3" s="294"/>
-      <c r="J3" s="294"/>
-      <c r="K3" s="294"/>
-      <c r="L3" s="294"/>
+      <c r="H3" s="290"/>
+      <c r="I3" s="290"/>
+      <c r="J3" s="290"/>
+      <c r="K3" s="290"/>
+      <c r="L3" s="290"/>
       <c r="M3" s="202" t="s">
         <v>303</v>
       </c>
@@ -9034,24 +9034,24 @@
       <c r="Q3" s="206"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="286" t="s">
+      <c r="A4" s="289" t="s">
         <v>246</v>
       </c>
-      <c r="B4" s="286"/>
-      <c r="C4" s="286"/>
-      <c r="D4" s="286" t="s">
+      <c r="B4" s="289"/>
+      <c r="C4" s="289"/>
+      <c r="D4" s="289" t="s">
         <v>247</v>
       </c>
-      <c r="E4" s="286"/>
-      <c r="F4" s="286"/>
-      <c r="G4" s="286" t="s">
+      <c r="E4" s="289"/>
+      <c r="F4" s="289"/>
+      <c r="G4" s="289" t="s">
         <v>250</v>
       </c>
-      <c r="H4" s="286"/>
-      <c r="I4" s="286"/>
-      <c r="J4" s="286"/>
-      <c r="K4" s="286"/>
-      <c r="L4" s="286"/>
+      <c r="H4" s="289"/>
+      <c r="I4" s="289"/>
+      <c r="J4" s="289"/>
+      <c r="K4" s="289"/>
+      <c r="L4" s="289"/>
       <c r="M4" s="167" t="s">
         <v>254</v>
       </c>
@@ -9066,12 +9066,12 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="287"/>
-      <c r="B5" s="287"/>
-      <c r="C5" s="287"/>
-      <c r="D5" s="287"/>
-      <c r="E5" s="287"/>
-      <c r="F5" s="287"/>
+      <c r="A5" s="286"/>
+      <c r="B5" s="286"/>
+      <c r="C5" s="286"/>
+      <c r="D5" s="286"/>
+      <c r="E5" s="286"/>
+      <c r="F5" s="286"/>
       <c r="G5" s="295" t="s">
         <v>4</v>
       </c>
@@ -9092,12 +9092,12 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="287"/>
-      <c r="B6" s="287"/>
-      <c r="C6" s="287"/>
-      <c r="D6" s="287"/>
-      <c r="E6" s="287"/>
-      <c r="F6" s="287"/>
+      <c r="A6" s="286"/>
+      <c r="B6" s="286"/>
+      <c r="C6" s="286"/>
+      <c r="D6" s="286"/>
+      <c r="E6" s="286"/>
+      <c r="F6" s="286"/>
       <c r="G6" s="295"/>
       <c r="H6" s="295"/>
       <c r="I6" s="295"/>
@@ -9110,12 +9110,12 @@
       <c r="P6" s="168"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="287"/>
-      <c r="B7" s="287"/>
-      <c r="C7" s="287"/>
-      <c r="D7" s="287"/>
-      <c r="E7" s="287"/>
-      <c r="F7" s="287"/>
+      <c r="A7" s="286"/>
+      <c r="B7" s="286"/>
+      <c r="C7" s="286"/>
+      <c r="D7" s="286"/>
+      <c r="E7" s="286"/>
+      <c r="F7" s="286"/>
       <c r="G7" s="295"/>
       <c r="H7" s="295"/>
       <c r="I7" s="295"/>
@@ -9128,12 +9128,12 @@
       <c r="P7" s="166"/>
     </row>
     <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="287"/>
-      <c r="B8" s="287"/>
-      <c r="C8" s="287"/>
-      <c r="D8" s="287"/>
-      <c r="E8" s="287"/>
-      <c r="F8" s="287"/>
+      <c r="A8" s="286"/>
+      <c r="B8" s="286"/>
+      <c r="C8" s="286"/>
+      <c r="D8" s="286"/>
+      <c r="E8" s="286"/>
+      <c r="F8" s="286"/>
       <c r="G8" s="295"/>
       <c r="H8" s="295"/>
       <c r="I8" s="295"/>
@@ -9147,17 +9147,17 @@
     </row>
     <row r="9" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:17" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="289" t="s">
+      <c r="A10" s="292" t="s">
         <v>358</v>
       </c>
-      <c r="B10" s="290"/>
-      <c r="C10" s="290"/>
-      <c r="D10" s="290"/>
-      <c r="E10" s="290"/>
-      <c r="F10" s="290"/>
-      <c r="G10" s="290"/>
-      <c r="H10" s="290"/>
-      <c r="I10" s="291"/>
+      <c r="B10" s="293"/>
+      <c r="C10" s="293"/>
+      <c r="D10" s="293"/>
+      <c r="E10" s="293"/>
+      <c r="F10" s="293"/>
+      <c r="G10" s="293"/>
+      <c r="H10" s="293"/>
+      <c r="I10" s="294"/>
     </row>
     <row r="11" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="132" t="s">
@@ -9490,6 +9490,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="G2:L2"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G5:L5"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="G3:L3"/>
     <mergeCell ref="A10:I10"/>
     <mergeCell ref="A21:G21"/>
     <mergeCell ref="D22:G22"/>
@@ -9506,16 +9516,6 @@
     <mergeCell ref="G7:L7"/>
     <mergeCell ref="G8:L8"/>
     <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G5:L5"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="G3:L3"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="G2:L2"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="A1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Created DataFile objects and updated tests
</commit_message>
<xml_diff>
--- a/test_templates/faulty_batch_template1.xlsx
+++ b/test_templates/faulty_batch_template1.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="527">
   <si>
     <t>blank plasmid</t>
   </si>
@@ -2506,12 +2506,6 @@
   </si>
   <si>
     <t>what type of pathname to write to point-cloud JSON header file. 0 stands for absolute, 1 stands for relative.</t>
-  </si>
-  <si>
-    <t>flow.defaultCSVReadHeader</t>
-  </si>
-  <si>
-    <t>what is absolute filename for the JSON header file needed to read in CSV files</t>
   </si>
   <si>
     <t>flow.smallFileWarning</t>
@@ -4212,20 +4206,145 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4247,102 +4366,6 @@
     </xf>
     <xf numFmtId="49" fontId="15" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4435,57 +4458,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -4498,6 +4470,57 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="16" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -4552,35 +4575,6 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4671,7 +4665,7 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="27432" bIns="27432" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
@@ -4737,7 +4731,7 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="27432" bIns="27432" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
@@ -4808,7 +4802,7 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="27432" bIns="27432" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
@@ -4879,7 +4873,7 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="27432" bIns="27432" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
@@ -4945,7 +4939,7 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="27432" bIns="27432" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
@@ -5016,7 +5010,7 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="27432" bIns="27432" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
@@ -5082,7 +5076,7 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="27432" bIns="27432" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
@@ -5433,86 +5427,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="252" t="s">
+      <c r="A1" s="271" t="s">
         <v>378</v>
       </c>
-      <c r="B1" s="253"/>
-      <c r="C1" s="253"/>
-      <c r="D1" s="253"/>
-      <c r="E1" s="253"/>
-      <c r="F1" s="253"/>
-      <c r="G1" s="253"/>
-      <c r="H1" s="253"/>
-      <c r="I1" s="253"/>
-      <c r="J1" s="253"/>
-      <c r="K1" s="254"/>
+      <c r="B1" s="272"/>
+      <c r="C1" s="272"/>
+      <c r="D1" s="272"/>
+      <c r="E1" s="272"/>
+      <c r="F1" s="272"/>
+      <c r="G1" s="272"/>
+      <c r="H1" s="272"/>
+      <c r="I1" s="272"/>
+      <c r="J1" s="272"/>
+      <c r="K1" s="273"/>
     </row>
     <row r="2" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="86"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="268" t="s">
+      <c r="A3" s="250" t="s">
         <v>316</v>
       </c>
-      <c r="B3" s="269"/>
+      <c r="B3" s="251"/>
     </row>
     <row r="4" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="266" t="s">
+      <c r="A4" s="264" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="267"/>
+      <c r="B4" s="265"/>
     </row>
     <row r="5" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="282" t="s">
+      <c r="A5" s="266" t="s">
         <v>182</v>
       </c>
-      <c r="B5" s="283"/>
+      <c r="B5" s="267"/>
     </row>
     <row r="6" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="86"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="268" t="s">
+      <c r="A7" s="250" t="s">
         <v>273</v>
       </c>
-      <c r="B7" s="270"/>
-      <c r="C7" s="270"/>
-      <c r="D7" s="270"/>
-      <c r="E7" s="270"/>
-      <c r="F7" s="270"/>
-      <c r="G7" s="270"/>
-      <c r="H7" s="270"/>
-      <c r="I7" s="270"/>
-      <c r="J7" s="270"/>
-      <c r="K7" s="269"/>
+      <c r="B7" s="252"/>
+      <c r="C7" s="252"/>
+      <c r="D7" s="252"/>
+      <c r="E7" s="252"/>
+      <c r="F7" s="252"/>
+      <c r="G7" s="252"/>
+      <c r="H7" s="252"/>
+      <c r="I7" s="252"/>
+      <c r="J7" s="252"/>
+      <c r="K7" s="251"/>
     </row>
     <row r="8" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="255" t="s">
+      <c r="A8" s="274" t="s">
         <v>162</v>
       </c>
-      <c r="B8" s="256"/>
-      <c r="C8" s="256"/>
-      <c r="D8" s="256"/>
-      <c r="E8" s="256"/>
-      <c r="F8" s="256"/>
-      <c r="G8" s="256"/>
-      <c r="H8" s="256"/>
-      <c r="I8" s="256"/>
-      <c r="J8" s="256"/>
-      <c r="K8" s="257"/>
+      <c r="B8" s="275"/>
+      <c r="C8" s="275"/>
+      <c r="D8" s="275"/>
+      <c r="E8" s="275"/>
+      <c r="F8" s="275"/>
+      <c r="G8" s="275"/>
+      <c r="H8" s="275"/>
+      <c r="I8" s="275"/>
+      <c r="J8" s="275"/>
+      <c r="K8" s="276"/>
     </row>
     <row r="9" spans="1:11" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="258"/>
-      <c r="B9" s="259"/>
-      <c r="C9" s="259"/>
-      <c r="D9" s="259"/>
-      <c r="E9" s="259"/>
-      <c r="F9" s="259"/>
-      <c r="G9" s="259"/>
-      <c r="H9" s="259"/>
-      <c r="I9" s="259"/>
-      <c r="J9" s="259"/>
-      <c r="K9" s="260"/>
+      <c r="A9" s="277"/>
+      <c r="B9" s="278"/>
+      <c r="C9" s="278"/>
+      <c r="D9" s="278"/>
+      <c r="E9" s="278"/>
+      <c r="F9" s="278"/>
+      <c r="G9" s="278"/>
+      <c r="H9" s="278"/>
+      <c r="I9" s="278"/>
+      <c r="J9" s="278"/>
+      <c r="K9" s="279"/>
     </row>
     <row r="10" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="155"/>
@@ -5523,62 +5517,62 @@
       <c r="F10" s="141"/>
     </row>
     <row r="11" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="271" t="s">
+      <c r="A11" s="253" t="s">
         <v>274</v>
       </c>
-      <c r="B11" s="272"/>
-      <c r="C11" s="272"/>
-      <c r="D11" s="273"/>
+      <c r="B11" s="254"/>
+      <c r="C11" s="254"/>
+      <c r="D11" s="255"/>
       <c r="E11" s="87"/>
       <c r="F11" s="141"/>
     </row>
     <row r="12" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="274" t="s">
+      <c r="A12" s="256" t="s">
         <v>163</v>
       </c>
-      <c r="B12" s="275"/>
-      <c r="C12" s="276" t="s">
+      <c r="B12" s="257"/>
+      <c r="C12" s="258" t="s">
         <v>164</v>
       </c>
-      <c r="D12" s="277"/>
+      <c r="D12" s="259"/>
       <c r="E12" s="87"/>
       <c r="F12" s="141"/>
     </row>
     <row r="13" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="278"/>
-      <c r="B13" s="279"/>
-      <c r="C13" s="280"/>
-      <c r="D13" s="281"/>
+      <c r="A13" s="260"/>
+      <c r="B13" s="261"/>
+      <c r="C13" s="262"/>
+      <c r="D13" s="263"/>
       <c r="E13" s="87"/>
       <c r="F13" s="141"/>
     </row>
     <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:11" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="271" t="s">
+      <c r="A15" s="253" t="s">
         <v>275</v>
       </c>
-      <c r="B15" s="273"/>
-      <c r="E15" s="271" t="s">
+      <c r="B15" s="255"/>
+      <c r="E15" s="253" t="s">
         <v>315</v>
       </c>
-      <c r="F15" s="272"/>
-      <c r="G15" s="272"/>
-      <c r="H15" s="272"/>
-      <c r="I15" s="273"/>
+      <c r="F15" s="254"/>
+      <c r="G15" s="254"/>
+      <c r="H15" s="254"/>
+      <c r="I15" s="255"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="266" t="s">
+      <c r="A16" s="264" t="s">
         <v>236</v>
       </c>
-      <c r="B16" s="267"/>
+      <c r="B16" s="265"/>
       <c r="D16" s="88"/>
-      <c r="E16" s="261" t="s">
+      <c r="E16" s="280" t="s">
         <v>197</v>
       </c>
-      <c r="F16" s="262"/>
-      <c r="G16" s="262"/>
-      <c r="H16" s="262"/>
-      <c r="I16" s="263"/>
+      <c r="F16" s="281"/>
+      <c r="G16" s="281"/>
+      <c r="H16" s="281"/>
+      <c r="I16" s="282"/>
     </row>
     <row r="17" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="156" t="s">
@@ -5588,10 +5582,10 @@
         <v>278</v>
       </c>
       <c r="C17" s="89"/>
-      <c r="E17" s="264" t="s">
+      <c r="E17" s="283" t="s">
         <v>235</v>
       </c>
-      <c r="F17" s="265"/>
+      <c r="F17" s="284"/>
       <c r="G17" s="82" t="s">
         <v>159</v>
       </c>
@@ -5621,7 +5615,7 @@
       <c r="H18" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="I18" s="240" t="s">
+      <c r="I18" s="268" t="s">
         <v>465</v>
       </c>
       <c r="J18" s="80"/>
@@ -5644,7 +5638,7 @@
       <c r="H19" s="73" t="s">
         <v>196</v>
       </c>
-      <c r="I19" s="240"/>
+      <c r="I19" s="268"/>
       <c r="J19" s="80"/>
     </row>
     <row r="20" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5661,7 +5655,7 @@
       </c>
       <c r="G20" s="70"/>
       <c r="H20" s="70"/>
-      <c r="I20" s="241"/>
+      <c r="I20" s="269"/>
       <c r="J20" s="80"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -5683,24 +5677,24 @@
       <c r="A23" s="160"/>
       <c r="B23" s="92"/>
       <c r="C23" s="91"/>
-      <c r="E23" s="242" t="s">
+      <c r="E23" s="248" t="s">
         <v>198</v>
       </c>
-      <c r="F23" s="243"/>
-      <c r="G23" s="243"/>
-      <c r="H23" s="243"/>
-      <c r="I23" s="244"/>
+      <c r="F23" s="270"/>
+      <c r="G23" s="270"/>
+      <c r="H23" s="270"/>
+      <c r="I23" s="249"/>
     </row>
     <row r="24" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="242" t="s">
+      <c r="A24" s="248" t="s">
         <v>240</v>
       </c>
-      <c r="B24" s="244"/>
+      <c r="B24" s="249"/>
       <c r="C24" s="31"/>
-      <c r="E24" s="248" t="s">
+      <c r="E24" s="288" t="s">
         <v>235</v>
       </c>
-      <c r="F24" s="249"/>
+      <c r="F24" s="289"/>
       <c r="G24" s="81" t="s">
         <v>159</v>
       </c>
@@ -5729,7 +5723,7 @@
       <c r="H25" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="I25" s="245" t="s">
+      <c r="I25" s="285" t="s">
         <v>466</v>
       </c>
     </row>
@@ -5753,7 +5747,7 @@
       <c r="H26" s="73" t="s">
         <v>201</v>
       </c>
-      <c r="I26" s="246"/>
+      <c r="I26" s="286"/>
     </row>
     <row r="27" spans="1:10" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="158" t="s">
@@ -5769,7 +5763,7 @@
       </c>
       <c r="G27" s="70"/>
       <c r="H27" s="70"/>
-      <c r="I27" s="247"/>
+      <c r="I27" s="287"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="158" t="s">
@@ -5793,22 +5787,22 @@
       <c r="A30" s="159"/>
       <c r="B30" s="116"/>
       <c r="C30" s="89"/>
-      <c r="E30" s="242" t="s">
+      <c r="E30" s="248" t="s">
         <v>199</v>
       </c>
-      <c r="F30" s="243"/>
-      <c r="G30" s="243"/>
-      <c r="H30" s="243"/>
-      <c r="I30" s="244"/>
+      <c r="F30" s="270"/>
+      <c r="G30" s="270"/>
+      <c r="H30" s="270"/>
+      <c r="I30" s="249"/>
     </row>
     <row r="31" spans="1:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="160"/>
       <c r="B31" s="91"/>
       <c r="C31" s="91"/>
-      <c r="E31" s="250" t="s">
+      <c r="E31" s="290" t="s">
         <v>463</v>
       </c>
-      <c r="F31" s="251"/>
+      <c r="F31" s="291"/>
       <c r="G31" s="198" t="s">
         <v>159</v>
       </c>
@@ -5820,10 +5814,10 @@
       </c>
     </row>
     <row r="32" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="242" t="s">
+      <c r="A32" s="248" t="s">
         <v>241</v>
       </c>
-      <c r="B32" s="244"/>
+      <c r="B32" s="249"/>
       <c r="C32" s="31"/>
       <c r="E32" s="83">
         <v>1</v>
@@ -5833,7 +5827,7 @@
       </c>
       <c r="G32" s="32"/>
       <c r="H32" s="73"/>
-      <c r="I32" s="240"/>
+      <c r="I32" s="268"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="156" t="s">
@@ -5853,7 +5847,7 @@
         <v>5</v>
       </c>
       <c r="H33" s="32"/>
-      <c r="I33" s="240"/>
+      <c r="I33" s="268"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="157" t="s">
@@ -5868,7 +5862,7 @@
       <c r="F34" s="93"/>
       <c r="G34" s="32"/>
       <c r="H34" s="73"/>
-      <c r="I34" s="240"/>
+      <c r="I34" s="268"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="158" t="s">
@@ -5881,7 +5875,7 @@
       <c r="F35" s="93"/>
       <c r="G35" s="32"/>
       <c r="H35" s="32"/>
-      <c r="I35" s="240"/>
+      <c r="I35" s="268"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="158" t="s">
@@ -5894,7 +5888,7 @@
       <c r="F36" s="93"/>
       <c r="G36" s="32"/>
       <c r="H36" s="32"/>
-      <c r="I36" s="240"/>
+      <c r="I36" s="268"/>
     </row>
     <row r="37" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="158" t="s">
@@ -5907,7 +5901,7 @@
       <c r="F37" s="139"/>
       <c r="G37" s="70"/>
       <c r="H37" s="70"/>
-      <c r="I37" s="241"/>
+      <c r="I37" s="269"/>
     </row>
     <row r="38" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="159" t="s">
@@ -5920,17 +5914,17 @@
       <c r="B39" s="120"/>
     </row>
     <row r="40" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="E40" s="242" t="s">
+      <c r="E40" s="248" t="s">
         <v>200</v>
       </c>
-      <c r="F40" s="243"/>
-      <c r="G40" s="243"/>
-      <c r="H40" s="243"/>
-      <c r="I40" s="244"/>
+      <c r="F40" s="270"/>
+      <c r="G40" s="270"/>
+      <c r="H40" s="270"/>
+      <c r="I40" s="249"/>
     </row>
     <row r="41" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="E41" s="248"/>
-      <c r="F41" s="249"/>
+      <c r="E41" s="288"/>
+      <c r="F41" s="289"/>
       <c r="G41" s="81" t="s">
         <v>159</v>
       </c>
@@ -5948,7 +5942,7 @@
       <c r="F42" s="93"/>
       <c r="G42" s="32"/>
       <c r="H42" s="73"/>
-      <c r="I42" s="240"/>
+      <c r="I42" s="268"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E43" s="83">
@@ -5957,7 +5951,7 @@
       <c r="F43" s="93"/>
       <c r="G43" s="32"/>
       <c r="H43" s="32"/>
-      <c r="I43" s="240"/>
+      <c r="I43" s="268"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E44" s="83">
@@ -5966,7 +5960,7 @@
       <c r="F44" s="93"/>
       <c r="G44" s="32"/>
       <c r="H44" s="73"/>
-      <c r="I44" s="240"/>
+      <c r="I44" s="268"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E45" s="83">
@@ -5975,7 +5969,7 @@
       <c r="F45" s="93"/>
       <c r="G45" s="32"/>
       <c r="H45" s="32"/>
-      <c r="I45" s="240"/>
+      <c r="I45" s="268"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E46" s="83">
@@ -5984,7 +5978,7 @@
       <c r="F46" s="93"/>
       <c r="G46" s="32"/>
       <c r="H46" s="32"/>
-      <c r="I46" s="240"/>
+      <c r="I46" s="268"/>
     </row>
     <row r="47" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E47" s="84">
@@ -5993,11 +5987,25 @@
       <c r="F47" s="139"/>
       <c r="G47" s="70"/>
       <c r="H47" s="70"/>
-      <c r="I47" s="241"/>
+      <c r="I47" s="269"/>
     </row>
     <row r="48" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="I42:I47"/>
+    <mergeCell ref="E40:I40"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="I25:I27"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A8:K8"/>
+    <mergeCell ref="A9:K9"/>
+    <mergeCell ref="E16:I16"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="A16:B16"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="A3:B3"/>
@@ -6013,20 +6021,6 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="I32:I37"/>
     <mergeCell ref="E30:I30"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A8:K8"/>
-    <mergeCell ref="A9:K9"/>
-    <mergeCell ref="E16:I16"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="I42:I47"/>
-    <mergeCell ref="E40:I40"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="I25:I27"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E31:F31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6066,32 +6060,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="286" t="s">
+      <c r="A1" s="294" t="s">
         <v>379</v>
       </c>
-      <c r="B1" s="287"/>
-      <c r="C1" s="287"/>
-      <c r="D1" s="287"/>
-      <c r="E1" s="287"/>
-      <c r="F1" s="287"/>
-      <c r="G1" s="287"/>
-      <c r="H1" s="287"/>
-      <c r="I1" s="287"/>
-      <c r="J1" s="288"/>
+      <c r="B1" s="295"/>
+      <c r="C1" s="295"/>
+      <c r="D1" s="295"/>
+      <c r="E1" s="295"/>
+      <c r="F1" s="295"/>
+      <c r="G1" s="295"/>
+      <c r="H1" s="295"/>
+      <c r="I1" s="295"/>
+      <c r="J1" s="296"/>
     </row>
     <row r="2" spans="1:15" s="1" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="289" t="s">
+      <c r="A2" s="297" t="s">
         <v>242</v>
       </c>
-      <c r="B2" s="290"/>
-      <c r="C2" s="290"/>
-      <c r="D2" s="290"/>
-      <c r="E2" s="290"/>
-      <c r="F2" s="290"/>
-      <c r="G2" s="290"/>
-      <c r="H2" s="290"/>
-      <c r="I2" s="290"/>
-      <c r="J2" s="291"/>
+      <c r="B2" s="298"/>
+      <c r="C2" s="298"/>
+      <c r="D2" s="298"/>
+      <c r="E2" s="298"/>
+      <c r="F2" s="298"/>
+      <c r="G2" s="298"/>
+      <c r="H2" s="298"/>
+      <c r="I2" s="298"/>
+      <c r="J2" s="299"/>
       <c r="K2" s="78"/>
       <c r="L2" s="78"/>
       <c r="M2" s="74"/>
@@ -6105,13 +6099,13 @@
       <c r="B3" s="176" t="s">
         <v>317</v>
       </c>
-      <c r="C3" s="292" t="s">
+      <c r="C3" s="300" t="s">
         <v>290</v>
       </c>
-      <c r="D3" s="293"/>
-      <c r="E3" s="293"/>
-      <c r="F3" s="293"/>
-      <c r="G3" s="294"/>
+      <c r="D3" s="301"/>
+      <c r="E3" s="301"/>
+      <c r="F3" s="301"/>
+      <c r="G3" s="302"/>
       <c r="H3" s="176" t="s">
         <v>318</v>
       </c>
@@ -6736,26 +6730,26 @@
     </row>
     <row r="26" spans="1:18" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:18" s="1" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="304" t="s">
+      <c r="A27" s="312" t="s">
         <v>243</v>
       </c>
-      <c r="B27" s="305"/>
-      <c r="C27" s="305"/>
-      <c r="D27" s="305"/>
-      <c r="E27" s="305"/>
-      <c r="F27" s="305"/>
-      <c r="G27" s="305"/>
-      <c r="H27" s="305"/>
-      <c r="I27" s="305"/>
-      <c r="J27" s="305"/>
-      <c r="K27" s="305"/>
-      <c r="L27" s="305"/>
-      <c r="M27" s="305"/>
-      <c r="N27" s="305"/>
-      <c r="O27" s="305"/>
-      <c r="P27" s="305"/>
-      <c r="Q27" s="305"/>
-      <c r="R27" s="306"/>
+      <c r="B27" s="313"/>
+      <c r="C27" s="313"/>
+      <c r="D27" s="313"/>
+      <c r="E27" s="313"/>
+      <c r="F27" s="313"/>
+      <c r="G27" s="313"/>
+      <c r="H27" s="313"/>
+      <c r="I27" s="313"/>
+      <c r="J27" s="313"/>
+      <c r="K27" s="313"/>
+      <c r="L27" s="313"/>
+      <c r="M27" s="313"/>
+      <c r="N27" s="313"/>
+      <c r="O27" s="313"/>
+      <c r="P27" s="313"/>
+      <c r="Q27" s="313"/>
+      <c r="R27" s="314"/>
     </row>
     <row r="28" spans="1:18" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="136" t="s">
@@ -6911,70 +6905,70 @@
     </row>
     <row r="31" spans="1:18" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:18" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A32" s="301" t="s">
+      <c r="A32" s="309" t="s">
         <v>280</v>
       </c>
-      <c r="B32" s="302"/>
-      <c r="C32" s="302"/>
-      <c r="D32" s="302"/>
-      <c r="E32" s="302"/>
-      <c r="F32" s="302"/>
-      <c r="G32" s="302"/>
-      <c r="H32" s="303"/>
+      <c r="B32" s="310"/>
+      <c r="C32" s="310"/>
+      <c r="D32" s="310"/>
+      <c r="E32" s="310"/>
+      <c r="F32" s="310"/>
+      <c r="G32" s="310"/>
+      <c r="H32" s="311"/>
     </row>
     <row r="33" spans="1:8" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="295" t="s">
+      <c r="A33" s="303" t="s">
         <v>361</v>
       </c>
-      <c r="B33" s="296"/>
-      <c r="C33" s="296"/>
-      <c r="D33" s="296"/>
-      <c r="E33" s="296"/>
-      <c r="F33" s="296"/>
-      <c r="G33" s="296"/>
-      <c r="H33" s="297"/>
+      <c r="B33" s="304"/>
+      <c r="C33" s="304"/>
+      <c r="D33" s="304"/>
+      <c r="E33" s="304"/>
+      <c r="F33" s="304"/>
+      <c r="G33" s="304"/>
+      <c r="H33" s="305"/>
     </row>
     <row r="34" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="295"/>
-      <c r="B34" s="296"/>
-      <c r="C34" s="296"/>
-      <c r="D34" s="296"/>
-      <c r="E34" s="296"/>
-      <c r="F34" s="296"/>
-      <c r="G34" s="296"/>
-      <c r="H34" s="297"/>
+      <c r="A34" s="303"/>
+      <c r="B34" s="304"/>
+      <c r="C34" s="304"/>
+      <c r="D34" s="304"/>
+      <c r="E34" s="304"/>
+      <c r="F34" s="304"/>
+      <c r="G34" s="304"/>
+      <c r="H34" s="305"/>
     </row>
     <row r="35" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="295"/>
-      <c r="B35" s="296"/>
-      <c r="C35" s="296"/>
-      <c r="D35" s="296"/>
-      <c r="E35" s="296"/>
-      <c r="F35" s="296"/>
-      <c r="G35" s="296"/>
-      <c r="H35" s="297"/>
+      <c r="A35" s="303"/>
+      <c r="B35" s="304"/>
+      <c r="C35" s="304"/>
+      <c r="D35" s="304"/>
+      <c r="E35" s="304"/>
+      <c r="F35" s="304"/>
+      <c r="G35" s="304"/>
+      <c r="H35" s="305"/>
     </row>
     <row r="36" spans="1:8" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="298"/>
-      <c r="B36" s="299"/>
-      <c r="C36" s="299"/>
-      <c r="D36" s="299"/>
-      <c r="E36" s="299"/>
-      <c r="F36" s="299"/>
-      <c r="G36" s="299"/>
-      <c r="H36" s="300"/>
+      <c r="A36" s="306"/>
+      <c r="B36" s="307"/>
+      <c r="C36" s="307"/>
+      <c r="D36" s="307"/>
+      <c r="E36" s="307"/>
+      <c r="F36" s="307"/>
+      <c r="G36" s="307"/>
+      <c r="H36" s="308"/>
     </row>
     <row r="37" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="38" spans="1:8" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A38" s="285" t="s">
+      <c r="A38" s="293" t="s">
         <v>307</v>
       </c>
-      <c r="B38" s="285"/>
-      <c r="C38" s="285"/>
-      <c r="D38" s="285"/>
-      <c r="E38" s="285"/>
-      <c r="F38" s="285"/>
-      <c r="G38" s="285"/>
+      <c r="B38" s="293"/>
+      <c r="C38" s="293"/>
+      <c r="D38" s="293"/>
+      <c r="E38" s="293"/>
+      <c r="F38" s="293"/>
+      <c r="G38" s="293"/>
     </row>
     <row r="39" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="77" t="s">
@@ -6986,12 +6980,12 @@
       <c r="C39" s="77" t="s">
         <v>309</v>
       </c>
-      <c r="D39" s="284" t="s">
+      <c r="D39" s="292" t="s">
         <v>310</v>
       </c>
-      <c r="E39" s="284"/>
-      <c r="F39" s="284"/>
-      <c r="G39" s="284"/>
+      <c r="E39" s="292"/>
+      <c r="F39" s="292"/>
+      <c r="G39" s="292"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
@@ -7536,32 +7530,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="112" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="307" t="s">
+      <c r="A1" s="315" t="s">
         <v>380</v>
       </c>
-      <c r="B1" s="308"/>
-      <c r="C1" s="308"/>
-      <c r="D1" s="308"/>
-      <c r="E1" s="308"/>
-      <c r="F1" s="308"/>
-      <c r="G1" s="308"/>
-      <c r="H1" s="308"/>
-      <c r="I1" s="308"/>
-      <c r="J1" s="309"/>
+      <c r="B1" s="316"/>
+      <c r="C1" s="316"/>
+      <c r="D1" s="316"/>
+      <c r="E1" s="316"/>
+      <c r="F1" s="316"/>
+      <c r="G1" s="316"/>
+      <c r="H1" s="316"/>
+      <c r="I1" s="316"/>
+      <c r="J1" s="317"/>
     </row>
     <row r="2" spans="1:10" s="112" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="304" t="s">
+      <c r="A2" s="312" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="305"/>
-      <c r="C2" s="305"/>
-      <c r="D2" s="305"/>
-      <c r="E2" s="305"/>
-      <c r="F2" s="305"/>
-      <c r="G2" s="305"/>
-      <c r="H2" s="305"/>
-      <c r="I2" s="305"/>
-      <c r="J2" s="306"/>
+      <c r="B2" s="313"/>
+      <c r="C2" s="313"/>
+      <c r="D2" s="313"/>
+      <c r="E2" s="313"/>
+      <c r="F2" s="313"/>
+      <c r="G2" s="313"/>
+      <c r="H2" s="313"/>
+      <c r="I2" s="313"/>
+      <c r="J2" s="314"/>
     </row>
     <row r="3" spans="1:10" s="112" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="130" t="s">
@@ -7640,18 +7634,18 @@
       <c r="J5" s="164"/>
     </row>
     <row r="6" spans="1:10" s="112" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="304" t="s">
+      <c r="A6" s="312" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="305"/>
-      <c r="C6" s="305"/>
-      <c r="D6" s="305"/>
-      <c r="E6" s="305"/>
-      <c r="F6" s="305"/>
-      <c r="G6" s="305"/>
-      <c r="H6" s="305"/>
-      <c r="I6" s="305"/>
-      <c r="J6" s="306"/>
+      <c r="B6" s="313"/>
+      <c r="C6" s="313"/>
+      <c r="D6" s="313"/>
+      <c r="E6" s="313"/>
+      <c r="F6" s="313"/>
+      <c r="G6" s="313"/>
+      <c r="H6" s="313"/>
+      <c r="I6" s="313"/>
+      <c r="J6" s="314"/>
     </row>
     <row r="7" spans="1:10" s="112" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="123" t="s">
@@ -7702,18 +7696,18 @@
       <c r="J9" s="71"/>
     </row>
     <row r="10" spans="1:10" s="112" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="304" t="s">
+      <c r="A10" s="312" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="305"/>
-      <c r="C10" s="305"/>
-      <c r="D10" s="305"/>
-      <c r="E10" s="305"/>
-      <c r="F10" s="305"/>
-      <c r="G10" s="305"/>
-      <c r="H10" s="305"/>
-      <c r="I10" s="305"/>
-      <c r="J10" s="306"/>
+      <c r="B10" s="313"/>
+      <c r="C10" s="313"/>
+      <c r="D10" s="313"/>
+      <c r="E10" s="313"/>
+      <c r="F10" s="313"/>
+      <c r="G10" s="313"/>
+      <c r="H10" s="313"/>
+      <c r="I10" s="313"/>
+      <c r="J10" s="314"/>
     </row>
     <row r="11" spans="1:10" s="112" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="126"/>
@@ -7882,18 +7876,18 @@
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:10" s="112" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="310" t="s">
+      <c r="A17" s="318" t="s">
         <v>482</v>
       </c>
-      <c r="B17" s="311"/>
-      <c r="C17" s="311"/>
-      <c r="D17" s="311"/>
-      <c r="E17" s="311"/>
-      <c r="F17" s="311"/>
-      <c r="G17" s="311"/>
-      <c r="H17" s="311"/>
-      <c r="I17" s="311"/>
-      <c r="J17" s="312"/>
+      <c r="B17" s="319"/>
+      <c r="C17" s="319"/>
+      <c r="D17" s="319"/>
+      <c r="E17" s="319"/>
+      <c r="F17" s="319"/>
+      <c r="G17" s="319"/>
+      <c r="H17" s="319"/>
+      <c r="I17" s="319"/>
+      <c r="J17" s="320"/>
     </row>
     <row r="18" spans="1:10" s="112" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="206"/>
@@ -7966,18 +7960,18 @@
       <c r="J21" s="220"/>
     </row>
     <row r="22" spans="1:10" s="112" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="304" t="s">
+      <c r="A22" s="312" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="305"/>
-      <c r="C22" s="305"/>
-      <c r="D22" s="305"/>
-      <c r="E22" s="305"/>
-      <c r="F22" s="305"/>
-      <c r="G22" s="305"/>
-      <c r="H22" s="305"/>
-      <c r="I22" s="305"/>
-      <c r="J22" s="306"/>
+      <c r="B22" s="313"/>
+      <c r="C22" s="313"/>
+      <c r="D22" s="313"/>
+      <c r="E22" s="313"/>
+      <c r="F22" s="313"/>
+      <c r="G22" s="313"/>
+      <c r="H22" s="313"/>
+      <c r="I22" s="313"/>
+      <c r="J22" s="314"/>
     </row>
     <row r="23" spans="1:10" s="112" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="130" t="s">
@@ -8040,18 +8034,18 @@
       <c r="J25" s="9"/>
     </row>
     <row r="26" spans="1:10" s="112" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="310" t="s">
+      <c r="A26" s="318" t="s">
         <v>486</v>
       </c>
-      <c r="B26" s="311"/>
-      <c r="C26" s="311"/>
-      <c r="D26" s="311"/>
-      <c r="E26" s="311"/>
-      <c r="F26" s="311"/>
-      <c r="G26" s="311"/>
-      <c r="H26" s="311"/>
-      <c r="I26" s="311"/>
-      <c r="J26" s="312"/>
+      <c r="B26" s="319"/>
+      <c r="C26" s="319"/>
+      <c r="D26" s="319"/>
+      <c r="E26" s="319"/>
+      <c r="F26" s="319"/>
+      <c r="G26" s="319"/>
+      <c r="H26" s="319"/>
+      <c r="I26" s="319"/>
+      <c r="J26" s="320"/>
     </row>
     <row r="27" spans="1:10" s="112" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="221" t="s">
@@ -8118,18 +8112,18 @@
       <c r="J29" s="235"/>
     </row>
     <row r="30" spans="1:10" s="112" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="304" t="s">
+      <c r="A30" s="312" t="s">
         <v>153</v>
       </c>
-      <c r="B30" s="305"/>
-      <c r="C30" s="305"/>
-      <c r="D30" s="305"/>
-      <c r="E30" s="305"/>
-      <c r="F30" s="305"/>
-      <c r="G30" s="305"/>
-      <c r="H30" s="305"/>
-      <c r="I30" s="305"/>
-      <c r="J30" s="306"/>
+      <c r="B30" s="313"/>
+      <c r="C30" s="313"/>
+      <c r="D30" s="313"/>
+      <c r="E30" s="313"/>
+      <c r="F30" s="313"/>
+      <c r="G30" s="313"/>
+      <c r="H30" s="313"/>
+      <c r="I30" s="313"/>
+      <c r="J30" s="314"/>
     </row>
     <row r="31" spans="1:10" s="112" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="130" t="s">
@@ -8191,58 +8185,58 @@
     </row>
     <row r="34" spans="1:10" s="112" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="35" spans="1:10" s="112" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="301" t="s">
+      <c r="A35" s="309" t="s">
         <v>280</v>
       </c>
-      <c r="B35" s="302"/>
-      <c r="C35" s="302"/>
-      <c r="D35" s="302"/>
-      <c r="E35" s="302"/>
-      <c r="F35" s="302"/>
-      <c r="G35" s="302"/>
-      <c r="H35" s="303"/>
+      <c r="B35" s="310"/>
+      <c r="C35" s="310"/>
+      <c r="D35" s="310"/>
+      <c r="E35" s="310"/>
+      <c r="F35" s="310"/>
+      <c r="G35" s="310"/>
+      <c r="H35" s="311"/>
     </row>
     <row r="36" spans="1:10" s="112" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="295" t="s">
+      <c r="A36" s="303" t="s">
         <v>360</v>
       </c>
-      <c r="B36" s="296"/>
-      <c r="C36" s="296"/>
-      <c r="D36" s="296"/>
-      <c r="E36" s="296"/>
-      <c r="F36" s="296"/>
-      <c r="G36" s="296"/>
-      <c r="H36" s="297"/>
+      <c r="B36" s="304"/>
+      <c r="C36" s="304"/>
+      <c r="D36" s="304"/>
+      <c r="E36" s="304"/>
+      <c r="F36" s="304"/>
+      <c r="G36" s="304"/>
+      <c r="H36" s="305"/>
     </row>
     <row r="37" spans="1:10" s="112" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="295"/>
-      <c r="B37" s="296"/>
-      <c r="C37" s="296"/>
-      <c r="D37" s="296"/>
-      <c r="E37" s="296"/>
-      <c r="F37" s="296"/>
-      <c r="G37" s="296"/>
-      <c r="H37" s="297"/>
+      <c r="A37" s="303"/>
+      <c r="B37" s="304"/>
+      <c r="C37" s="304"/>
+      <c r="D37" s="304"/>
+      <c r="E37" s="304"/>
+      <c r="F37" s="304"/>
+      <c r="G37" s="304"/>
+      <c r="H37" s="305"/>
     </row>
     <row r="38" spans="1:10" s="112" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="295"/>
-      <c r="B38" s="296"/>
-      <c r="C38" s="296"/>
-      <c r="D38" s="296"/>
-      <c r="E38" s="296"/>
-      <c r="F38" s="296"/>
-      <c r="G38" s="296"/>
-      <c r="H38" s="297"/>
+      <c r="A38" s="303"/>
+      <c r="B38" s="304"/>
+      <c r="C38" s="304"/>
+      <c r="D38" s="304"/>
+      <c r="E38" s="304"/>
+      <c r="F38" s="304"/>
+      <c r="G38" s="304"/>
+      <c r="H38" s="305"/>
     </row>
     <row r="39" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="298"/>
-      <c r="B39" s="299"/>
-      <c r="C39" s="299"/>
-      <c r="D39" s="299"/>
-      <c r="E39" s="299"/>
-      <c r="F39" s="299"/>
-      <c r="G39" s="299"/>
-      <c r="H39" s="300"/>
+      <c r="A39" s="306"/>
+      <c r="B39" s="307"/>
+      <c r="C39" s="307"/>
+      <c r="D39" s="307"/>
+      <c r="E39" s="307"/>
+      <c r="F39" s="307"/>
+      <c r="G39" s="307"/>
+      <c r="H39" s="308"/>
       <c r="I39" s="112"/>
       <c r="J39" s="112"/>
     </row>
@@ -8259,15 +8253,15 @@
       <c r="J40" s="112"/>
     </row>
     <row r="41" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="A41" s="285" t="s">
+      <c r="A41" s="293" t="s">
         <v>307</v>
       </c>
-      <c r="B41" s="285"/>
-      <c r="C41" s="285"/>
-      <c r="D41" s="285"/>
-      <c r="E41" s="285"/>
-      <c r="F41" s="285"/>
-      <c r="G41" s="285"/>
+      <c r="B41" s="293"/>
+      <c r="C41" s="293"/>
+      <c r="D41" s="293"/>
+      <c r="E41" s="293"/>
+      <c r="F41" s="293"/>
+      <c r="G41" s="293"/>
       <c r="H41" s="112"/>
       <c r="I41" s="112"/>
       <c r="J41" s="112"/>
@@ -8282,12 +8276,12 @@
       <c r="C42" s="77" t="s">
         <v>309</v>
       </c>
-      <c r="D42" s="284" t="s">
+      <c r="D42" s="292" t="s">
         <v>310</v>
       </c>
-      <c r="E42" s="284"/>
-      <c r="F42" s="284"/>
-      <c r="G42" s="284"/>
+      <c r="E42" s="292"/>
+      <c r="F42" s="292"/>
+      <c r="G42" s="292"/>
       <c r="H42" s="112"/>
       <c r="I42" s="112"/>
       <c r="J42" s="112"/>
@@ -8529,68 +8523,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="324" t="s">
+      <c r="A1" s="325" t="s">
         <v>244</v>
       </c>
-      <c r="B1" s="324"/>
-      <c r="C1" s="324"/>
-      <c r="D1" s="324"/>
-      <c r="E1" s="324"/>
-      <c r="F1" s="324"/>
-      <c r="G1" s="324"/>
-      <c r="H1" s="324"/>
-      <c r="I1" s="324"/>
-      <c r="J1" s="324"/>
-      <c r="K1" s="324"/>
-      <c r="L1" s="324"/>
-      <c r="M1" s="324"/>
-      <c r="N1" s="324"/>
-      <c r="O1" s="324"/>
+      <c r="B1" s="325"/>
+      <c r="C1" s="325"/>
+      <c r="D1" s="325"/>
+      <c r="E1" s="325"/>
+      <c r="F1" s="325"/>
+      <c r="G1" s="325"/>
+      <c r="H1" s="325"/>
+      <c r="I1" s="325"/>
+      <c r="J1" s="325"/>
+      <c r="K1" s="325"/>
+      <c r="L1" s="325"/>
+      <c r="M1" s="325"/>
+      <c r="N1" s="325"/>
+      <c r="O1" s="325"/>
       <c r="P1" s="30"/>
       <c r="Q1" s="30"/>
     </row>
     <row r="2" spans="1:17" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="318" t="s">
+      <c r="A2" s="336" t="s">
         <v>279</v>
       </c>
-      <c r="B2" s="319"/>
-      <c r="C2" s="319"/>
-      <c r="D2" s="319"/>
-      <c r="E2" s="319"/>
-      <c r="F2" s="320"/>
-      <c r="G2" s="325" t="s">
+      <c r="B2" s="337"/>
+      <c r="C2" s="337"/>
+      <c r="D2" s="337"/>
+      <c r="E2" s="337"/>
+      <c r="F2" s="338"/>
+      <c r="G2" s="326" t="s">
         <v>246</v>
       </c>
-      <c r="H2" s="325"/>
-      <c r="I2" s="325"/>
-      <c r="J2" s="325"/>
-      <c r="K2" s="325"/>
-      <c r="L2" s="325"/>
-      <c r="M2" s="314" t="s">
+      <c r="H2" s="326"/>
+      <c r="I2" s="326"/>
+      <c r="J2" s="326"/>
+      <c r="K2" s="326"/>
+      <c r="L2" s="326"/>
+      <c r="M2" s="332" t="s">
         <v>295</v>
       </c>
-      <c r="N2" s="314"/>
-      <c r="O2" s="314"/>
+      <c r="N2" s="332"/>
+      <c r="O2" s="332"/>
       <c r="P2" s="88"/>
       <c r="Q2" s="88"/>
     </row>
     <row r="3" spans="1:17" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="321" t="s">
+      <c r="A3" s="339" t="s">
         <v>472</v>
       </c>
-      <c r="B3" s="322"/>
-      <c r="C3" s="322"/>
-      <c r="D3" s="322"/>
-      <c r="E3" s="322"/>
-      <c r="F3" s="323"/>
-      <c r="G3" s="327" t="s">
+      <c r="B3" s="340"/>
+      <c r="C3" s="340"/>
+      <c r="D3" s="340"/>
+      <c r="E3" s="340"/>
+      <c r="F3" s="341"/>
+      <c r="G3" s="328" t="s">
         <v>301</v>
       </c>
-      <c r="H3" s="327"/>
-      <c r="I3" s="327"/>
-      <c r="J3" s="327"/>
-      <c r="K3" s="327"/>
-      <c r="L3" s="327"/>
+      <c r="H3" s="328"/>
+      <c r="I3" s="328"/>
+      <c r="J3" s="328"/>
+      <c r="K3" s="328"/>
+      <c r="L3" s="328"/>
       <c r="M3" s="202" t="s">
         <v>299</v>
       </c>
@@ -8603,24 +8597,24 @@
       <c r="P3" s="194"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="328" t="s">
+      <c r="A4" s="329" t="s">
         <v>473</v>
       </c>
-      <c r="B4" s="329"/>
-      <c r="C4" s="329"/>
-      <c r="D4" s="329"/>
-      <c r="E4" s="329"/>
-      <c r="F4" s="330"/>
-      <c r="G4" s="326" t="s">
+      <c r="B4" s="330"/>
+      <c r="C4" s="330"/>
+      <c r="D4" s="330"/>
+      <c r="E4" s="330"/>
+      <c r="F4" s="331"/>
+      <c r="G4" s="327" t="s">
         <v>247</v>
       </c>
-      <c r="H4" s="326"/>
-      <c r="I4" s="326"/>
-      <c r="J4" s="326" t="s">
+      <c r="H4" s="327"/>
+      <c r="I4" s="327"/>
+      <c r="J4" s="327" t="s">
         <v>302</v>
       </c>
-      <c r="K4" s="326"/>
-      <c r="L4" s="326"/>
+      <c r="K4" s="327"/>
+      <c r="L4" s="327"/>
       <c r="M4" s="203" t="s">
         <v>154</v>
       </c>
@@ -8632,22 +8626,22 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="331"/>
-      <c r="B5" s="332"/>
-      <c r="C5" s="332"/>
-      <c r="D5" s="332"/>
-      <c r="E5" s="332"/>
-      <c r="F5" s="333"/>
-      <c r="G5" s="313" t="s">
+      <c r="A5" s="322"/>
+      <c r="B5" s="323"/>
+      <c r="C5" s="323"/>
+      <c r="D5" s="323"/>
+      <c r="E5" s="323"/>
+      <c r="F5" s="324"/>
+      <c r="G5" s="321" t="s">
         <v>278</v>
       </c>
-      <c r="H5" s="313"/>
-      <c r="I5" s="313"/>
-      <c r="J5" s="313" t="s">
+      <c r="H5" s="321"/>
+      <c r="I5" s="321"/>
+      <c r="J5" s="321" t="s">
         <v>292</v>
       </c>
-      <c r="K5" s="313"/>
-      <c r="L5" s="313"/>
+      <c r="K5" s="321"/>
+      <c r="L5" s="321"/>
       <c r="M5" s="204"/>
       <c r="N5" s="204" t="s">
         <v>384</v>
@@ -8657,22 +8651,22 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="331" t="s">
+      <c r="A6" s="322" t="s">
         <v>474</v>
       </c>
-      <c r="B6" s="332"/>
-      <c r="C6" s="332"/>
-      <c r="D6" s="332"/>
-      <c r="E6" s="332"/>
-      <c r="F6" s="333"/>
-      <c r="G6" s="313" t="s">
+      <c r="B6" s="323"/>
+      <c r="C6" s="323"/>
+      <c r="D6" s="323"/>
+      <c r="E6" s="323"/>
+      <c r="F6" s="324"/>
+      <c r="G6" s="321" t="s">
         <v>285</v>
       </c>
-      <c r="H6" s="313"/>
-      <c r="I6" s="313"/>
-      <c r="J6" s="313"/>
-      <c r="K6" s="313"/>
-      <c r="L6" s="313"/>
+      <c r="H6" s="321"/>
+      <c r="I6" s="321"/>
+      <c r="J6" s="321"/>
+      <c r="K6" s="321"/>
+      <c r="L6" s="321"/>
       <c r="M6" s="204"/>
       <c r="N6" s="204" t="s">
         <v>385</v>
@@ -8682,54 +8676,54 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="331" t="s">
+      <c r="A7" s="322" t="s">
         <v>475</v>
       </c>
-      <c r="B7" s="332"/>
-      <c r="C7" s="332"/>
-      <c r="D7" s="332"/>
-      <c r="E7" s="332"/>
-      <c r="F7" s="333"/>
-      <c r="G7" s="313"/>
-      <c r="H7" s="313"/>
-      <c r="I7" s="313"/>
-      <c r="J7" s="313"/>
-      <c r="K7" s="313"/>
-      <c r="L7" s="313"/>
+      <c r="B7" s="323"/>
+      <c r="C7" s="323"/>
+      <c r="D7" s="323"/>
+      <c r="E7" s="323"/>
+      <c r="F7" s="324"/>
+      <c r="G7" s="321"/>
+      <c r="H7" s="321"/>
+      <c r="I7" s="321"/>
+      <c r="J7" s="321"/>
+      <c r="K7" s="321"/>
+      <c r="L7" s="321"/>
       <c r="M7" s="204"/>
       <c r="N7" s="204"/>
       <c r="O7" s="205"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="331"/>
-      <c r="B8" s="332"/>
-      <c r="C8" s="332"/>
-      <c r="D8" s="332"/>
-      <c r="E8" s="332"/>
-      <c r="F8" s="333"/>
-      <c r="G8" s="313"/>
-      <c r="H8" s="313"/>
-      <c r="I8" s="313"/>
-      <c r="J8" s="313"/>
-      <c r="K8" s="313"/>
-      <c r="L8" s="313"/>
+      <c r="A8" s="322"/>
+      <c r="B8" s="323"/>
+      <c r="C8" s="323"/>
+      <c r="D8" s="323"/>
+      <c r="E8" s="323"/>
+      <c r="F8" s="324"/>
+      <c r="G8" s="321"/>
+      <c r="H8" s="321"/>
+      <c r="I8" s="321"/>
+      <c r="J8" s="321"/>
+      <c r="K8" s="321"/>
+      <c r="L8" s="321"/>
       <c r="M8" s="204"/>
       <c r="N8" s="204"/>
       <c r="O8" s="205"/>
     </row>
     <row r="9" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:17" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="315" t="s">
+      <c r="A10" s="333" t="s">
         <v>354</v>
       </c>
-      <c r="B10" s="316"/>
-      <c r="C10" s="316"/>
-      <c r="D10" s="316"/>
-      <c r="E10" s="316"/>
-      <c r="F10" s="316"/>
-      <c r="G10" s="316"/>
-      <c r="H10" s="316"/>
-      <c r="I10" s="317"/>
+      <c r="B10" s="334"/>
+      <c r="C10" s="334"/>
+      <c r="D10" s="334"/>
+      <c r="E10" s="334"/>
+      <c r="F10" s="334"/>
+      <c r="G10" s="334"/>
+      <c r="H10" s="334"/>
+      <c r="I10" s="335"/>
     </row>
     <row r="11" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="130" t="s">
@@ -8819,69 +8813,69 @@
     </row>
     <row r="14" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="301" t="s">
+      <c r="A15" s="309" t="s">
         <v>280</v>
       </c>
-      <c r="B15" s="302"/>
-      <c r="C15" s="302"/>
-      <c r="D15" s="302"/>
-      <c r="E15" s="302"/>
-      <c r="F15" s="302"/>
-      <c r="G15" s="302"/>
-      <c r="H15" s="303"/>
+      <c r="B15" s="310"/>
+      <c r="C15" s="310"/>
+      <c r="D15" s="310"/>
+      <c r="E15" s="310"/>
+      <c r="F15" s="310"/>
+      <c r="G15" s="310"/>
+      <c r="H15" s="311"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="295" t="s">
+      <c r="A16" s="303" t="s">
         <v>362</v>
       </c>
-      <c r="B16" s="296"/>
-      <c r="C16" s="296"/>
-      <c r="D16" s="296"/>
-      <c r="E16" s="296"/>
-      <c r="F16" s="296"/>
-      <c r="G16" s="296"/>
-      <c r="H16" s="297"/>
+      <c r="B16" s="304"/>
+      <c r="C16" s="304"/>
+      <c r="D16" s="304"/>
+      <c r="E16" s="304"/>
+      <c r="F16" s="304"/>
+      <c r="G16" s="304"/>
+      <c r="H16" s="305"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="295"/>
-      <c r="B17" s="296"/>
-      <c r="C17" s="296"/>
-      <c r="D17" s="296"/>
-      <c r="E17" s="296"/>
-      <c r="F17" s="296"/>
-      <c r="G17" s="296"/>
-      <c r="H17" s="297"/>
+      <c r="A17" s="303"/>
+      <c r="B17" s="304"/>
+      <c r="C17" s="304"/>
+      <c r="D17" s="304"/>
+      <c r="E17" s="304"/>
+      <c r="F17" s="304"/>
+      <c r="G17" s="304"/>
+      <c r="H17" s="305"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="295"/>
-      <c r="B18" s="296"/>
-      <c r="C18" s="296"/>
-      <c r="D18" s="296"/>
-      <c r="E18" s="296"/>
-      <c r="F18" s="296"/>
-      <c r="G18" s="296"/>
-      <c r="H18" s="297"/>
+      <c r="A18" s="303"/>
+      <c r="B18" s="304"/>
+      <c r="C18" s="304"/>
+      <c r="D18" s="304"/>
+      <c r="E18" s="304"/>
+      <c r="F18" s="304"/>
+      <c r="G18" s="304"/>
+      <c r="H18" s="305"/>
     </row>
     <row r="19" spans="1:8" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="298"/>
-      <c r="B19" s="299"/>
-      <c r="C19" s="299"/>
-      <c r="D19" s="299"/>
-      <c r="E19" s="299"/>
-      <c r="F19" s="299"/>
-      <c r="G19" s="299"/>
-      <c r="H19" s="300"/>
+      <c r="A19" s="306"/>
+      <c r="B19" s="307"/>
+      <c r="C19" s="307"/>
+      <c r="D19" s="307"/>
+      <c r="E19" s="307"/>
+      <c r="F19" s="307"/>
+      <c r="G19" s="307"/>
+      <c r="H19" s="308"/>
     </row>
     <row r="21" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A21" s="285" t="s">
+      <c r="A21" s="293" t="s">
         <v>307</v>
       </c>
-      <c r="B21" s="285"/>
-      <c r="C21" s="285"/>
-      <c r="D21" s="285"/>
-      <c r="E21" s="285"/>
-      <c r="F21" s="285"/>
-      <c r="G21" s="285"/>
+      <c r="B21" s="293"/>
+      <c r="C21" s="293"/>
+      <c r="D21" s="293"/>
+      <c r="E21" s="293"/>
+      <c r="F21" s="293"/>
+      <c r="G21" s="293"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="77" t="s">
@@ -8893,12 +8887,12 @@
       <c r="C22" s="77" t="s">
         <v>309</v>
       </c>
-      <c r="D22" s="284" t="s">
+      <c r="D22" s="292" t="s">
         <v>310</v>
       </c>
-      <c r="E22" s="284"/>
-      <c r="F22" s="284"/>
-      <c r="G22" s="284"/>
+      <c r="E22" s="292"/>
+      <c r="F22" s="292"/>
+      <c r="G22" s="292"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -9336,12 +9330,14 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="A16:H19"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="G6:I6"/>
     <mergeCell ref="J6:L6"/>
@@ -9354,14 +9350,12 @@
     <mergeCell ref="A4:F4"/>
     <mergeCell ref="A5:F5"/>
     <mergeCell ref="A6:F6"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="A16:H19"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A8:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9453,68 +9447,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="324" t="s">
+      <c r="A1" s="325" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="324"/>
-      <c r="C1" s="324"/>
-      <c r="D1" s="324"/>
-      <c r="E1" s="324"/>
-      <c r="F1" s="324"/>
-      <c r="G1" s="324"/>
-      <c r="H1" s="324"/>
-      <c r="I1" s="324"/>
-      <c r="J1" s="324"/>
-      <c r="K1" s="324"/>
-      <c r="L1" s="324"/>
-      <c r="M1" s="324"/>
-      <c r="N1" s="324"/>
-      <c r="O1" s="324"/>
-      <c r="P1" s="324"/>
+      <c r="B1" s="325"/>
+      <c r="C1" s="325"/>
+      <c r="D1" s="325"/>
+      <c r="E1" s="325"/>
+      <c r="F1" s="325"/>
+      <c r="G1" s="325"/>
+      <c r="H1" s="325"/>
+      <c r="I1" s="325"/>
+      <c r="J1" s="325"/>
+      <c r="K1" s="325"/>
+      <c r="L1" s="325"/>
+      <c r="M1" s="325"/>
+      <c r="N1" s="325"/>
+      <c r="O1" s="325"/>
+      <c r="P1" s="325"/>
       <c r="Q1" s="30"/>
     </row>
     <row r="2" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="325" t="s">
+      <c r="A2" s="326" t="s">
         <v>279</v>
       </c>
-      <c r="B2" s="325"/>
-      <c r="C2" s="325"/>
-      <c r="D2" s="325"/>
-      <c r="E2" s="325"/>
-      <c r="F2" s="325"/>
-      <c r="G2" s="325" t="s">
+      <c r="B2" s="326"/>
+      <c r="C2" s="326"/>
+      <c r="D2" s="326"/>
+      <c r="E2" s="326"/>
+      <c r="F2" s="326"/>
+      <c r="G2" s="326" t="s">
         <v>246</v>
       </c>
-      <c r="H2" s="325"/>
-      <c r="I2" s="325"/>
-      <c r="J2" s="325"/>
-      <c r="K2" s="325"/>
-      <c r="L2" s="325"/>
-      <c r="M2" s="314" t="s">
+      <c r="H2" s="326"/>
+      <c r="I2" s="326"/>
+      <c r="J2" s="326"/>
+      <c r="K2" s="326"/>
+      <c r="L2" s="326"/>
+      <c r="M2" s="332" t="s">
         <v>294</v>
       </c>
-      <c r="N2" s="314"/>
-      <c r="O2" s="314"/>
-      <c r="P2" s="314"/>
+      <c r="N2" s="332"/>
+      <c r="O2" s="332"/>
+      <c r="P2" s="332"/>
       <c r="Q2" s="88"/>
     </row>
     <row r="3" spans="1:17" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="327" t="s">
+      <c r="A3" s="328" t="s">
         <v>476</v>
       </c>
-      <c r="B3" s="327"/>
-      <c r="C3" s="327"/>
-      <c r="D3" s="327"/>
-      <c r="E3" s="327"/>
-      <c r="F3" s="327"/>
-      <c r="G3" s="327" t="s">
+      <c r="B3" s="328"/>
+      <c r="C3" s="328"/>
+      <c r="D3" s="328"/>
+      <c r="E3" s="328"/>
+      <c r="F3" s="328"/>
+      <c r="G3" s="328" t="s">
         <v>296</v>
       </c>
-      <c r="H3" s="327"/>
-      <c r="I3" s="327"/>
-      <c r="J3" s="327"/>
-      <c r="K3" s="327"/>
-      <c r="L3" s="327"/>
+      <c r="H3" s="328"/>
+      <c r="I3" s="328"/>
+      <c r="J3" s="328"/>
+      <c r="K3" s="328"/>
+      <c r="L3" s="328"/>
       <c r="M3" s="202" t="s">
         <v>298</v>
       </c>
@@ -9530,22 +9524,22 @@
       <c r="Q3" s="193"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="328" t="s">
+      <c r="A4" s="329" t="s">
         <v>473</v>
       </c>
-      <c r="B4" s="329"/>
-      <c r="C4" s="329"/>
-      <c r="D4" s="329"/>
-      <c r="E4" s="329"/>
-      <c r="F4" s="330"/>
-      <c r="G4" s="326" t="s">
+      <c r="B4" s="330"/>
+      <c r="C4" s="330"/>
+      <c r="D4" s="330"/>
+      <c r="E4" s="330"/>
+      <c r="F4" s="331"/>
+      <c r="G4" s="327" t="s">
         <v>248</v>
       </c>
-      <c r="H4" s="326"/>
-      <c r="I4" s="326"/>
-      <c r="J4" s="326"/>
-      <c r="K4" s="326"/>
-      <c r="L4" s="326"/>
+      <c r="H4" s="327"/>
+      <c r="I4" s="327"/>
+      <c r="J4" s="327"/>
+      <c r="K4" s="327"/>
+      <c r="L4" s="327"/>
       <c r="M4" s="203" t="s">
         <v>252</v>
       </c>
@@ -9560,20 +9554,20 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="331"/>
-      <c r="B5" s="332"/>
-      <c r="C5" s="332"/>
-      <c r="D5" s="332"/>
-      <c r="E5" s="332"/>
-      <c r="F5" s="333"/>
-      <c r="G5" s="334" t="s">
+      <c r="A5" s="322"/>
+      <c r="B5" s="323"/>
+      <c r="C5" s="323"/>
+      <c r="D5" s="323"/>
+      <c r="E5" s="323"/>
+      <c r="F5" s="324"/>
+      <c r="G5" s="342" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="334"/>
-      <c r="I5" s="334"/>
-      <c r="J5" s="334"/>
-      <c r="K5" s="334"/>
-      <c r="L5" s="334"/>
+      <c r="H5" s="342"/>
+      <c r="I5" s="342"/>
+      <c r="J5" s="342"/>
+      <c r="K5" s="342"/>
+      <c r="L5" s="342"/>
       <c r="M5" s="204" t="s">
         <v>291</v>
       </c>
@@ -9586,22 +9580,22 @@
       </c>
     </row>
     <row r="6" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="331" t="s">
+      <c r="A6" s="322" t="s">
         <v>479</v>
       </c>
-      <c r="B6" s="332"/>
-      <c r="C6" s="332"/>
-      <c r="D6" s="332"/>
-      <c r="E6" s="332"/>
-      <c r="F6" s="333"/>
-      <c r="G6" s="334" t="s">
+      <c r="B6" s="323"/>
+      <c r="C6" s="323"/>
+      <c r="D6" s="323"/>
+      <c r="E6" s="323"/>
+      <c r="F6" s="324"/>
+      <c r="G6" s="342" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="334"/>
-      <c r="I6" s="334"/>
-      <c r="J6" s="334"/>
-      <c r="K6" s="334"/>
-      <c r="L6" s="334"/>
+      <c r="H6" s="342"/>
+      <c r="I6" s="342"/>
+      <c r="J6" s="342"/>
+      <c r="K6" s="342"/>
+      <c r="L6" s="342"/>
       <c r="M6" s="204"/>
       <c r="N6" s="204"/>
       <c r="O6" s="204" t="s">
@@ -9612,36 +9606,36 @@
       </c>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="331"/>
-      <c r="B7" s="332"/>
-      <c r="C7" s="332"/>
-      <c r="D7" s="332"/>
-      <c r="E7" s="332"/>
-      <c r="F7" s="333"/>
-      <c r="G7" s="334"/>
-      <c r="H7" s="334"/>
-      <c r="I7" s="334"/>
-      <c r="J7" s="334"/>
-      <c r="K7" s="334"/>
-      <c r="L7" s="334"/>
+      <c r="A7" s="322"/>
+      <c r="B7" s="323"/>
+      <c r="C7" s="323"/>
+      <c r="D7" s="323"/>
+      <c r="E7" s="323"/>
+      <c r="F7" s="324"/>
+      <c r="G7" s="342"/>
+      <c r="H7" s="342"/>
+      <c r="I7" s="342"/>
+      <c r="J7" s="342"/>
+      <c r="K7" s="342"/>
+      <c r="L7" s="342"/>
       <c r="M7" s="204"/>
       <c r="N7" s="204"/>
       <c r="O7" s="204"/>
       <c r="P7" s="205"/>
     </row>
     <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="331"/>
-      <c r="B8" s="332"/>
-      <c r="C8" s="332"/>
-      <c r="D8" s="332"/>
-      <c r="E8" s="332"/>
-      <c r="F8" s="333"/>
-      <c r="G8" s="334"/>
-      <c r="H8" s="334"/>
-      <c r="I8" s="334"/>
-      <c r="J8" s="334"/>
-      <c r="K8" s="334"/>
-      <c r="L8" s="334"/>
+      <c r="A8" s="322"/>
+      <c r="B8" s="323"/>
+      <c r="C8" s="323"/>
+      <c r="D8" s="323"/>
+      <c r="E8" s="323"/>
+      <c r="F8" s="324"/>
+      <c r="G8" s="342"/>
+      <c r="H8" s="342"/>
+      <c r="I8" s="342"/>
+      <c r="J8" s="342"/>
+      <c r="K8" s="342"/>
+      <c r="L8" s="342"/>
       <c r="M8" s="204"/>
       <c r="N8" s="204"/>
       <c r="O8" s="204"/>
@@ -9649,17 +9643,17 @@
     </row>
     <row r="9" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:17" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="315" t="s">
+      <c r="A10" s="333" t="s">
         <v>353</v>
       </c>
-      <c r="B10" s="316"/>
-      <c r="C10" s="316"/>
-      <c r="D10" s="316"/>
-      <c r="E10" s="316"/>
-      <c r="F10" s="316"/>
-      <c r="G10" s="316"/>
-      <c r="H10" s="316"/>
-      <c r="I10" s="317"/>
+      <c r="B10" s="334"/>
+      <c r="C10" s="334"/>
+      <c r="D10" s="334"/>
+      <c r="E10" s="334"/>
+      <c r="F10" s="334"/>
+      <c r="G10" s="334"/>
+      <c r="H10" s="334"/>
+      <c r="I10" s="335"/>
     </row>
     <row r="11" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="130" t="s">
@@ -9748,69 +9742,69 @@
     </row>
     <row r="14" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="301" t="s">
+      <c r="A15" s="309" t="s">
         <v>280</v>
       </c>
-      <c r="B15" s="302"/>
-      <c r="C15" s="302"/>
-      <c r="D15" s="302"/>
-      <c r="E15" s="302"/>
-      <c r="F15" s="302"/>
-      <c r="G15" s="302"/>
-      <c r="H15" s="303"/>
+      <c r="B15" s="310"/>
+      <c r="C15" s="310"/>
+      <c r="D15" s="310"/>
+      <c r="E15" s="310"/>
+      <c r="F15" s="310"/>
+      <c r="G15" s="310"/>
+      <c r="H15" s="311"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="295" t="s">
+      <c r="A16" s="303" t="s">
         <v>363</v>
       </c>
-      <c r="B16" s="296"/>
-      <c r="C16" s="296"/>
-      <c r="D16" s="296"/>
-      <c r="E16" s="296"/>
-      <c r="F16" s="296"/>
-      <c r="G16" s="296"/>
-      <c r="H16" s="297"/>
+      <c r="B16" s="304"/>
+      <c r="C16" s="304"/>
+      <c r="D16" s="304"/>
+      <c r="E16" s="304"/>
+      <c r="F16" s="304"/>
+      <c r="G16" s="304"/>
+      <c r="H16" s="305"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="295"/>
-      <c r="B17" s="296"/>
-      <c r="C17" s="296"/>
-      <c r="D17" s="296"/>
-      <c r="E17" s="296"/>
-      <c r="F17" s="296"/>
-      <c r="G17" s="296"/>
-      <c r="H17" s="297"/>
+      <c r="A17" s="303"/>
+      <c r="B17" s="304"/>
+      <c r="C17" s="304"/>
+      <c r="D17" s="304"/>
+      <c r="E17" s="304"/>
+      <c r="F17" s="304"/>
+      <c r="G17" s="304"/>
+      <c r="H17" s="305"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="295"/>
-      <c r="B18" s="296"/>
-      <c r="C18" s="296"/>
-      <c r="D18" s="296"/>
-      <c r="E18" s="296"/>
-      <c r="F18" s="296"/>
-      <c r="G18" s="296"/>
-      <c r="H18" s="297"/>
+      <c r="A18" s="303"/>
+      <c r="B18" s="304"/>
+      <c r="C18" s="304"/>
+      <c r="D18" s="304"/>
+      <c r="E18" s="304"/>
+      <c r="F18" s="304"/>
+      <c r="G18" s="304"/>
+      <c r="H18" s="305"/>
     </row>
     <row r="19" spans="1:8" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="298"/>
-      <c r="B19" s="299"/>
-      <c r="C19" s="299"/>
-      <c r="D19" s="299"/>
-      <c r="E19" s="299"/>
-      <c r="F19" s="299"/>
-      <c r="G19" s="299"/>
-      <c r="H19" s="300"/>
+      <c r="A19" s="306"/>
+      <c r="B19" s="307"/>
+      <c r="C19" s="307"/>
+      <c r="D19" s="307"/>
+      <c r="E19" s="307"/>
+      <c r="F19" s="307"/>
+      <c r="G19" s="307"/>
+      <c r="H19" s="308"/>
     </row>
     <row r="21" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A21" s="285" t="s">
+      <c r="A21" s="293" t="s">
         <v>307</v>
       </c>
-      <c r="B21" s="285"/>
-      <c r="C21" s="285"/>
-      <c r="D21" s="285"/>
-      <c r="E21" s="285"/>
-      <c r="F21" s="285"/>
-      <c r="G21" s="285"/>
+      <c r="B21" s="293"/>
+      <c r="C21" s="293"/>
+      <c r="D21" s="293"/>
+      <c r="E21" s="293"/>
+      <c r="F21" s="293"/>
+      <c r="G21" s="293"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="77" t="s">
@@ -9822,12 +9816,12 @@
       <c r="C22" s="77" t="s">
         <v>309</v>
       </c>
-      <c r="D22" s="284" t="s">
+      <c r="D22" s="292" t="s">
         <v>310</v>
       </c>
-      <c r="E22" s="284"/>
-      <c r="F22" s="284"/>
-      <c r="G22" s="284"/>
+      <c r="E22" s="292"/>
+      <c r="F22" s="292"/>
+      <c r="G22" s="292"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -9999,6 +9993,12 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="G2:L2"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="G3:L3"/>
     <mergeCell ref="A21:G21"/>
     <mergeCell ref="D22:G22"/>
     <mergeCell ref="G4:L4"/>
@@ -10014,12 +10014,6 @@
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="A8:F8"/>
     <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="G2:L2"/>
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="G3:L3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10083,10 +10077,10 @@
   <sheetPr codeName="Sheet6">
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:M85"/>
+  <dimension ref="A1:M84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -10101,12 +10095,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="335" t="s">
+      <c r="A1" s="343" t="s">
         <v>249</v>
       </c>
-      <c r="B1" s="336"/>
-      <c r="C1" s="336"/>
-      <c r="D1" s="337"/>
+      <c r="B1" s="344"/>
+      <c r="C1" s="344"/>
+      <c r="D1" s="345"/>
       <c r="E1" s="65"/>
       <c r="F1" s="65"/>
       <c r="G1" s="65"/>
@@ -10127,7 +10121,7 @@
       <c r="C2" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="D2" s="351" t="s">
+      <c r="D2" s="240" t="s">
         <v>75</v>
       </c>
       <c r="F2" s="134" t="s">
@@ -10181,7 +10175,7 @@
       <c r="B6" s="16" t="s">
         <v>491</v>
       </c>
-      <c r="C6" s="352"/>
+      <c r="C6" s="241"/>
       <c r="D6" s="23">
         <v>1000000</v>
       </c>
@@ -10193,7 +10187,7 @@
       <c r="B7" s="16" t="s">
         <v>493</v>
       </c>
-      <c r="C7" s="353"/>
+      <c r="C7" s="242"/>
       <c r="D7" s="23">
         <v>0</v>
       </c>
@@ -10205,7 +10199,7 @@
       <c r="B8" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="354"/>
+      <c r="C8" s="243"/>
       <c r="D8" s="23">
         <v>0</v>
       </c>
@@ -10217,31 +10211,33 @@
       <c r="B9" s="15" t="s">
         <v>495</v>
       </c>
-      <c r="C9" s="354"/>
+      <c r="C9" s="243"/>
       <c r="D9" s="23">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="200" t="s">
+      <c r="A10" s="12" t="s">
+        <v>467</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>468</v>
+      </c>
+      <c r="C10" s="201"/>
+      <c r="D10" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="200" t="s">
         <v>496</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B11" s="16" t="s">
         <v>497</v>
       </c>
-      <c r="C10" s="352"/>
-      <c r="D10" s="23"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
-        <v>467</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>468</v>
-      </c>
-      <c r="C11" s="201"/>
+      <c r="C11" s="241"/>
       <c r="D11" s="23">
-        <v>1</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -10251,9 +10247,9 @@
       <c r="B12" s="16" t="s">
         <v>499</v>
       </c>
-      <c r="C12" s="352"/>
+      <c r="C12" s="241"/>
       <c r="D12" s="23">
-        <v>10000</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -10263,10 +10259,8 @@
       <c r="B13" s="16" t="s">
         <v>501</v>
       </c>
-      <c r="C13" s="352"/>
-      <c r="D13" s="23">
-        <v>0.1</v>
-      </c>
+      <c r="C13" s="241"/>
+      <c r="D13" s="23"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="200" t="s">
@@ -10275,7 +10269,7 @@
       <c r="B14" s="16" t="s">
         <v>503</v>
       </c>
-      <c r="C14" s="352"/>
+      <c r="C14" s="241"/>
       <c r="D14" s="23"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -10285,8 +10279,10 @@
       <c r="B15" s="16" t="s">
         <v>505</v>
       </c>
-      <c r="C15" s="352"/>
-      <c r="D15" s="23"/>
+      <c r="C15" s="241"/>
+      <c r="D15" s="23">
+        <v>10</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="200" t="s">
@@ -10295,10 +10291,8 @@
       <c r="B16" s="16" t="s">
         <v>507</v>
       </c>
-      <c r="C16" s="352"/>
-      <c r="D16" s="23">
-        <v>10</v>
-      </c>
+      <c r="C16" s="241"/>
+      <c r="D16" s="23"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="200" t="s">
@@ -10307,386 +10301,388 @@
       <c r="B17" s="16" t="s">
         <v>509</v>
       </c>
-      <c r="C17" s="352"/>
+      <c r="C17" s="241"/>
       <c r="D17" s="23"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="200" t="s">
-        <v>510</v>
+      <c r="A18" s="12" t="s">
+        <v>469</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>511</v>
-      </c>
-      <c r="C18" s="352"/>
-      <c r="D18" s="23"/>
+        <v>470</v>
+      </c>
+      <c r="C18" s="201"/>
+      <c r="D18" s="23">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>469</v>
+        <v>102</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>470</v>
-      </c>
-      <c r="C19" s="201"/>
-      <c r="D19" s="23">
-        <v>1</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="C19" s="181"/>
+      <c r="D19" s="23"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="181"/>
-      <c r="D20" s="23"/>
+      <c r="A20" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="180"/>
+      <c r="D20" s="22"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="180"/>
-      <c r="D21" s="22"/>
+      <c r="A21" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="181"/>
+      <c r="D21" s="23">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>29</v>
+        <v>71</v>
       </c>
       <c r="C22" s="181"/>
-      <c r="D22" s="23">
-        <v>0</v>
+      <c r="D22" s="24" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C23" s="181"/>
       <c r="D23" s="24" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="C24" s="181"/>
-      <c r="D24" s="24" t="s">
-        <v>69</v>
+      <c r="D24" s="23">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C25" s="181"/>
-      <c r="D25" s="23">
-        <v>0</v>
+      <c r="D25" s="23" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" s="181"/>
-      <c r="D26" s="23" t="s">
-        <v>31</v>
-      </c>
+      <c r="A26" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="180"/>
+      <c r="D26" s="22"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27" s="180"/>
-      <c r="D27" s="22"/>
+      <c r="A27" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="181"/>
+      <c r="D27" s="23"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C28" s="181"/>
       <c r="D28" s="23"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C29" s="181"/>
       <c r="D29" s="23"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C30" s="181"/>
       <c r="D30" s="23"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C31" s="181"/>
-      <c r="D31" s="23"/>
+      <c r="D31" s="23">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C32" s="181"/>
-      <c r="D32" s="23">
-        <v>1</v>
-      </c>
+      <c r="D32" s="23"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="C33" s="181"/>
       <c r="D33" s="23"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C34" s="181"/>
       <c r="D34" s="23"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="B35" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C35" s="181"/>
-      <c r="D35" s="23"/>
+      <c r="A35" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35" s="180"/>
+      <c r="D35" s="22"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="B36" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C36" s="180"/>
-      <c r="D36" s="22"/>
+      <c r="A36" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36" s="181"/>
+      <c r="D36" s="23">
+        <v>100</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C37" s="181"/>
       <c r="D37" s="23">
-        <v>100</v>
+        <v>65535</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C38" s="181"/>
       <c r="D38" s="23">
-        <v>65535</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C39" s="181"/>
       <c r="D39" s="23">
-        <v>10</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C40" s="181"/>
-      <c r="D40" s="23">
-        <v>0.1</v>
-      </c>
+      <c r="D40" s="23"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C41" s="181"/>
       <c r="D41" s="23"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>48</v>
+        <v>83</v>
       </c>
       <c r="C42" s="181"/>
       <c r="D42" s="23"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="B43" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="C43" s="181"/>
-      <c r="D43" s="23"/>
+      <c r="A43" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C43" s="180"/>
+      <c r="D43" s="22"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="B44" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="C44" s="180"/>
-      <c r="D44" s="22"/>
+      <c r="A44" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C44" s="181"/>
+      <c r="D44" s="23"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C45" s="181"/>
-      <c r="D45" s="23"/>
+      <c r="D45" s="23">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C46" s="181"/>
-      <c r="D46" s="23">
-        <v>0.02</v>
-      </c>
+      <c r="D46" s="23"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C47" s="181"/>
       <c r="D47" s="23"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C48" s="181"/>
       <c r="D48" s="23"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="C49" s="181"/>
-      <c r="D49" s="23"/>
+      <c r="D49" s="24" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
-        <v>128</v>
+        <v>166</v>
       </c>
       <c r="B50" s="15" t="s">
-        <v>73</v>
+        <v>167</v>
       </c>
       <c r="C50" s="181"/>
-      <c r="D50" s="24" t="s">
-        <v>72</v>
+      <c r="D50" s="24">
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="B51" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="C51" s="181"/>
-      <c r="D51" s="24">
-        <v>0</v>
-      </c>
+      <c r="A51" s="21" t="s">
+        <v>510</v>
+      </c>
+      <c r="B51" s="17" t="s">
+        <v>511</v>
+      </c>
+      <c r="C51" s="244"/>
+      <c r="D51" s="245"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="21" t="s">
+      <c r="A52" s="12" t="s">
         <v>512</v>
       </c>
-      <c r="B52" s="17" t="s">
+      <c r="B52" s="16" t="s">
         <v>513</v>
       </c>
-      <c r="C52" s="355"/>
-      <c r="D52" s="356"/>
+      <c r="C52" s="242"/>
+      <c r="D52" s="246">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
@@ -10695,10 +10691,8 @@
       <c r="B53" s="16" t="s">
         <v>515</v>
       </c>
-      <c r="C53" s="353"/>
-      <c r="D53" s="357">
-        <v>0.02</v>
-      </c>
+      <c r="C53" s="242"/>
+      <c r="D53" s="246"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
@@ -10707,8 +10701,8 @@
       <c r="B54" s="16" t="s">
         <v>517</v>
       </c>
-      <c r="C54" s="353"/>
-      <c r="D54" s="357"/>
+      <c r="C54" s="242"/>
+      <c r="D54" s="246"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
@@ -10717,8 +10711,8 @@
       <c r="B55" s="16" t="s">
         <v>519</v>
       </c>
-      <c r="C55" s="353"/>
-      <c r="D55" s="357"/>
+      <c r="C55" s="242"/>
+      <c r="D55" s="246"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
@@ -10727,145 +10721,147 @@
       <c r="B56" s="16" t="s">
         <v>521</v>
       </c>
-      <c r="C56" s="353"/>
-      <c r="D56" s="357"/>
+      <c r="C56" s="242"/>
+      <c r="D56" s="24" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="12" t="s">
-        <v>522</v>
-      </c>
-      <c r="B57" s="16" t="s">
-        <v>523</v>
-      </c>
-      <c r="C57" s="353"/>
-      <c r="D57" s="24" t="s">
-        <v>72</v>
-      </c>
+      <c r="A57" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B57" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C57" s="180"/>
+      <c r="D57" s="22"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="B58" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C58" s="180"/>
-      <c r="D58" s="22"/>
+      <c r="A58" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="B58" s="15"/>
+      <c r="C58" s="181"/>
+      <c r="D58" s="23"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="B59" s="15"/>
+        <v>130</v>
+      </c>
+      <c r="B59" s="15" t="s">
+        <v>85</v>
+      </c>
       <c r="C59" s="181"/>
       <c r="D59" s="23"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B60" s="15" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C60" s="181"/>
       <c r="D60" s="23"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C61" s="181"/>
       <c r="D61" s="23"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="12" t="s">
-        <v>132</v>
+        <v>168</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>87</v>
+        <v>169</v>
       </c>
       <c r="C62" s="181"/>
       <c r="D62" s="23"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="12" t="s">
-        <v>168</v>
+        <v>133</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>169</v>
+        <v>89</v>
       </c>
       <c r="C63" s="181"/>
       <c r="D63" s="23"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C64" s="181"/>
       <c r="D64" s="23"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="12" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C65" s="181"/>
       <c r="D65" s="23"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="12" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C66" s="181"/>
       <c r="D66" s="23"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="12" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B67" s="15" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C67" s="181"/>
       <c r="D67" s="23"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="12" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B68" s="15" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C68" s="181"/>
       <c r="D68" s="23"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="12" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B69" s="15" t="s">
-        <v>93</v>
+        <v>59</v>
       </c>
       <c r="C69" s="181"/>
-      <c r="D69" s="23"/>
+      <c r="D69" s="23">
+        <v>1</v>
+      </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="12" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B70" s="15" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C70" s="181"/>
       <c r="D70" s="23">
@@ -10874,10 +10870,10 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="12" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C71" s="181"/>
       <c r="D71" s="23">
@@ -10886,10 +10882,10 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="12" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B72" s="15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C72" s="181"/>
       <c r="D72" s="23">
@@ -10898,10 +10894,10 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="12" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B73" s="15" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C73" s="181"/>
       <c r="D73" s="23">
@@ -10910,138 +10906,126 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="12" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B74" s="15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C74" s="181"/>
       <c r="D74" s="23">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="12" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B75" s="15" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="C75" s="181"/>
-      <c r="D75" s="23">
-        <v>0</v>
-      </c>
+      <c r="D75" s="23"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="12" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B76" s="15" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C76" s="181"/>
       <c r="D76" s="23"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="B77" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="C77" s="181"/>
-      <c r="D77" s="23"/>
+      <c r="A77" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="B77" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="C77" s="180"/>
+      <c r="D77" s="179"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="B78" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="C78" s="180"/>
-      <c r="D78" s="179"/>
+      <c r="A78" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="B78" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="C78" s="181"/>
+      <c r="D78" s="25">
+        <v>0</v>
+      </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="B79" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="C79" s="181"/>
-      <c r="D79" s="25">
+      <c r="A79" s="21" t="s">
+        <v>350</v>
+      </c>
+      <c r="B79" s="17" t="s">
+        <v>522</v>
+      </c>
+      <c r="C79" s="180"/>
+      <c r="D79" s="179"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="12" t="s">
+        <v>351</v>
+      </c>
+      <c r="B80" s="16" t="s">
+        <v>352</v>
+      </c>
+      <c r="C80" s="181"/>
+      <c r="D80" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="21" t="s">
-        <v>350</v>
-      </c>
-      <c r="B80" s="17" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="21" t="s">
+        <v>523</v>
+      </c>
+      <c r="B81" s="247" t="s">
         <v>524</v>
       </c>
-      <c r="C80" s="180"/>
-      <c r="D80" s="179"/>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="12" t="s">
-        <v>351</v>
-      </c>
-      <c r="B81" s="16" t="s">
-        <v>352</v>
-      </c>
-      <c r="C81" s="181"/>
-      <c r="D81" s="25">
+      <c r="C81" s="180"/>
+      <c r="D81" s="179"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="12" t="s">
+        <v>525</v>
+      </c>
+      <c r="B82" s="16" t="s">
+        <v>526</v>
+      </c>
+      <c r="C82" s="181"/>
+      <c r="D82" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="21" t="s">
+        <v>155</v>
+      </c>
+      <c r="B83" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="C83" s="180"/>
+      <c r="D83" s="179"/>
+    </row>
+    <row r="84" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="B84" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="C84" s="182"/>
+      <c r="D84" s="28">
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="21" t="s">
-        <v>525</v>
-      </c>
-      <c r="B82" s="358" t="s">
-        <v>526</v>
-      </c>
-      <c r="C82" s="180"/>
-      <c r="D82" s="179"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="12" t="s">
-        <v>527</v>
-      </c>
-      <c r="B83" s="16" t="s">
-        <v>528</v>
-      </c>
-      <c r="C83" s="181"/>
-      <c r="D83" s="25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="B84" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="C84" s="180"/>
-      <c r="D84" s="179"/>
-    </row>
-    <row r="85" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="26" t="s">
-        <v>157</v>
-      </c>
-      <c r="B85" s="27" t="s">
-        <v>158</v>
-      </c>
-      <c r="C85" s="182"/>
-      <c r="D85" s="28">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="nz+s2XO+ftXiPvDFdCb363Kdxpm8/rTzkaQvNt3hixFy/XzDLwk3vacxi/mnwp2lCzlwAgpdDUMXZxUkXUE4MA==" saltValue="5VzOwROovNDqiQdmD//x7A==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection selectLockedCells="1"/>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
@@ -11075,23 +11059,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="341" t="s">
+      <c r="A1" s="349" t="s">
         <v>222</v>
       </c>
-      <c r="B1" s="342"/>
-      <c r="C1" s="342"/>
-      <c r="D1" s="342"/>
-      <c r="E1" s="342"/>
-      <c r="F1" s="342"/>
-      <c r="G1" s="342"/>
-      <c r="H1" s="342"/>
-      <c r="I1" s="342"/>
-      <c r="J1" s="342"/>
-      <c r="K1" s="342"/>
-      <c r="L1" s="342"/>
-      <c r="M1" s="342"/>
-      <c r="N1" s="342"/>
-      <c r="O1" s="342"/>
+      <c r="B1" s="350"/>
+      <c r="C1" s="350"/>
+      <c r="D1" s="350"/>
+      <c r="E1" s="350"/>
+      <c r="F1" s="350"/>
+      <c r="G1" s="350"/>
+      <c r="H1" s="350"/>
+      <c r="I1" s="350"/>
+      <c r="J1" s="350"/>
+      <c r="K1" s="350"/>
+      <c r="L1" s="350"/>
+      <c r="M1" s="350"/>
+      <c r="N1" s="350"/>
+      <c r="O1" s="350"/>
     </row>
     <row r="2" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33"/>
@@ -11109,17 +11093,17 @@
       <c r="M2" s="34"/>
     </row>
     <row r="3" spans="1:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="338" t="s">
+      <c r="B3" s="346" t="s">
         <v>223</v>
       </c>
-      <c r="C3" s="339"/>
-      <c r="D3" s="339"/>
-      <c r="E3" s="339"/>
-      <c r="F3" s="339"/>
-      <c r="G3" s="339"/>
-      <c r="H3" s="339"/>
-      <c r="I3" s="339"/>
-      <c r="J3" s="340"/>
+      <c r="C3" s="347"/>
+      <c r="D3" s="347"/>
+      <c r="E3" s="347"/>
+      <c r="F3" s="347"/>
+      <c r="G3" s="347"/>
+      <c r="H3" s="347"/>
+      <c r="I3" s="347"/>
+      <c r="J3" s="348"/>
     </row>
     <row r="4" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B4" s="36"/>
@@ -11310,21 +11294,21 @@
     </row>
     <row r="18" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="2:14" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B19" s="338" t="s">
+      <c r="B19" s="346" t="s">
         <v>223</v>
       </c>
-      <c r="C19" s="339"/>
-      <c r="D19" s="339"/>
-      <c r="E19" s="339"/>
-      <c r="F19" s="339"/>
-      <c r="G19" s="339"/>
-      <c r="H19" s="339"/>
-      <c r="I19" s="339"/>
-      <c r="J19" s="339"/>
-      <c r="K19" s="339"/>
-      <c r="L19" s="339"/>
-      <c r="M19" s="339"/>
-      <c r="N19" s="340"/>
+      <c r="C19" s="347"/>
+      <c r="D19" s="347"/>
+      <c r="E19" s="347"/>
+      <c r="F19" s="347"/>
+      <c r="G19" s="347"/>
+      <c r="H19" s="347"/>
+      <c r="I19" s="347"/>
+      <c r="J19" s="347"/>
+      <c r="K19" s="347"/>
+      <c r="L19" s="347"/>
+      <c r="M19" s="347"/>
+      <c r="N19" s="348"/>
     </row>
     <row r="20" spans="2:14" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B20" s="36"/>
@@ -11526,27 +11510,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="346" t="s">
+      <c r="A1" s="354" t="s">
         <v>233</v>
       </c>
-      <c r="B1" s="347"/>
-      <c r="C1" s="347"/>
-      <c r="D1" s="347"/>
-      <c r="E1" s="347"/>
-      <c r="F1" s="347"/>
-      <c r="G1" s="347"/>
-      <c r="H1" s="347"/>
-      <c r="I1" s="347"/>
-      <c r="J1" s="347"/>
-      <c r="K1" s="347"/>
-      <c r="L1" s="347"/>
-      <c r="M1" s="347"/>
-      <c r="N1" s="347"/>
-      <c r="O1" s="347"/>
-      <c r="P1" s="347"/>
-      <c r="Q1" s="347"/>
-      <c r="R1" s="347"/>
-      <c r="S1" s="347"/>
+      <c r="B1" s="355"/>
+      <c r="C1" s="355"/>
+      <c r="D1" s="355"/>
+      <c r="E1" s="355"/>
+      <c r="F1" s="355"/>
+      <c r="G1" s="355"/>
+      <c r="H1" s="355"/>
+      <c r="I1" s="355"/>
+      <c r="J1" s="355"/>
+      <c r="K1" s="355"/>
+      <c r="L1" s="355"/>
+      <c r="M1" s="355"/>
+      <c r="N1" s="355"/>
+      <c r="O1" s="355"/>
+      <c r="P1" s="355"/>
+      <c r="Q1" s="355"/>
+      <c r="R1" s="355"/>
+      <c r="S1" s="355"/>
     </row>
     <row r="2" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="34"/>
@@ -11560,26 +11544,26 @@
       <c r="I2" s="34"/>
     </row>
     <row r="3" spans="1:20" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="338" t="s">
+      <c r="B3" s="346" t="s">
         <v>223</v>
       </c>
-      <c r="C3" s="339"/>
-      <c r="D3" s="339"/>
-      <c r="E3" s="339"/>
-      <c r="F3" s="339"/>
-      <c r="G3" s="339"/>
-      <c r="H3" s="339"/>
-      <c r="I3" s="339"/>
-      <c r="J3" s="340"/>
-      <c r="L3" s="343" t="s">
+      <c r="C3" s="347"/>
+      <c r="D3" s="347"/>
+      <c r="E3" s="347"/>
+      <c r="F3" s="347"/>
+      <c r="G3" s="347"/>
+      <c r="H3" s="347"/>
+      <c r="I3" s="347"/>
+      <c r="J3" s="348"/>
+      <c r="L3" s="351" t="s">
         <v>223</v>
       </c>
-      <c r="M3" s="344"/>
-      <c r="N3" s="344"/>
-      <c r="O3" s="344"/>
-      <c r="P3" s="344"/>
-      <c r="Q3" s="344"/>
-      <c r="R3" s="345"/>
+      <c r="M3" s="352"/>
+      <c r="N3" s="352"/>
+      <c r="O3" s="352"/>
+      <c r="P3" s="352"/>
+      <c r="Q3" s="352"/>
+      <c r="R3" s="353"/>
       <c r="S3" s="35"/>
       <c r="T3" s="35"/>
     </row>
@@ -11810,23 +11794,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="348" t="s">
+      <c r="A1" s="356" t="s">
         <v>232</v>
       </c>
-      <c r="B1" s="349"/>
-      <c r="C1" s="349"/>
-      <c r="D1" s="349"/>
-      <c r="E1" s="349"/>
-      <c r="F1" s="349"/>
-      <c r="G1" s="349"/>
-      <c r="H1" s="349"/>
-      <c r="I1" s="349"/>
-      <c r="J1" s="349"/>
-      <c r="K1" s="349"/>
-      <c r="L1" s="349"/>
-      <c r="M1" s="349"/>
-      <c r="N1" s="349"/>
-      <c r="O1" s="350"/>
+      <c r="B1" s="357"/>
+      <c r="C1" s="357"/>
+      <c r="D1" s="357"/>
+      <c r="E1" s="357"/>
+      <c r="F1" s="357"/>
+      <c r="G1" s="357"/>
+      <c r="H1" s="357"/>
+      <c r="I1" s="357"/>
+      <c r="J1" s="357"/>
+      <c r="K1" s="357"/>
+      <c r="L1" s="357"/>
+      <c r="M1" s="357"/>
+      <c r="N1" s="357"/>
+      <c r="O1" s="358"/>
     </row>
     <row r="2" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33"/>
@@ -11839,22 +11823,22 @@
       <c r="H2" s="51"/>
     </row>
     <row r="3" spans="1:16" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="338" t="s">
+      <c r="B3" s="346" t="s">
         <v>223</v>
       </c>
-      <c r="C3" s="339"/>
-      <c r="D3" s="339"/>
-      <c r="E3" s="339"/>
-      <c r="F3" s="339"/>
-      <c r="G3" s="339"/>
-      <c r="H3" s="340"/>
-      <c r="J3" s="343" t="s">
+      <c r="C3" s="347"/>
+      <c r="D3" s="347"/>
+      <c r="E3" s="347"/>
+      <c r="F3" s="347"/>
+      <c r="G3" s="347"/>
+      <c r="H3" s="348"/>
+      <c r="J3" s="351" t="s">
         <v>223</v>
       </c>
-      <c r="K3" s="344"/>
-      <c r="L3" s="344"/>
-      <c r="M3" s="344"/>
-      <c r="N3" s="345"/>
+      <c r="K3" s="352"/>
+      <c r="L3" s="352"/>
+      <c r="M3" s="352"/>
+      <c r="N3" s="353"/>
       <c r="O3" s="35"/>
       <c r="P3" s="35"/>
     </row>

</xml_diff>

<commit_message>
Addressed #421 and #409
</commit_message>
<xml_diff>
--- a/test_templates/faulty_batch_template1.xlsx
+++ b/test_templates/faulty_batch_template1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coverney\Documents\GitHub\TASBEFlowAnalytics\test_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B4DA3AF-075D-4F36-91E1-408AC3A93831}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-50385" yWindow="1080" windowWidth="47745" windowHeight="25665" firstSheet="5" activeTab="5"/>
+    <workbookView xWindow="-50385" yWindow="1080" windowWidth="47745" windowHeight="25665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiment" sheetId="6" r:id="rId1"/>
@@ -32,17 +33,22 @@
     <definedName name="I7577I">1</definedName>
     <definedName name="I896I">0</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="531">
   <si>
     <t>blank plasmid</t>
   </si>
@@ -2600,11 +2606,23 @@
   <si>
     <t>When true, controls the random seed for GMM Gating</t>
   </si>
+  <si>
+    <t>CSV Header 1</t>
+  </si>
+  <si>
+    <t>CSV Header 4</t>
+  </si>
+  <si>
+    <t>CSV Header 3</t>
+  </si>
+  <si>
+    <t>CSV Header 2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="34" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2912,7 +2930,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="48">
+  <borders count="54">
     <border>
       <left/>
       <right/>
@@ -3517,11 +3535,77 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="359">
+  <cellXfs count="373">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4235,74 +4319,41 @@
     <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4346,26 +4397,59 @@
     <xf numFmtId="0" fontId="15" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4458,17 +4542,35 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -4491,35 +4593,17 @@
     <xf numFmtId="0" fontId="28" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="16" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4575,6 +4659,62 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4645,6 +4785,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3074"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000020C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -4710,6 +4853,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3075"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000030C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4782,6 +4928,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1027"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -4853,6 +5002,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4098"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -4918,6 +5070,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4097"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000001100000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4990,6 +5145,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s7169"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000011C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -5055,6 +5213,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s7170"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000021C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5399,14 +5560,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1">
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView topLeftCell="C16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5420,93 +5581,93 @@
     <col min="7" max="7" width="10.5" style="85" customWidth="1"/>
     <col min="8" max="8" width="12.125" style="85" customWidth="1"/>
     <col min="9" max="9" width="20" style="85" customWidth="1"/>
-    <col min="10" max="10" width="8.625" style="85" customWidth="1"/>
-    <col min="11" max="11" width="6" style="85" customWidth="1"/>
+    <col min="10" max="10" width="10.75" style="85" customWidth="1"/>
+    <col min="11" max="11" width="6.375" style="85" customWidth="1"/>
     <col min="12" max="12" width="21.25" style="85" customWidth="1"/>
     <col min="13" max="16384" width="10.875" style="85"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="271" t="s">
+      <c r="A1" s="260" t="s">
         <v>378</v>
       </c>
-      <c r="B1" s="272"/>
-      <c r="C1" s="272"/>
-      <c r="D1" s="272"/>
-      <c r="E1" s="272"/>
-      <c r="F1" s="272"/>
-      <c r="G1" s="272"/>
-      <c r="H1" s="272"/>
-      <c r="I1" s="272"/>
-      <c r="J1" s="272"/>
-      <c r="K1" s="273"/>
+      <c r="B1" s="261"/>
+      <c r="C1" s="261"/>
+      <c r="D1" s="261"/>
+      <c r="E1" s="261"/>
+      <c r="F1" s="261"/>
+      <c r="G1" s="261"/>
+      <c r="H1" s="261"/>
+      <c r="I1" s="261"/>
+      <c r="J1" s="261"/>
+      <c r="K1" s="262"/>
     </row>
     <row r="2" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="86"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="250" t="s">
+      <c r="A3" s="276" t="s">
         <v>316</v>
       </c>
-      <c r="B3" s="251"/>
+      <c r="B3" s="277"/>
     </row>
     <row r="4" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="264" t="s">
+      <c r="A4" s="274" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="265"/>
+      <c r="B4" s="275"/>
     </row>
     <row r="5" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="266" t="s">
+      <c r="A5" s="290" t="s">
         <v>182</v>
       </c>
-      <c r="B5" s="267"/>
+      <c r="B5" s="291"/>
     </row>
     <row r="6" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="86"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="250" t="s">
+      <c r="A7" s="276" t="s">
         <v>273</v>
       </c>
-      <c r="B7" s="252"/>
-      <c r="C7" s="252"/>
-      <c r="D7" s="252"/>
-      <c r="E7" s="252"/>
-      <c r="F7" s="252"/>
-      <c r="G7" s="252"/>
-      <c r="H7" s="252"/>
-      <c r="I7" s="252"/>
-      <c r="J7" s="252"/>
-      <c r="K7" s="251"/>
+      <c r="B7" s="278"/>
+      <c r="C7" s="278"/>
+      <c r="D7" s="278"/>
+      <c r="E7" s="278"/>
+      <c r="F7" s="278"/>
+      <c r="G7" s="278"/>
+      <c r="H7" s="278"/>
+      <c r="I7" s="278"/>
+      <c r="J7" s="278"/>
+      <c r="K7" s="277"/>
     </row>
     <row r="8" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="274" t="s">
+      <c r="A8" s="263" t="s">
         <v>162</v>
       </c>
-      <c r="B8" s="275"/>
-      <c r="C8" s="275"/>
-      <c r="D8" s="275"/>
-      <c r="E8" s="275"/>
-      <c r="F8" s="275"/>
-      <c r="G8" s="275"/>
-      <c r="H8" s="275"/>
-      <c r="I8" s="275"/>
-      <c r="J8" s="275"/>
-      <c r="K8" s="276"/>
+      <c r="B8" s="264"/>
+      <c r="C8" s="264"/>
+      <c r="D8" s="264"/>
+      <c r="E8" s="264"/>
+      <c r="F8" s="264"/>
+      <c r="G8" s="264"/>
+      <c r="H8" s="264"/>
+      <c r="I8" s="264"/>
+      <c r="J8" s="264"/>
+      <c r="K8" s="265"/>
     </row>
     <row r="9" spans="1:11" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="277"/>
-      <c r="B9" s="278"/>
-      <c r="C9" s="278"/>
-      <c r="D9" s="278"/>
-      <c r="E9" s="278"/>
-      <c r="F9" s="278"/>
-      <c r="G9" s="278"/>
-      <c r="H9" s="278"/>
-      <c r="I9" s="278"/>
-      <c r="J9" s="278"/>
-      <c r="K9" s="279"/>
+      <c r="A9" s="266"/>
+      <c r="B9" s="267"/>
+      <c r="C9" s="267"/>
+      <c r="D9" s="267"/>
+      <c r="E9" s="267"/>
+      <c r="F9" s="267"/>
+      <c r="G9" s="267"/>
+      <c r="H9" s="267"/>
+      <c r="I9" s="267"/>
+      <c r="J9" s="267"/>
+      <c r="K9" s="268"/>
     </row>
     <row r="10" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="155"/>
@@ -5517,64 +5678,64 @@
       <c r="F10" s="141"/>
     </row>
     <row r="11" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="253" t="s">
+      <c r="A11" s="279" t="s">
         <v>274</v>
       </c>
-      <c r="B11" s="254"/>
-      <c r="C11" s="254"/>
-      <c r="D11" s="255"/>
+      <c r="B11" s="280"/>
+      <c r="C11" s="280"/>
+      <c r="D11" s="281"/>
       <c r="E11" s="87"/>
       <c r="F11" s="141"/>
     </row>
     <row r="12" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="256" t="s">
+      <c r="A12" s="282" t="s">
         <v>163</v>
       </c>
-      <c r="B12" s="257"/>
-      <c r="C12" s="258" t="s">
+      <c r="B12" s="283"/>
+      <c r="C12" s="284" t="s">
         <v>164</v>
       </c>
-      <c r="D12" s="259"/>
+      <c r="D12" s="285"/>
       <c r="E12" s="87"/>
       <c r="F12" s="141"/>
     </row>
     <row r="13" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="260"/>
-      <c r="B13" s="261"/>
-      <c r="C13" s="262"/>
-      <c r="D13" s="263"/>
+      <c r="A13" s="286"/>
+      <c r="B13" s="287"/>
+      <c r="C13" s="288"/>
+      <c r="D13" s="289"/>
       <c r="E13" s="87"/>
       <c r="F13" s="141"/>
     </row>
     <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:11" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="253" t="s">
+      <c r="A15" s="279" t="s">
         <v>275</v>
       </c>
-      <c r="B15" s="255"/>
-      <c r="E15" s="253" t="s">
+      <c r="B15" s="281"/>
+      <c r="E15" s="279" t="s">
         <v>315</v>
       </c>
-      <c r="F15" s="254"/>
-      <c r="G15" s="254"/>
-      <c r="H15" s="254"/>
-      <c r="I15" s="255"/>
+      <c r="F15" s="280"/>
+      <c r="G15" s="280"/>
+      <c r="H15" s="280"/>
+      <c r="I15" s="281"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="264" t="s">
+      <c r="A16" s="274" t="s">
         <v>236</v>
       </c>
-      <c r="B16" s="265"/>
+      <c r="B16" s="275"/>
       <c r="D16" s="88"/>
-      <c r="E16" s="280" t="s">
+      <c r="E16" s="269" t="s">
         <v>197</v>
       </c>
-      <c r="F16" s="281"/>
-      <c r="G16" s="281"/>
-      <c r="H16" s="281"/>
-      <c r="I16" s="282"/>
-    </row>
-    <row r="17" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F16" s="270"/>
+      <c r="G16" s="270"/>
+      <c r="H16" s="270"/>
+      <c r="I16" s="271"/>
+    </row>
+    <row r="17" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="156" t="s">
         <v>237</v>
       </c>
@@ -5582,10 +5743,10 @@
         <v>278</v>
       </c>
       <c r="C17" s="89"/>
-      <c r="E17" s="283" t="s">
+      <c r="E17" s="272" t="s">
         <v>235</v>
       </c>
-      <c r="F17" s="284"/>
+      <c r="F17" s="273"/>
       <c r="G17" s="82" t="s">
         <v>159</v>
       </c>
@@ -5595,9 +5756,12 @@
       <c r="I17" s="188" t="s">
         <v>356</v>
       </c>
-      <c r="J17" s="80"/>
-    </row>
-    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J17" s="359" t="s">
+        <v>527</v>
+      </c>
+      <c r="K17" s="360"/>
+    </row>
+    <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="157" t="s">
         <v>269</v>
       </c>
@@ -5615,12 +5779,13 @@
       <c r="H18" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="I18" s="268" t="s">
+      <c r="I18" s="248" t="s">
         <v>465</v>
       </c>
-      <c r="J18" s="80"/>
-    </row>
-    <row r="19" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="J18" s="361"/>
+      <c r="K18" s="362"/>
+    </row>
+    <row r="19" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A19" s="158" t="s">
         <v>288</v>
       </c>
@@ -5638,10 +5803,11 @@
       <c r="H19" s="73" t="s">
         <v>196</v>
       </c>
-      <c r="I19" s="268"/>
-      <c r="J19" s="80"/>
-    </row>
-    <row r="20" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I19" s="248"/>
+      <c r="J19" s="361"/>
+      <c r="K19" s="362"/>
+    </row>
+    <row r="20" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="158" t="s">
         <v>289</v>
       </c>
@@ -5655,10 +5821,11 @@
       </c>
       <c r="G20" s="70"/>
       <c r="H20" s="70"/>
-      <c r="I20" s="269"/>
-      <c r="J20" s="80"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I20" s="249"/>
+      <c r="J20" s="363"/>
+      <c r="K20" s="364"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="158" t="s">
         <v>293</v>
       </c>
@@ -5667,34 +5834,34 @@
       <c r="I21" s="80"/>
       <c r="J21" s="80"/>
     </row>
-    <row r="22" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="159"/>
       <c r="B22" s="116"/>
       <c r="C22" s="89"/>
       <c r="J22" s="80"/>
     </row>
-    <row r="23" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="160"/>
       <c r="B23" s="92"/>
       <c r="C23" s="91"/>
-      <c r="E23" s="248" t="s">
+      <c r="E23" s="250" t="s">
         <v>198</v>
       </c>
-      <c r="F23" s="270"/>
-      <c r="G23" s="270"/>
-      <c r="H23" s="270"/>
-      <c r="I23" s="249"/>
-    </row>
-    <row r="24" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="248" t="s">
+      <c r="F23" s="251"/>
+      <c r="G23" s="251"/>
+      <c r="H23" s="251"/>
+      <c r="I23" s="252"/>
+    </row>
+    <row r="24" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="250" t="s">
         <v>240</v>
       </c>
-      <c r="B24" s="249"/>
+      <c r="B24" s="252"/>
       <c r="C24" s="31"/>
-      <c r="E24" s="288" t="s">
+      <c r="E24" s="256" t="s">
         <v>235</v>
       </c>
-      <c r="F24" s="289"/>
+      <c r="F24" s="257"/>
       <c r="G24" s="81" t="s">
         <v>159</v>
       </c>
@@ -5704,8 +5871,12 @@
       <c r="I24" s="188" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J24" s="359" t="s">
+        <v>530</v>
+      </c>
+      <c r="K24" s="360"/>
+    </row>
+    <row r="25" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="156" t="s">
         <v>237</v>
       </c>
@@ -5723,11 +5894,13 @@
       <c r="H25" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="I25" s="285" t="s">
+      <c r="I25" s="253" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="J25" s="361"/>
+      <c r="K25" s="362"/>
+    </row>
+    <row r="26" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="157" t="s">
         <v>269</v>
       </c>
@@ -5747,9 +5920,11 @@
       <c r="H26" s="73" t="s">
         <v>201</v>
       </c>
-      <c r="I26" s="286"/>
-    </row>
-    <row r="27" spans="1:10" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I26" s="254"/>
+      <c r="J26" s="361"/>
+      <c r="K26" s="362"/>
+    </row>
+    <row r="27" spans="1:11" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="158" t="s">
         <v>286</v>
       </c>
@@ -5763,9 +5938,11 @@
       </c>
       <c r="G27" s="70"/>
       <c r="H27" s="70"/>
-      <c r="I27" s="287"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I27" s="255"/>
+      <c r="J27" s="363"/>
+      <c r="K27" s="364"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="158" t="s">
         <v>287</v>
       </c>
@@ -5777,32 +5954,32 @@
       <c r="H28" s="94"/>
       <c r="I28" s="80"/>
     </row>
-    <row r="29" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="158"/>
       <c r="B29" s="115"/>
       <c r="C29" s="31"/>
       <c r="I29" s="80"/>
     </row>
-    <row r="30" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="159"/>
       <c r="B30" s="116"/>
       <c r="C30" s="89"/>
-      <c r="E30" s="248" t="s">
+      <c r="E30" s="250" t="s">
         <v>199</v>
       </c>
-      <c r="F30" s="270"/>
-      <c r="G30" s="270"/>
-      <c r="H30" s="270"/>
-      <c r="I30" s="249"/>
-    </row>
-    <row r="31" spans="1:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F30" s="251"/>
+      <c r="G30" s="251"/>
+      <c r="H30" s="251"/>
+      <c r="I30" s="252"/>
+    </row>
+    <row r="31" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="160"/>
       <c r="B31" s="91"/>
       <c r="C31" s="91"/>
-      <c r="E31" s="290" t="s">
+      <c r="E31" s="258" t="s">
         <v>463</v>
       </c>
-      <c r="F31" s="291"/>
+      <c r="F31" s="259"/>
       <c r="G31" s="198" t="s">
         <v>159</v>
       </c>
@@ -5812,12 +5989,16 @@
       <c r="I31" s="188" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="248" t="s">
+      <c r="J31" s="366" t="s">
+        <v>529</v>
+      </c>
+      <c r="K31" s="367"/>
+    </row>
+    <row r="32" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="250" t="s">
         <v>241</v>
       </c>
-      <c r="B32" s="249"/>
+      <c r="B32" s="252"/>
       <c r="C32" s="31"/>
       <c r="E32" s="83">
         <v>1</v>
@@ -5827,9 +6008,11 @@
       </c>
       <c r="G32" s="32"/>
       <c r="H32" s="73"/>
-      <c r="I32" s="268"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I32" s="248"/>
+      <c r="J32" s="368"/>
+      <c r="K32" s="369"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="156" t="s">
         <v>237</v>
       </c>
@@ -5847,9 +6030,11 @@
         <v>5</v>
       </c>
       <c r="H33" s="32"/>
-      <c r="I33" s="268"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I33" s="248"/>
+      <c r="J33" s="365"/>
+      <c r="K33" s="370"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="157" t="s">
         <v>239</v>
       </c>
@@ -5862,9 +6047,11 @@
       <c r="F34" s="93"/>
       <c r="G34" s="32"/>
       <c r="H34" s="73"/>
-      <c r="I34" s="268"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I34" s="248"/>
+      <c r="J34" s="365"/>
+      <c r="K34" s="370"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="158" t="s">
         <v>224</v>
       </c>
@@ -5875,9 +6062,11 @@
       <c r="F35" s="93"/>
       <c r="G35" s="32"/>
       <c r="H35" s="32"/>
-      <c r="I35" s="268"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I35" s="248"/>
+      <c r="J35" s="365"/>
+      <c r="K35" s="370"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="158" t="s">
         <v>225</v>
       </c>
@@ -5888,9 +6077,11 @@
       <c r="F36" s="93"/>
       <c r="G36" s="32"/>
       <c r="H36" s="32"/>
-      <c r="I36" s="268"/>
-    </row>
-    <row r="37" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I36" s="248"/>
+      <c r="J36" s="365"/>
+      <c r="K36" s="370"/>
+    </row>
+    <row r="37" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="158" t="s">
         <v>226</v>
       </c>
@@ -5901,30 +6092,32 @@
       <c r="F37" s="139"/>
       <c r="G37" s="70"/>
       <c r="H37" s="70"/>
-      <c r="I37" s="269"/>
-    </row>
-    <row r="38" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I37" s="249"/>
+      <c r="J37" s="371"/>
+      <c r="K37" s="372"/>
+    </row>
+    <row r="38" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="159" t="s">
         <v>227</v>
       </c>
       <c r="B38" s="116"/>
     </row>
-    <row r="39" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="161"/>
       <c r="B39" s="120"/>
     </row>
-    <row r="40" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="E40" s="248" t="s">
+    <row r="40" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="E40" s="250" t="s">
         <v>200</v>
       </c>
-      <c r="F40" s="270"/>
-      <c r="G40" s="270"/>
-      <c r="H40" s="270"/>
-      <c r="I40" s="249"/>
-    </row>
-    <row r="41" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="E41" s="288"/>
-      <c r="F41" s="289"/>
+      <c r="F40" s="251"/>
+      <c r="G40" s="251"/>
+      <c r="H40" s="251"/>
+      <c r="I40" s="252"/>
+    </row>
+    <row r="41" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E41" s="256"/>
+      <c r="F41" s="257"/>
       <c r="G41" s="81" t="s">
         <v>159</v>
       </c>
@@ -5934,78 +6127,86 @@
       <c r="I41" s="188" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J41" s="366" t="s">
+        <v>528</v>
+      </c>
+      <c r="K41" s="367"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E42" s="83">
         <v>1</v>
       </c>
       <c r="F42" s="93"/>
       <c r="G42" s="32"/>
       <c r="H42" s="73"/>
-      <c r="I42" s="268"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I42" s="248"/>
+      <c r="J42" s="368"/>
+      <c r="K42" s="369"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E43" s="83">
         <v>2</v>
       </c>
       <c r="F43" s="93"/>
       <c r="G43" s="32"/>
       <c r="H43" s="32"/>
-      <c r="I43" s="268"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I43" s="248"/>
+      <c r="J43" s="365"/>
+      <c r="K43" s="370"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E44" s="83">
         <v>3</v>
       </c>
       <c r="F44" s="93"/>
       <c r="G44" s="32"/>
       <c r="H44" s="73"/>
-      <c r="I44" s="268"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I44" s="248"/>
+      <c r="J44" s="365"/>
+      <c r="K44" s="370"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E45" s="83">
         <v>4</v>
       </c>
       <c r="F45" s="93"/>
       <c r="G45" s="32"/>
       <c r="H45" s="32"/>
-      <c r="I45" s="268"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I45" s="248"/>
+      <c r="J45" s="365"/>
+      <c r="K45" s="370"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E46" s="83">
         <v>5</v>
       </c>
       <c r="F46" s="93"/>
       <c r="G46" s="32"/>
       <c r="H46" s="32"/>
-      <c r="I46" s="268"/>
-    </row>
-    <row r="47" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I46" s="248"/>
+      <c r="J46" s="365"/>
+      <c r="K46" s="370"/>
+    </row>
+    <row r="47" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E47" s="84">
         <v>6</v>
       </c>
       <c r="F47" s="139"/>
       <c r="G47" s="70"/>
       <c r="H47" s="70"/>
-      <c r="I47" s="269"/>
-    </row>
-    <row r="48" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="I47" s="249"/>
+      <c r="J47" s="371"/>
+      <c r="K47" s="372"/>
+    </row>
+    <row r="48" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="I42:I47"/>
-    <mergeCell ref="E40:I40"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="I25:I27"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A8:K8"/>
-    <mergeCell ref="A9:K9"/>
-    <mergeCell ref="E16:I16"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="A16:B16"/>
+  <mergeCells count="37">
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="J42:K47"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="J25:K27"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="J32:K37"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="A3:B3"/>
@@ -6021,6 +6222,22 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="I32:I37"/>
     <mergeCell ref="E30:I30"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A8:K8"/>
+    <mergeCell ref="A9:K9"/>
+    <mergeCell ref="E16:I16"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="J18:K20"/>
+    <mergeCell ref="I42:I47"/>
+    <mergeCell ref="E40:I40"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="I25:I27"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E31:F31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6028,13 +6245,13 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2">
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
   <dimension ref="A1:R71"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
@@ -7504,7 +7721,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3">
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
@@ -8491,7 +8708,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4">
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
@@ -8523,68 +8740,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="325" t="s">
+      <c r="A1" s="332" t="s">
         <v>244</v>
       </c>
-      <c r="B1" s="325"/>
-      <c r="C1" s="325"/>
-      <c r="D1" s="325"/>
-      <c r="E1" s="325"/>
-      <c r="F1" s="325"/>
-      <c r="G1" s="325"/>
-      <c r="H1" s="325"/>
-      <c r="I1" s="325"/>
-      <c r="J1" s="325"/>
-      <c r="K1" s="325"/>
-      <c r="L1" s="325"/>
-      <c r="M1" s="325"/>
-      <c r="N1" s="325"/>
-      <c r="O1" s="325"/>
+      <c r="B1" s="332"/>
+      <c r="C1" s="332"/>
+      <c r="D1" s="332"/>
+      <c r="E1" s="332"/>
+      <c r="F1" s="332"/>
+      <c r="G1" s="332"/>
+      <c r="H1" s="332"/>
+      <c r="I1" s="332"/>
+      <c r="J1" s="332"/>
+      <c r="K1" s="332"/>
+      <c r="L1" s="332"/>
+      <c r="M1" s="332"/>
+      <c r="N1" s="332"/>
+      <c r="O1" s="332"/>
       <c r="P1" s="30"/>
       <c r="Q1" s="30"/>
     </row>
     <row r="2" spans="1:17" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="336" t="s">
+      <c r="A2" s="326" t="s">
         <v>279</v>
       </c>
-      <c r="B2" s="337"/>
-      <c r="C2" s="337"/>
-      <c r="D2" s="337"/>
-      <c r="E2" s="337"/>
-      <c r="F2" s="338"/>
-      <c r="G2" s="326" t="s">
+      <c r="B2" s="327"/>
+      <c r="C2" s="327"/>
+      <c r="D2" s="327"/>
+      <c r="E2" s="327"/>
+      <c r="F2" s="328"/>
+      <c r="G2" s="333" t="s">
         <v>246</v>
       </c>
-      <c r="H2" s="326"/>
-      <c r="I2" s="326"/>
-      <c r="J2" s="326"/>
-      <c r="K2" s="326"/>
-      <c r="L2" s="326"/>
-      <c r="M2" s="332" t="s">
+      <c r="H2" s="333"/>
+      <c r="I2" s="333"/>
+      <c r="J2" s="333"/>
+      <c r="K2" s="333"/>
+      <c r="L2" s="333"/>
+      <c r="M2" s="322" t="s">
         <v>295</v>
       </c>
-      <c r="N2" s="332"/>
-      <c r="O2" s="332"/>
+      <c r="N2" s="322"/>
+      <c r="O2" s="322"/>
       <c r="P2" s="88"/>
       <c r="Q2" s="88"/>
     </row>
     <row r="3" spans="1:17" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="339" t="s">
+      <c r="A3" s="329" t="s">
         <v>472</v>
       </c>
-      <c r="B3" s="340"/>
-      <c r="C3" s="340"/>
-      <c r="D3" s="340"/>
-      <c r="E3" s="340"/>
-      <c r="F3" s="341"/>
-      <c r="G3" s="328" t="s">
+      <c r="B3" s="330"/>
+      <c r="C3" s="330"/>
+      <c r="D3" s="330"/>
+      <c r="E3" s="330"/>
+      <c r="F3" s="331"/>
+      <c r="G3" s="335" t="s">
         <v>301</v>
       </c>
-      <c r="H3" s="328"/>
-      <c r="I3" s="328"/>
-      <c r="J3" s="328"/>
-      <c r="K3" s="328"/>
-      <c r="L3" s="328"/>
+      <c r="H3" s="335"/>
+      <c r="I3" s="335"/>
+      <c r="J3" s="335"/>
+      <c r="K3" s="335"/>
+      <c r="L3" s="335"/>
       <c r="M3" s="202" t="s">
         <v>299</v>
       </c>
@@ -8597,24 +8814,24 @@
       <c r="P3" s="194"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="329" t="s">
+      <c r="A4" s="336" t="s">
         <v>473</v>
       </c>
-      <c r="B4" s="330"/>
-      <c r="C4" s="330"/>
-      <c r="D4" s="330"/>
-      <c r="E4" s="330"/>
-      <c r="F4" s="331"/>
-      <c r="G4" s="327" t="s">
+      <c r="B4" s="337"/>
+      <c r="C4" s="337"/>
+      <c r="D4" s="337"/>
+      <c r="E4" s="337"/>
+      <c r="F4" s="338"/>
+      <c r="G4" s="334" t="s">
         <v>247</v>
       </c>
-      <c r="H4" s="327"/>
-      <c r="I4" s="327"/>
-      <c r="J4" s="327" t="s">
+      <c r="H4" s="334"/>
+      <c r="I4" s="334"/>
+      <c r="J4" s="334" t="s">
         <v>302</v>
       </c>
-      <c r="K4" s="327"/>
-      <c r="L4" s="327"/>
+      <c r="K4" s="334"/>
+      <c r="L4" s="334"/>
       <c r="M4" s="203" t="s">
         <v>154</v>
       </c>
@@ -8626,12 +8843,12 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="322"/>
-      <c r="B5" s="323"/>
-      <c r="C5" s="323"/>
-      <c r="D5" s="323"/>
-      <c r="E5" s="323"/>
-      <c r="F5" s="324"/>
+      <c r="A5" s="339"/>
+      <c r="B5" s="340"/>
+      <c r="C5" s="340"/>
+      <c r="D5" s="340"/>
+      <c r="E5" s="340"/>
+      <c r="F5" s="341"/>
       <c r="G5" s="321" t="s">
         <v>278</v>
       </c>
@@ -8651,14 +8868,14 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="322" t="s">
+      <c r="A6" s="339" t="s">
         <v>474</v>
       </c>
-      <c r="B6" s="323"/>
-      <c r="C6" s="323"/>
-      <c r="D6" s="323"/>
-      <c r="E6" s="323"/>
-      <c r="F6" s="324"/>
+      <c r="B6" s="340"/>
+      <c r="C6" s="340"/>
+      <c r="D6" s="340"/>
+      <c r="E6" s="340"/>
+      <c r="F6" s="341"/>
       <c r="G6" s="321" t="s">
         <v>285</v>
       </c>
@@ -8676,14 +8893,14 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="322" t="s">
+      <c r="A7" s="339" t="s">
         <v>475</v>
       </c>
-      <c r="B7" s="323"/>
-      <c r="C7" s="323"/>
-      <c r="D7" s="323"/>
-      <c r="E7" s="323"/>
-      <c r="F7" s="324"/>
+      <c r="B7" s="340"/>
+      <c r="C7" s="340"/>
+      <c r="D7" s="340"/>
+      <c r="E7" s="340"/>
+      <c r="F7" s="341"/>
       <c r="G7" s="321"/>
       <c r="H7" s="321"/>
       <c r="I7" s="321"/>
@@ -8695,12 +8912,12 @@
       <c r="O7" s="205"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="322"/>
-      <c r="B8" s="323"/>
-      <c r="C8" s="323"/>
-      <c r="D8" s="323"/>
-      <c r="E8" s="323"/>
-      <c r="F8" s="324"/>
+      <c r="A8" s="339"/>
+      <c r="B8" s="340"/>
+      <c r="C8" s="340"/>
+      <c r="D8" s="340"/>
+      <c r="E8" s="340"/>
+      <c r="F8" s="341"/>
       <c r="G8" s="321"/>
       <c r="H8" s="321"/>
       <c r="I8" s="321"/>
@@ -8713,17 +8930,17 @@
     </row>
     <row r="9" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:17" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="333" t="s">
+      <c r="A10" s="323" t="s">
         <v>354</v>
       </c>
-      <c r="B10" s="334"/>
-      <c r="C10" s="334"/>
-      <c r="D10" s="334"/>
-      <c r="E10" s="334"/>
-      <c r="F10" s="334"/>
-      <c r="G10" s="334"/>
-      <c r="H10" s="334"/>
-      <c r="I10" s="335"/>
+      <c r="B10" s="324"/>
+      <c r="C10" s="324"/>
+      <c r="D10" s="324"/>
+      <c r="E10" s="324"/>
+      <c r="F10" s="324"/>
+      <c r="G10" s="324"/>
+      <c r="H10" s="324"/>
+      <c r="I10" s="325"/>
     </row>
     <row r="11" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="130" t="s">
@@ -9330,14 +9547,12 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="A16:H19"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A8:F8"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="G6:I6"/>
     <mergeCell ref="J6:L6"/>
@@ -9350,12 +9565,14 @@
     <mergeCell ref="A4:F4"/>
     <mergeCell ref="A5:F5"/>
     <mergeCell ref="A6:F6"/>
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="A16:H19"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9415,7 +9632,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet5">
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
@@ -9447,68 +9664,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="325" t="s">
+      <c r="A1" s="332" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="325"/>
-      <c r="C1" s="325"/>
-      <c r="D1" s="325"/>
-      <c r="E1" s="325"/>
-      <c r="F1" s="325"/>
-      <c r="G1" s="325"/>
-      <c r="H1" s="325"/>
-      <c r="I1" s="325"/>
-      <c r="J1" s="325"/>
-      <c r="K1" s="325"/>
-      <c r="L1" s="325"/>
-      <c r="M1" s="325"/>
-      <c r="N1" s="325"/>
-      <c r="O1" s="325"/>
-      <c r="P1" s="325"/>
+      <c r="B1" s="332"/>
+      <c r="C1" s="332"/>
+      <c r="D1" s="332"/>
+      <c r="E1" s="332"/>
+      <c r="F1" s="332"/>
+      <c r="G1" s="332"/>
+      <c r="H1" s="332"/>
+      <c r="I1" s="332"/>
+      <c r="J1" s="332"/>
+      <c r="K1" s="332"/>
+      <c r="L1" s="332"/>
+      <c r="M1" s="332"/>
+      <c r="N1" s="332"/>
+      <c r="O1" s="332"/>
+      <c r="P1" s="332"/>
       <c r="Q1" s="30"/>
     </row>
     <row r="2" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="326" t="s">
+      <c r="A2" s="333" t="s">
         <v>279</v>
       </c>
-      <c r="B2" s="326"/>
-      <c r="C2" s="326"/>
-      <c r="D2" s="326"/>
-      <c r="E2" s="326"/>
-      <c r="F2" s="326"/>
-      <c r="G2" s="326" t="s">
+      <c r="B2" s="333"/>
+      <c r="C2" s="333"/>
+      <c r="D2" s="333"/>
+      <c r="E2" s="333"/>
+      <c r="F2" s="333"/>
+      <c r="G2" s="333" t="s">
         <v>246</v>
       </c>
-      <c r="H2" s="326"/>
-      <c r="I2" s="326"/>
-      <c r="J2" s="326"/>
-      <c r="K2" s="326"/>
-      <c r="L2" s="326"/>
-      <c r="M2" s="332" t="s">
+      <c r="H2" s="333"/>
+      <c r="I2" s="333"/>
+      <c r="J2" s="333"/>
+      <c r="K2" s="333"/>
+      <c r="L2" s="333"/>
+      <c r="M2" s="322" t="s">
         <v>294</v>
       </c>
-      <c r="N2" s="332"/>
-      <c r="O2" s="332"/>
-      <c r="P2" s="332"/>
+      <c r="N2" s="322"/>
+      <c r="O2" s="322"/>
+      <c r="P2" s="322"/>
       <c r="Q2" s="88"/>
     </row>
     <row r="3" spans="1:17" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="328" t="s">
+      <c r="A3" s="335" t="s">
         <v>476</v>
       </c>
-      <c r="B3" s="328"/>
-      <c r="C3" s="328"/>
-      <c r="D3" s="328"/>
-      <c r="E3" s="328"/>
-      <c r="F3" s="328"/>
-      <c r="G3" s="328" t="s">
+      <c r="B3" s="335"/>
+      <c r="C3" s="335"/>
+      <c r="D3" s="335"/>
+      <c r="E3" s="335"/>
+      <c r="F3" s="335"/>
+      <c r="G3" s="335" t="s">
         <v>296</v>
       </c>
-      <c r="H3" s="328"/>
-      <c r="I3" s="328"/>
-      <c r="J3" s="328"/>
-      <c r="K3" s="328"/>
-      <c r="L3" s="328"/>
+      <c r="H3" s="335"/>
+      <c r="I3" s="335"/>
+      <c r="J3" s="335"/>
+      <c r="K3" s="335"/>
+      <c r="L3" s="335"/>
       <c r="M3" s="202" t="s">
         <v>298</v>
       </c>
@@ -9524,22 +9741,22 @@
       <c r="Q3" s="193"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="329" t="s">
+      <c r="A4" s="336" t="s">
         <v>473</v>
       </c>
-      <c r="B4" s="330"/>
-      <c r="C4" s="330"/>
-      <c r="D4" s="330"/>
-      <c r="E4" s="330"/>
-      <c r="F4" s="331"/>
-      <c r="G4" s="327" t="s">
+      <c r="B4" s="337"/>
+      <c r="C4" s="337"/>
+      <c r="D4" s="337"/>
+      <c r="E4" s="337"/>
+      <c r="F4" s="338"/>
+      <c r="G4" s="334" t="s">
         <v>248</v>
       </c>
-      <c r="H4" s="327"/>
-      <c r="I4" s="327"/>
-      <c r="J4" s="327"/>
-      <c r="K4" s="327"/>
-      <c r="L4" s="327"/>
+      <c r="H4" s="334"/>
+      <c r="I4" s="334"/>
+      <c r="J4" s="334"/>
+      <c r="K4" s="334"/>
+      <c r="L4" s="334"/>
       <c r="M4" s="203" t="s">
         <v>252</v>
       </c>
@@ -9554,12 +9771,12 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="322"/>
-      <c r="B5" s="323"/>
-      <c r="C5" s="323"/>
-      <c r="D5" s="323"/>
-      <c r="E5" s="323"/>
-      <c r="F5" s="324"/>
+      <c r="A5" s="339"/>
+      <c r="B5" s="340"/>
+      <c r="C5" s="340"/>
+      <c r="D5" s="340"/>
+      <c r="E5" s="340"/>
+      <c r="F5" s="341"/>
       <c r="G5" s="342" t="s">
         <v>4</v>
       </c>
@@ -9580,14 +9797,14 @@
       </c>
     </row>
     <row r="6" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="322" t="s">
+      <c r="A6" s="339" t="s">
         <v>479</v>
       </c>
-      <c r="B6" s="323"/>
-      <c r="C6" s="323"/>
-      <c r="D6" s="323"/>
-      <c r="E6" s="323"/>
-      <c r="F6" s="324"/>
+      <c r="B6" s="340"/>
+      <c r="C6" s="340"/>
+      <c r="D6" s="340"/>
+      <c r="E6" s="340"/>
+      <c r="F6" s="341"/>
       <c r="G6" s="342" t="s">
         <v>4</v>
       </c>
@@ -9606,12 +9823,12 @@
       </c>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="322"/>
-      <c r="B7" s="323"/>
-      <c r="C7" s="323"/>
-      <c r="D7" s="323"/>
-      <c r="E7" s="323"/>
-      <c r="F7" s="324"/>
+      <c r="A7" s="339"/>
+      <c r="B7" s="340"/>
+      <c r="C7" s="340"/>
+      <c r="D7" s="340"/>
+      <c r="E7" s="340"/>
+      <c r="F7" s="341"/>
       <c r="G7" s="342"/>
       <c r="H7" s="342"/>
       <c r="I7" s="342"/>
@@ -9624,12 +9841,12 @@
       <c r="P7" s="205"/>
     </row>
     <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="322"/>
-      <c r="B8" s="323"/>
-      <c r="C8" s="323"/>
-      <c r="D8" s="323"/>
-      <c r="E8" s="323"/>
-      <c r="F8" s="324"/>
+      <c r="A8" s="339"/>
+      <c r="B8" s="340"/>
+      <c r="C8" s="340"/>
+      <c r="D8" s="340"/>
+      <c r="E8" s="340"/>
+      <c r="F8" s="341"/>
       <c r="G8" s="342"/>
       <c r="H8" s="342"/>
       <c r="I8" s="342"/>
@@ -9643,17 +9860,17 @@
     </row>
     <row r="9" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:17" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="333" t="s">
+      <c r="A10" s="323" t="s">
         <v>353</v>
       </c>
-      <c r="B10" s="334"/>
-      <c r="C10" s="334"/>
-      <c r="D10" s="334"/>
-      <c r="E10" s="334"/>
-      <c r="F10" s="334"/>
-      <c r="G10" s="334"/>
-      <c r="H10" s="334"/>
-      <c r="I10" s="335"/>
+      <c r="B10" s="324"/>
+      <c r="C10" s="324"/>
+      <c r="D10" s="324"/>
+      <c r="E10" s="324"/>
+      <c r="F10" s="324"/>
+      <c r="G10" s="324"/>
+      <c r="H10" s="324"/>
+      <c r="I10" s="325"/>
     </row>
     <row r="11" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="130" t="s">
@@ -9993,12 +10210,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="G2:L2"/>
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="G3:L3"/>
     <mergeCell ref="A21:G21"/>
     <mergeCell ref="D22:G22"/>
     <mergeCell ref="G4:L4"/>
@@ -10014,6 +10225,12 @@
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="A8:F8"/>
     <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="G2:L2"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="G3:L3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10073,13 +10290,13 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet6">
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
   <dimension ref="A1:M84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+    <sheetView zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -11035,7 +11252,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:O28"/>
   <sheetViews>
@@ -11496,7 +11713,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:T12"/>
   <sheetViews>
@@ -11778,7 +11995,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:P15"/>
   <sheetViews>

</xml_diff>